<commit_message>
Updating papers and readme
</commit_message>
<xml_diff>
--- a/output_automatizado.xlsx
+++ b/output_automatizado.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cartera" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mora" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -134,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
@@ -177,6 +178,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -586,7 +591,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ120"/>
+  <dimension ref="A2:AJ120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,7 +630,6 @@
     <col width="12.44140625" customWidth="1" min="36" max="36"/>
   </cols>
   <sheetData>
-    <row r="1"/>
     <row r="2">
       <c r="N2" s="1" t="n"/>
     </row>
@@ -15824,4 +15828,128 @@
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="31.44140625" customWidth="1" min="1" max="1"/>
+    <col width="27.88671875" customWidth="1" min="2" max="2"/>
+    <col width="12.33203125" customWidth="1" min="3" max="3"/>
+    <col width="35.5546875" customWidth="1" min="4" max="4"/>
+    <col width="5.88671875" customWidth="1" min="5" max="5"/>
+    <col width="18.109375" customWidth="1" min="6" max="6"/>
+    <col width="11.5546875" customWidth="1" min="7" max="7"/>
+    <col width="16.109375" customWidth="1" min="8" max="8"/>
+    <col width="7.88671875" customWidth="1" min="9" max="9"/>
+    <col width="16.88671875" customWidth="1" min="10" max="10"/>
+    <col width="11.5546875" customWidth="1" min="11" max="11"/>
+    <col width="12.44140625" customWidth="1" min="12" max="12"/>
+    <col width="16.109375" customWidth="1" min="13" max="13"/>
+    <col width="12.6640625" customWidth="1" min="14" max="14"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2">
+      <c r="N2" s="17" t="n"/>
+    </row>
+    <row r="3">
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Reporte de Antigüedad Grupal</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n"/>
+    </row>
+    <row r="4"/>
+    <row r="5">
+      <c r="F5" s="18" t="n"/>
+      <c r="G5" s="18" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>Nombre del gerente</t>
+        </is>
+      </c>
+      <c r="B6" s="12" t="inlineStr">
+        <is>
+          <t>Nombre del promotor</t>
+        </is>
+      </c>
+      <c r="C6" s="12" t="inlineStr">
+        <is>
+          <t>ID GRUPO</t>
+        </is>
+      </c>
+      <c r="D6" s="12" t="inlineStr">
+        <is>
+          <t>Nombre de grupo</t>
+        </is>
+      </c>
+      <c r="E6" s="12" t="inlineStr">
+        <is>
+          <t>Ciclo</t>
+        </is>
+      </c>
+      <c r="F6" s="13" t="inlineStr">
+        <is>
+          <t>Monto del crédito</t>
+        </is>
+      </c>
+      <c r="G6" s="13" t="inlineStr">
+        <is>
+          <t>Semana</t>
+        </is>
+      </c>
+      <c r="H6" s="13" t="inlineStr">
+        <is>
+          <t>Pago semanal</t>
+        </is>
+      </c>
+      <c r="I6" s="13" t="inlineStr">
+        <is>
+          <t>Cartera vencida total</t>
+        </is>
+      </c>
+      <c r="J6" s="13" t="inlineStr">
+        <is>
+          <t>%mora</t>
+        </is>
+      </c>
+      <c r="K6" s="13" t="inlineStr">
+        <is>
+          <t>Saldo en riesgo</t>
+        </is>
+      </c>
+      <c r="L6" s="13" t="inlineStr">
+        <is>
+          <t>Días de mora</t>
+        </is>
+      </c>
+      <c r="M6" s="13" t="inlineStr">
+        <is>
+          <t>Mora potencial mensual</t>
+        </is>
+      </c>
+      <c r="N6" s="13" t="inlineStr">
+        <is>
+          <t>Cartera vencida total</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correct: fixing algorithm to get the CARTERA INIICAL SISTEMA field
</commit_message>
<xml_diff>
--- a/output_automatizado.xlsx
+++ b/output_automatizado.xlsx
@@ -954,19 +954,19 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>27000.24</v>
+        <v>32832.51</v>
       </c>
       <c r="P7" t="n">
         <v>58368.48</v>
       </c>
       <c r="Q7" t="n">
-        <v>32832.27</v>
+        <v>32832.51</v>
       </c>
       <c r="R7" t="n">
         <v>27000.24</v>
       </c>
       <c r="S7" t="n">
-        <v>-5832.030000000002</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
         <v>0</v>
@@ -1086,7 +1086,7 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>88500</v>
+        <v>107585.26</v>
       </c>
       <c r="P8" t="n">
         <v>143489.28</v>
@@ -1098,7 +1098,7 @@
         <v>88500</v>
       </c>
       <c r="S8" t="n">
-        <v>-19116.95999999999</v>
+        <v>-31.69999999998254</v>
       </c>
       <c r="T8" t="n">
         <v>0</v>
@@ -1218,19 +1218,19 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>54000.02</v>
+        <v>65664.59</v>
       </c>
       <c r="P9" t="n">
         <v>131329.12</v>
       </c>
       <c r="Q9" t="n">
-        <v>65664.56</v>
+        <v>65664.59</v>
       </c>
       <c r="R9" t="n">
         <v>54000.02</v>
       </c>
       <c r="S9" t="n">
-        <v>-11664.53999999999</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
         <v>0</v>
@@ -1350,19 +1350,19 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>45500.02</v>
+        <v>55328.49</v>
       </c>
       <c r="P10" t="n">
         <v>110656.96</v>
       </c>
       <c r="Q10" t="n">
-        <v>55328.48</v>
+        <v>55328.49</v>
       </c>
       <c r="R10" t="n">
         <v>45500.02</v>
       </c>
       <c r="S10" t="n">
-        <v>-9828.459999999999</v>
+        <v>0</v>
       </c>
       <c r="T10" t="n">
         <v>0</v>
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>34875</v>
+        <v>42366.66</v>
       </c>
       <c r="P11" t="n">
         <v>75392.64</v>
@@ -1494,7 +1494,7 @@
         <v>34875</v>
       </c>
       <c r="S11" t="n">
-        <v>-12245.4</v>
+        <v>-4753.739999999998</v>
       </c>
       <c r="T11" t="n">
         <v>0</v>
@@ -1614,7 +1614,7 @@
         </is>
       </c>
       <c r="O12" t="n">
-        <v>100000</v>
+        <v>121599.71</v>
       </c>
       <c r="P12" t="n">
         <v>194561.76</v>
@@ -1626,7 +1626,7 @@
         <v>100000</v>
       </c>
       <c r="S12" t="n">
-        <v>-21601.10000000001</v>
+        <v>-1.389999999999418</v>
       </c>
       <c r="T12" t="n">
         <v>0</v>
@@ -1746,7 +1746,7 @@
         </is>
       </c>
       <c r="O13" t="n">
-        <v>47500</v>
+        <v>57724.76</v>
       </c>
       <c r="P13" t="n">
         <v>92416.8</v>
@@ -1758,7 +1758,7 @@
         <v>47500</v>
       </c>
       <c r="S13" t="n">
-        <v>-10260.5</v>
+        <v>-35.73999999999796</v>
       </c>
       <c r="T13" t="n">
         <v>0</v>
@@ -1878,7 +1878,7 @@
         </is>
       </c>
       <c r="O14" t="n">
-        <v>37500.86</v>
+        <v>45601.28</v>
       </c>
       <c r="P14" t="n">
         <v>145921.28</v>
@@ -1890,7 +1890,7 @@
         <v>37500.86</v>
       </c>
       <c r="S14" t="n">
-        <v>-17219.62</v>
+        <v>-9119.199999999997</v>
       </c>
       <c r="T14" t="n">
         <v>0</v>
@@ -2010,19 +2010,19 @@
         </is>
       </c>
       <c r="O15" t="n">
-        <v>64126.14</v>
+        <v>77977.82000000001</v>
       </c>
       <c r="P15" t="n">
         <v>207937.76</v>
       </c>
       <c r="Q15" t="n">
-        <v>77976.66</v>
+        <v>77977.82000000001</v>
       </c>
       <c r="R15" t="n">
         <v>64126.14</v>
       </c>
       <c r="S15" t="n">
-        <v>-13850.52</v>
+        <v>0</v>
       </c>
       <c r="T15" t="n">
         <v>0</v>
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="O16" t="n">
-        <v>93750</v>
+        <v>113995.07</v>
       </c>
       <c r="P16" t="n">
         <v>121601.12</v>
@@ -2154,7 +2154,7 @@
         <v>93750</v>
       </c>
       <c r="S16" t="n">
-        <v>-20251.04999999999</v>
+        <v>-5.979999999981374</v>
       </c>
       <c r="T16" t="n">
         <v>0</v>
@@ -2274,7 +2274,7 @@
         </is>
       </c>
       <c r="O17" t="n">
-        <v>45000</v>
+        <v>54719.64</v>
       </c>
       <c r="P17" t="n">
         <v>72960.64</v>
@@ -2286,7 +2286,7 @@
         <v>45000</v>
       </c>
       <c r="S17" t="n">
-        <v>-9720.479999999996</v>
+        <v>-0.8399999999965075</v>
       </c>
       <c r="T17" t="n">
         <v>0</v>
@@ -2406,7 +2406,7 @@
         </is>
       </c>
       <c r="O18" t="n">
-        <v>52500</v>
+        <v>63838.75</v>
       </c>
       <c r="P18" t="n">
         <v>85120.8</v>
@@ -2418,7 +2418,7 @@
         <v>52500</v>
       </c>
       <c r="S18" t="n">
-        <v>-11340.60000000001</v>
+        <v>-1.850000000005821</v>
       </c>
       <c r="T18" t="n">
         <v>0</v>
@@ -2538,7 +2538,7 @@
         </is>
       </c>
       <c r="O19" t="n">
-        <v>70000</v>
+        <v>85120.75</v>
       </c>
       <c r="P19" t="n">
         <v>85120.8</v>
@@ -2550,7 +2550,7 @@
         <v>70000</v>
       </c>
       <c r="S19" t="n">
-        <v>-15120.8</v>
+        <v>-0.05000000000291038</v>
       </c>
       <c r="T19" t="n">
         <v>0</v>
@@ -2670,19 +2670,19 @@
         </is>
       </c>
       <c r="O20" t="n">
-        <v>17750.51</v>
+        <v>21584.71</v>
       </c>
       <c r="P20" t="n">
         <v>86336.8</v>
       </c>
       <c r="Q20" t="n">
-        <v>21584.2</v>
+        <v>21584.71</v>
       </c>
       <c r="R20" t="n">
         <v>17750.51</v>
       </c>
       <c r="S20" t="n">
-        <v>-3833.689999999995</v>
+        <v>0</v>
       </c>
       <c r="T20" t="n">
         <v>0</v>
@@ -2802,7 +2802,7 @@
         </is>
       </c>
       <c r="O21" t="n">
-        <v>92125</v>
+        <v>112024.43</v>
       </c>
       <c r="P21" t="n">
         <v>162945.44</v>
@@ -2814,7 +2814,7 @@
         <v>92125</v>
       </c>
       <c r="S21" t="n">
-        <v>-19899.99000000001</v>
+        <v>-0.5599999999976717</v>
       </c>
       <c r="T21" t="n">
         <v>0</v>
@@ -2934,19 +2934,19 @@
         </is>
       </c>
       <c r="O22" t="n">
-        <v>24063.07</v>
+        <v>29260.82</v>
       </c>
       <c r="P22" t="n">
         <v>93632.8</v>
       </c>
       <c r="Q22" t="n">
-        <v>29260.25</v>
+        <v>29260.82</v>
       </c>
       <c r="R22" t="n">
         <v>24063.07</v>
       </c>
       <c r="S22" t="n">
-        <v>-5197.18</v>
+        <v>0</v>
       </c>
       <c r="T22" t="n">
         <v>0</v>
@@ -3066,19 +3066,19 @@
         </is>
       </c>
       <c r="O23" t="n">
-        <v>41250.26</v>
+        <v>50160.7</v>
       </c>
       <c r="P23" t="n">
         <v>80256.64</v>
       </c>
       <c r="Q23" t="n">
-        <v>50160.4</v>
+        <v>50160.7</v>
       </c>
       <c r="R23" t="n">
         <v>41250.26</v>
       </c>
       <c r="S23" t="n">
-        <v>-8910.139999999999</v>
+        <v>0</v>
       </c>
       <c r="T23" t="n">
         <v>0</v>
@@ -3198,7 +3198,7 @@
         </is>
       </c>
       <c r="O24" t="n">
-        <v>24062.5</v>
+        <v>29258.77</v>
       </c>
       <c r="P24" t="n">
         <v>93632.8</v>
@@ -3210,7 +3210,7 @@
         <v>24062.5</v>
       </c>
       <c r="S24" t="n">
-        <v>-5197.75</v>
+        <v>-1.479999999999563</v>
       </c>
       <c r="T24" t="n">
         <v>0</v>
@@ -3330,7 +3330,7 @@
         </is>
       </c>
       <c r="O25" t="n">
-        <v>30937.5</v>
+        <v>37620.31</v>
       </c>
       <c r="P25" t="n">
         <v>66880.64</v>
@@ -3342,7 +3342,7 @@
         <v>30937.5</v>
       </c>
       <c r="S25" t="n">
-        <v>-6682.860000000001</v>
+        <v>-0.05000000000291038</v>
       </c>
       <c r="T25" t="n">
         <v>0</v>
@@ -3462,7 +3462,7 @@
         </is>
       </c>
       <c r="O26" t="n">
-        <v>35437.5</v>
+        <v>43086.67</v>
       </c>
       <c r="P26" t="n">
         <v>76608.64</v>
@@ -3474,7 +3474,7 @@
         <v>35437.5</v>
       </c>
       <c r="S26" t="n">
-        <v>-7654.860000000001</v>
+        <v>-5.690000000002328</v>
       </c>
       <c r="T26" t="n">
         <v>0</v>
@@ -3594,7 +3594,7 @@
         </is>
       </c>
       <c r="O27" t="n">
-        <v>45625</v>
+        <v>55479.46</v>
       </c>
       <c r="P27" t="n">
         <v>177537.6</v>
@@ -3606,7 +3606,7 @@
         <v>45625</v>
       </c>
       <c r="S27" t="n">
-        <v>-9855.5</v>
+        <v>-1.040000000000873</v>
       </c>
       <c r="T27" t="n">
         <v>0</v>
@@ -3726,7 +3726,7 @@
         </is>
       </c>
       <c r="O28" t="n">
-        <v>76000</v>
+        <v>92409.62</v>
       </c>
       <c r="P28" t="n">
         <v>184833.6</v>
@@ -3738,7 +3738,7 @@
         <v>76000</v>
       </c>
       <c r="S28" t="n">
-        <v>-16416.8</v>
+        <v>-7.180000000007567</v>
       </c>
       <c r="T28" t="n">
         <v>0</v>
@@ -3858,19 +3858,19 @@
         </is>
       </c>
       <c r="O29" t="n">
-        <v>88125</v>
+        <v>107160.94</v>
       </c>
       <c r="P29" t="n">
         <v>114304.96</v>
       </c>
       <c r="Q29" t="n">
-        <v>107160.9</v>
+        <v>107160.94</v>
       </c>
       <c r="R29" t="n">
         <v>88125</v>
       </c>
       <c r="S29" t="n">
-        <v>-19035.90000000001</v>
+        <v>0</v>
       </c>
       <c r="T29" t="n">
         <v>0</v>
@@ -3990,7 +3990,7 @@
         </is>
       </c>
       <c r="O30" t="n">
-        <v>21875</v>
+        <v>26594.51</v>
       </c>
       <c r="P30" t="n">
         <v>60800.48</v>
@@ -4002,7 +4002,7 @@
         <v>21875</v>
       </c>
       <c r="S30" t="n">
-        <v>-4725.209999999999</v>
+        <v>-5.69999999999709</v>
       </c>
       <c r="T30" t="n">
         <v>0</v>
@@ -4122,19 +4122,19 @@
         </is>
       </c>
       <c r="O31" t="n">
-        <v>48750.13</v>
+        <v>59280.64</v>
       </c>
       <c r="P31" t="n">
         <v>72960.64</v>
       </c>
       <c r="Q31" t="n">
-        <v>59280.52</v>
+        <v>59280.64</v>
       </c>
       <c r="R31" t="n">
         <v>48750.13</v>
       </c>
       <c r="S31" t="n">
-        <v>-10530.39000000001</v>
+        <v>0</v>
       </c>
       <c r="T31" t="n">
         <v>0</v>
@@ -4254,7 +4254,7 @@
         </is>
       </c>
       <c r="O32" t="n">
-        <v>48562.5</v>
+        <v>59020.11</v>
       </c>
       <c r="P32" t="n">
         <v>134977.12</v>
@@ -4266,7 +4266,7 @@
         <v>48562.5</v>
       </c>
       <c r="S32" t="n">
-        <v>-10489.98999999999</v>
+        <v>-32.3799999999901</v>
       </c>
       <c r="T32" t="n">
         <v>0</v>
@@ -4386,19 +4386,19 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>92500.00999999999</v>
+        <v>112480.97</v>
       </c>
       <c r="P33" t="n">
         <v>224961.92</v>
       </c>
       <c r="Q33" t="n">
-        <v>112480.96</v>
+        <v>112480.97</v>
       </c>
       <c r="R33" t="n">
         <v>92500.00999999999</v>
       </c>
       <c r="S33" t="n">
-        <v>-19980.95000000001</v>
+        <v>0</v>
       </c>
       <c r="T33" t="n">
         <v>0</v>
@@ -4518,7 +4518,7 @@
         </is>
       </c>
       <c r="O34" t="n">
-        <v>39626.82</v>
+        <v>47524.69</v>
       </c>
       <c r="P34" t="n">
         <v>79040.64</v>
@@ -4530,7 +4530,7 @@
         <v>39626.82</v>
       </c>
       <c r="S34" t="n">
-        <v>-9773.580000000002</v>
+        <v>-1875.709999999999</v>
       </c>
       <c r="T34" t="n">
         <v>0</v>
@@ -4650,19 +4650,19 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>588000</v>
+        <v>715014.27</v>
       </c>
       <c r="P35" t="n">
         <v>715014.24</v>
       </c>
       <c r="Q35" t="n">
-        <v>715014.24</v>
+        <v>715014.27</v>
       </c>
       <c r="R35" t="n">
         <v>588000</v>
       </c>
       <c r="S35" t="n">
-        <v>-127014.24</v>
+        <v>0</v>
       </c>
       <c r="T35" t="n">
         <v>0</v>
@@ -4782,19 +4782,19 @@
         </is>
       </c>
       <c r="O36" t="n">
-        <v>588000</v>
+        <v>715014.27</v>
       </c>
       <c r="P36" t="n">
         <v>715014.24</v>
       </c>
       <c r="Q36" t="n">
-        <v>715014.24</v>
+        <v>715014.27</v>
       </c>
       <c r="R36" t="n">
         <v>588000</v>
       </c>
       <c r="S36" t="n">
-        <v>-127014.24</v>
+        <v>0</v>
       </c>
       <c r="T36" t="n">
         <v>0</v>
@@ -4914,19 +4914,19 @@
         </is>
       </c>
       <c r="O37" t="n">
-        <v>29625.03</v>
+        <v>36024.34</v>
       </c>
       <c r="P37" t="n">
         <v>96064.8</v>
       </c>
       <c r="Q37" t="n">
-        <v>36024.3</v>
+        <v>36024.34</v>
       </c>
       <c r="R37" t="n">
         <v>29625.03</v>
       </c>
       <c r="S37" t="n">
-        <v>-6399.270000000004</v>
+        <v>0</v>
       </c>
       <c r="T37" t="n">
         <v>0</v>
@@ -5046,7 +5046,7 @@
         </is>
       </c>
       <c r="O38" t="n">
-        <v>19125</v>
+        <v>23252.54</v>
       </c>
       <c r="P38" t="n">
         <v>62016.48</v>
@@ -5058,7 +5058,7 @@
         <v>19125</v>
       </c>
       <c r="S38" t="n">
-        <v>-4131.18</v>
+        <v>-3.639999999999418</v>
       </c>
       <c r="T38" t="n">
         <v>0</v>
@@ -5178,7 +5178,7 @@
         </is>
       </c>
       <c r="O39" t="n">
-        <v>63000</v>
+        <v>76607.54000000001</v>
       </c>
       <c r="P39" t="n">
         <v>175105.6</v>
@@ -5190,7 +5190,7 @@
         <v>63000</v>
       </c>
       <c r="S39" t="n">
-        <v>-13608.7</v>
+        <v>-1.159999999988941</v>
       </c>
       <c r="T39" t="n">
         <v>0</v>
@@ -5310,7 +5310,7 @@
         </is>
       </c>
       <c r="O40" t="n">
-        <v>30000</v>
+        <v>36430.85</v>
       </c>
       <c r="P40" t="n">
         <v>97280.8</v>
@@ -5322,7 +5322,7 @@
         <v>30000</v>
       </c>
       <c r="S40" t="n">
-        <v>-6480.300000000003</v>
+        <v>-49.45000000000437</v>
       </c>
       <c r="T40" t="n">
         <v>0</v>
@@ -5442,7 +5442,7 @@
         </is>
       </c>
       <c r="O41" t="n">
-        <v>112875.16</v>
+        <v>137257.38</v>
       </c>
       <c r="P41" t="n">
         <v>156865.44</v>
@@ -5454,7 +5454,7 @@
         <v>112875.16</v>
       </c>
       <c r="S41" t="n">
-        <v>-34186.19</v>
+        <v>-9803.970000000001</v>
       </c>
       <c r="T41" t="n">
         <v>0</v>
@@ -5574,7 +5574,7 @@
         </is>
       </c>
       <c r="O42" t="n">
-        <v>180000</v>
+        <v>218881.92</v>
       </c>
       <c r="P42" t="n">
         <v>218881.92</v>
@@ -5586,7 +5586,7 @@
         <v>180000</v>
       </c>
       <c r="S42" t="n">
-        <v>-38881.92000000001</v>
+        <v>0</v>
       </c>
       <c r="T42" t="n">
         <v>0</v>
@@ -5706,7 +5706,7 @@
         </is>
       </c>
       <c r="O43" t="n">
-        <v>180000</v>
+        <v>218881.92</v>
       </c>
       <c r="P43" t="n">
         <v>218881.92</v>
@@ -5718,7 +5718,7 @@
         <v>180000</v>
       </c>
       <c r="S43" t="n">
-        <v>-38881.92000000001</v>
+        <v>0</v>
       </c>
       <c r="T43" t="n">
         <v>0</v>
@@ -5838,7 +5838,7 @@
         </is>
       </c>
       <c r="O44" t="n">
-        <v>77687.5</v>
+        <v>94461.21000000001</v>
       </c>
       <c r="P44" t="n">
         <v>137409.28</v>
@@ -5850,7 +5850,7 @@
         <v>77687.5</v>
       </c>
       <c r="S44" t="n">
-        <v>-16781.38</v>
+        <v>-7.669999999998254</v>
       </c>
       <c r="T44" t="n">
         <v>0</v>
@@ -5970,7 +5970,7 @@
         </is>
       </c>
       <c r="O45" t="n">
-        <v>99000</v>
+        <v>119293.11</v>
       </c>
       <c r="P45" t="n">
         <v>240770.08</v>
@@ -5982,7 +5982,7 @@
         <v>99000</v>
       </c>
       <c r="S45" t="n">
-        <v>-21385.04000000001</v>
+        <v>-1091.930000000008</v>
       </c>
       <c r="T45" t="n">
         <v>0</v>
@@ -6102,7 +6102,7 @@
         </is>
       </c>
       <c r="O46" t="n">
-        <v>50000</v>
+        <v>60768.07</v>
       </c>
       <c r="P46" t="n">
         <v>121601.12</v>
@@ -6114,7 +6114,7 @@
         <v>50000</v>
       </c>
       <c r="S46" t="n">
-        <v>-10800.56</v>
+        <v>-32.48999999999796</v>
       </c>
       <c r="T46" t="n">
         <v>0</v>
@@ -6234,7 +6234,7 @@
         </is>
       </c>
       <c r="O47" t="n">
-        <v>50625</v>
+        <v>61559.58</v>
       </c>
       <c r="P47" t="n">
         <v>65664.64</v>
@@ -6246,7 +6246,7 @@
         <v>50625</v>
       </c>
       <c r="S47" t="n">
-        <v>-10935.6</v>
+        <v>-1.019999999996799</v>
       </c>
       <c r="T47" t="n">
         <v>0</v>
@@ -6366,7 +6366,7 @@
         </is>
       </c>
       <c r="O48" t="n">
-        <v>19500</v>
+        <v>23559.73</v>
       </c>
       <c r="P48" t="n">
         <v>94848.8</v>
@@ -6378,7 +6378,7 @@
         <v>19500</v>
       </c>
       <c r="S48" t="n">
-        <v>-4212.199999999997</v>
+        <v>-152.4699999999975</v>
       </c>
       <c r="T48" t="n">
         <v>0</v>
@@ -6498,7 +6498,7 @@
         </is>
       </c>
       <c r="O49" t="n">
-        <v>168750</v>
+        <v>205200.92</v>
       </c>
       <c r="P49" t="n">
         <v>218881.92</v>
@@ -6510,7 +6510,7 @@
         <v>168750</v>
       </c>
       <c r="S49" t="n">
-        <v>-36451.80000000002</v>
+        <v>-0.8800000000046566</v>
       </c>
       <c r="T49" t="n">
         <v>0</v>
@@ -6630,7 +6630,7 @@
         </is>
       </c>
       <c r="O50" t="n">
-        <v>134375</v>
+        <v>163401.15</v>
       </c>
       <c r="P50" t="n">
         <v>261442.24</v>
@@ -6642,7 +6642,7 @@
         <v>134375</v>
       </c>
       <c r="S50" t="n">
-        <v>-29026.40000000002</v>
+        <v>-0.2500000000291038</v>
       </c>
       <c r="T50" t="n">
         <v>0</v>
@@ -6762,19 +6762,19 @@
         </is>
       </c>
       <c r="O51" t="n">
-        <v>37500.2</v>
+        <v>45600.6</v>
       </c>
       <c r="P51" t="n">
         <v>72960.64</v>
       </c>
       <c r="Q51" t="n">
-        <v>45600.4</v>
+        <v>45600.6</v>
       </c>
       <c r="R51" t="n">
         <v>37500.2</v>
       </c>
       <c r="S51" t="n">
-        <v>-8100.199999999997</v>
+        <v>0</v>
       </c>
       <c r="T51" t="n">
         <v>0</v>
@@ -6894,19 +6894,19 @@
         </is>
       </c>
       <c r="O52" t="n">
-        <v>101562.74</v>
+        <v>123501.33</v>
       </c>
       <c r="P52" t="n">
         <v>152001.28</v>
       </c>
       <c r="Q52" t="n">
-        <v>123501.04</v>
+        <v>123501.33</v>
       </c>
       <c r="R52" t="n">
         <v>101562.74</v>
       </c>
       <c r="S52" t="n">
-        <v>-21938.3</v>
+        <v>0</v>
       </c>
       <c r="T52" t="n">
         <v>0</v>
@@ -7026,7 +7026,7 @@
         </is>
       </c>
       <c r="O53" t="n">
-        <v>50375</v>
+        <v>61251.66</v>
       </c>
       <c r="P53" t="n">
         <v>75392.64</v>
@@ -7038,7 +7038,7 @@
         <v>50375</v>
       </c>
       <c r="S53" t="n">
-        <v>-10881.52</v>
+        <v>-4.860000000000582</v>
       </c>
       <c r="T53" t="n">
         <v>0</v>
@@ -7158,7 +7158,7 @@
         </is>
       </c>
       <c r="O54" t="n">
-        <v>64312.5</v>
+        <v>78161.57000000001</v>
       </c>
       <c r="P54" t="n">
         <v>178753.6</v>
@@ -7170,7 +7170,7 @@
         <v>64312.5</v>
       </c>
       <c r="S54" t="n">
-        <v>-13892.2</v>
+        <v>-43.1299999999901</v>
       </c>
       <c r="T54" t="n">
         <v>0</v>
@@ -7290,7 +7290,7 @@
         </is>
       </c>
       <c r="O55" t="n">
-        <v>50625</v>
+        <v>61559.96</v>
       </c>
       <c r="P55" t="n">
         <v>109440.96</v>
@@ -7302,7 +7302,7 @@
         <v>50625</v>
       </c>
       <c r="S55" t="n">
-        <v>-10935.54</v>
+        <v>-0.5800000000017462</v>
       </c>
       <c r="T55" t="n">
         <v>0</v>
@@ -7422,7 +7422,7 @@
         </is>
       </c>
       <c r="O56" t="n">
-        <v>46875</v>
+        <v>56913.6</v>
       </c>
       <c r="P56" t="n">
         <v>182401.6</v>
@@ -7434,7 +7434,7 @@
         <v>46875</v>
       </c>
       <c r="S56" t="n">
-        <v>-10125.5</v>
+        <v>-86.90000000000146</v>
       </c>
       <c r="T56" t="n">
         <v>0</v>
@@ -7554,19 +7554,19 @@
         </is>
       </c>
       <c r="O57" t="n">
-        <v>187500.02</v>
+        <v>228002</v>
       </c>
       <c r="P57" t="n">
         <v>243202.08</v>
       </c>
       <c r="Q57" t="n">
-        <v>228001.95</v>
+        <v>228002</v>
       </c>
       <c r="R57" t="n">
         <v>187500.02</v>
       </c>
       <c r="S57" t="n">
-        <v>-40501.93000000002</v>
+        <v>0</v>
       </c>
       <c r="T57" t="n">
         <v>0</v>
@@ -7686,7 +7686,7 @@
         </is>
       </c>
       <c r="O58" t="n">
-        <v>151375</v>
+        <v>184064.85</v>
       </c>
       <c r="P58" t="n">
         <v>210369.92</v>
@@ -7698,7 +7698,7 @@
         <v>151375</v>
       </c>
       <c r="S58" t="n">
-        <v>-32698.68000000002</v>
+        <v>-8.830000000016298</v>
       </c>
       <c r="T58" t="n">
         <v>0</v>
@@ -7818,19 +7818,19 @@
         </is>
       </c>
       <c r="O59" t="n">
-        <v>48125.02</v>
+        <v>58520.54</v>
       </c>
       <c r="P59" t="n">
         <v>133761.12</v>
       </c>
       <c r="Q59" t="n">
-        <v>58520.48999999999</v>
+        <v>58520.54</v>
       </c>
       <c r="R59" t="n">
         <v>48125.02</v>
       </c>
       <c r="S59" t="n">
-        <v>-10395.46999999999</v>
+        <v>0</v>
       </c>
       <c r="T59" t="n">
         <v>0</v>
@@ -7950,7 +7950,7 @@
         </is>
       </c>
       <c r="O60" t="n">
-        <v>50500</v>
+        <v>61318.08</v>
       </c>
       <c r="P60" t="n">
         <v>122817.12</v>
@@ -7962,7 +7962,7 @@
         <v>50500</v>
       </c>
       <c r="S60" t="n">
-        <v>-10908.56</v>
+        <v>-90.47999999999593</v>
       </c>
       <c r="T60" t="n">
         <v>0</v>
@@ -8082,7 +8082,7 @@
         </is>
       </c>
       <c r="O61" t="n">
-        <v>30500</v>
+        <v>37083.65</v>
       </c>
       <c r="P61" t="n">
         <v>74176.64</v>
@@ -8094,7 +8094,7 @@
         <v>30500</v>
       </c>
       <c r="S61" t="n">
-        <v>-6588.32</v>
+        <v>-4.669999999998254</v>
       </c>
       <c r="T61" t="n">
         <v>0</v>
@@ -8214,7 +8214,7 @@
         </is>
       </c>
       <c r="O62" t="n">
-        <v>38000</v>
+        <v>46161.81</v>
       </c>
       <c r="P62" t="n">
         <v>92416.8</v>
@@ -8226,7 +8226,7 @@
         <v>38000</v>
       </c>
       <c r="S62" t="n">
-        <v>-8208.400000000001</v>
+        <v>-46.59000000000378</v>
       </c>
       <c r="T62" t="n">
         <v>0</v>
@@ -8346,7 +8346,7 @@
         </is>
       </c>
       <c r="O63" t="n">
-        <v>36875.24</v>
+        <v>44840.63</v>
       </c>
       <c r="P63" t="n">
         <v>71744.64</v>
@@ -8358,7 +8358,7 @@
         <v>36875.24</v>
       </c>
       <c r="S63" t="n">
-        <v>-12449.2</v>
+        <v>-4483.810000000005</v>
       </c>
       <c r="T63" t="n">
         <v>0</v>
@@ -8478,19 +8478,19 @@
         </is>
       </c>
       <c r="O64" t="n">
-        <v>52500</v>
+        <v>84353.49000000001</v>
       </c>
       <c r="P64" t="n">
         <v>170241.44</v>
       </c>
       <c r="Q64" t="n">
-        <v>63840.54000000001</v>
+        <v>84353.49000000001</v>
       </c>
       <c r="R64" t="n">
         <v>52500</v>
       </c>
       <c r="S64" t="n">
-        <v>-11340.54000000001</v>
+        <v>0</v>
       </c>
       <c r="T64" t="n">
         <v>15230</v>
@@ -8610,7 +8610,7 @@
         </is>
       </c>
       <c r="O65" t="n">
-        <v>94687.5</v>
+        <v>115133.08</v>
       </c>
       <c r="P65" t="n">
         <v>122817.12</v>
@@ -8622,7 +8622,7 @@
         <v>94687.5</v>
       </c>
       <c r="S65" t="n">
-        <v>-20453.54999999999</v>
+        <v>-7.969999999986612</v>
       </c>
       <c r="T65" t="n">
         <v>0</v>
@@ -8742,7 +8742,7 @@
         </is>
       </c>
       <c r="O66" t="n">
-        <v>43000</v>
+        <v>52288.46</v>
       </c>
       <c r="P66" t="n">
         <v>52288.48</v>
@@ -8754,7 +8754,7 @@
         <v>43000</v>
       </c>
       <c r="S66" t="n">
-        <v>-9288.480000000003</v>
+        <v>-0.02000000000407454</v>
       </c>
       <c r="T66" t="n">
         <v>0</v>
@@ -8874,19 +8874,19 @@
         </is>
       </c>
       <c r="O67" t="n">
-        <v>26250.16</v>
+        <v>31920.45</v>
       </c>
       <c r="P67" t="n">
         <v>51072.48</v>
       </c>
       <c r="Q67" t="n">
-        <v>31920.3</v>
+        <v>31920.45</v>
       </c>
       <c r="R67" t="n">
         <v>26250.16</v>
       </c>
       <c r="S67" t="n">
-        <v>-5670.140000000003</v>
+        <v>0</v>
       </c>
       <c r="T67" t="n">
         <v>0</v>
@@ -9006,7 +9006,7 @@
         </is>
       </c>
       <c r="O68" t="n">
-        <v>70687.5</v>
+        <v>85954.92</v>
       </c>
       <c r="P68" t="n">
         <v>105792.96</v>
@@ -9018,7 +9018,7 @@
         <v>70687.5</v>
       </c>
       <c r="S68" t="n">
-        <v>-15269.28</v>
+        <v>-1.860000000000582</v>
       </c>
       <c r="T68" t="n">
         <v>0</v>
@@ -9138,7 +9138,7 @@
         </is>
       </c>
       <c r="O69" t="n">
-        <v>28500</v>
+        <v>34586.81</v>
       </c>
       <c r="P69" t="n">
         <v>92416.8</v>
@@ -9150,7 +9150,7 @@
         <v>28500</v>
       </c>
       <c r="S69" t="n">
-        <v>-6156.300000000003</v>
+        <v>-69.49000000000524</v>
       </c>
       <c r="T69" t="n">
         <v>0</v>
@@ -9270,19 +9270,19 @@
         </is>
       </c>
       <c r="O70" t="n">
-        <v>35625.63</v>
+        <v>43321.01</v>
       </c>
       <c r="P70" t="n">
         <v>115520.96</v>
       </c>
       <c r="Q70" t="n">
-        <v>43320.36</v>
+        <v>43321.01</v>
       </c>
       <c r="R70" t="n">
         <v>35625.63</v>
       </c>
       <c r="S70" t="n">
-        <v>-7694.730000000003</v>
+        <v>0</v>
       </c>
       <c r="T70" t="n">
         <v>0</v>
@@ -9402,19 +9402,19 @@
         </is>
       </c>
       <c r="O71" t="n">
-        <v>52812.51</v>
+        <v>64220.57</v>
       </c>
       <c r="P71" t="n">
         <v>79040.64</v>
       </c>
       <c r="Q71" t="n">
-        <v>64220.52</v>
+        <v>64220.57</v>
       </c>
       <c r="R71" t="n">
         <v>52812.51</v>
       </c>
       <c r="S71" t="n">
-        <v>-11408.01</v>
+        <v>0</v>
       </c>
       <c r="T71" t="n">
         <v>0</v>
@@ -9534,19 +9534,19 @@
         </is>
       </c>
       <c r="O72" t="n">
-        <v>25500</v>
+        <v>36176.28</v>
       </c>
       <c r="P72" t="n">
         <v>82688.8</v>
       </c>
       <c r="Q72" t="n">
-        <v>31008.3</v>
+        <v>36176.28</v>
       </c>
       <c r="R72" t="n">
         <v>25500</v>
       </c>
       <c r="S72" t="n">
-        <v>-5508.300000000003</v>
+        <v>0</v>
       </c>
       <c r="T72" t="n">
         <v>4250</v>
@@ -9666,19 +9666,19 @@
         </is>
       </c>
       <c r="O73" t="n">
-        <v>79750.39</v>
+        <v>96977.24000000001</v>
       </c>
       <c r="P73" t="n">
         <v>141057.28</v>
       </c>
       <c r="Q73" t="n">
-        <v>96976.88</v>
+        <v>96977.24000000001</v>
       </c>
       <c r="R73" t="n">
         <v>79750.39</v>
       </c>
       <c r="S73" t="n">
-        <v>-17226.49000000001</v>
+        <v>0</v>
       </c>
       <c r="T73" t="n">
         <v>0</v>
@@ -9798,19 +9798,19 @@
         </is>
       </c>
       <c r="O74" t="n">
-        <v>48000</v>
+        <v>58368.51</v>
       </c>
       <c r="P74" t="n">
         <v>58368.48</v>
       </c>
       <c r="Q74" t="n">
-        <v>58368.48</v>
+        <v>58368.51</v>
       </c>
       <c r="R74" t="n">
         <v>48000</v>
       </c>
       <c r="S74" t="n">
-        <v>-10368.48</v>
+        <v>0</v>
       </c>
       <c r="T74" t="n">
         <v>0</v>
@@ -9930,7 +9930,7 @@
         </is>
       </c>
       <c r="O75" t="n">
-        <v>87500</v>
+        <v>106395.49</v>
       </c>
       <c r="P75" t="n">
         <v>170241.44</v>
@@ -9942,7 +9942,7 @@
         <v>87500</v>
       </c>
       <c r="S75" t="n">
-        <v>-18900.89999999999</v>
+        <v>-5.409999999988941</v>
       </c>
       <c r="T75" t="n">
         <v>0</v>
@@ -10062,7 +10062,7 @@
         </is>
       </c>
       <c r="O76" t="n">
-        <v>75250</v>
+        <v>91503.92</v>
       </c>
       <c r="P76" t="n">
         <v>104576.96</v>
@@ -10074,7 +10074,7 @@
         <v>75250</v>
       </c>
       <c r="S76" t="n">
-        <v>-22790.90000000001</v>
+        <v>-6536.98000000001</v>
       </c>
       <c r="T76" t="n">
         <v>0</v>
@@ -10194,7 +10194,7 @@
         </is>
       </c>
       <c r="O77" t="n">
-        <v>51562.5</v>
+        <v>62691.59</v>
       </c>
       <c r="P77" t="n">
         <v>66880.64</v>
@@ -10206,7 +10206,7 @@
         <v>51562.5</v>
       </c>
       <c r="S77" t="n">
-        <v>-11138.1</v>
+        <v>-9.009999999994761</v>
       </c>
       <c r="T77" t="n">
         <v>0</v>
@@ -10326,7 +10326,7 @@
         </is>
       </c>
       <c r="O78" t="n">
-        <v>78125</v>
+        <v>94967.33</v>
       </c>
       <c r="P78" t="n">
         <v>152001.28</v>
@@ -10338,7 +10338,7 @@
         <v>78125</v>
       </c>
       <c r="S78" t="n">
-        <v>-16875.8</v>
+        <v>-33.47000000000116</v>
       </c>
       <c r="T78" t="n">
         <v>0</v>
@@ -10458,19 +10458,19 @@
         </is>
       </c>
       <c r="O79" t="n">
-        <v>41875.03</v>
+        <v>50920.48</v>
       </c>
       <c r="P79" t="n">
         <v>162945.44</v>
       </c>
       <c r="Q79" t="n">
-        <v>50920.45</v>
+        <v>50920.48</v>
       </c>
       <c r="R79" t="n">
         <v>41875.03</v>
       </c>
       <c r="S79" t="n">
-        <v>-9045.419999999998</v>
+        <v>0</v>
       </c>
       <c r="T79" t="n">
         <v>0</v>
@@ -10590,7 +10590,7 @@
         </is>
       </c>
       <c r="O80" t="n">
-        <v>52187.5</v>
+        <v>63421.78</v>
       </c>
       <c r="P80" t="n">
         <v>203073.76</v>
@@ -10602,7 +10602,7 @@
         <v>52187.5</v>
       </c>
       <c r="S80" t="n">
-        <v>-11273.04999999999</v>
+        <v>-38.76999999998952</v>
       </c>
       <c r="T80" t="n">
         <v>0</v>
@@ -10722,7 +10722,7 @@
         </is>
       </c>
       <c r="O81" t="n">
-        <v>43125</v>
+        <v>52251.23</v>
       </c>
       <c r="P81" t="n">
         <v>139841.28</v>
@@ -10734,7 +10734,7 @@
         <v>43125</v>
       </c>
       <c r="S81" t="n">
-        <v>-9315.479999999996</v>
+        <v>-189.2499999999927</v>
       </c>
       <c r="T81" t="n">
         <v>0</v>
@@ -10854,7 +10854,7 @@
         </is>
       </c>
       <c r="O82" t="n">
-        <v>30000</v>
+        <v>36477.64</v>
       </c>
       <c r="P82" t="n">
         <v>72960.64</v>
@@ -10866,7 +10866,7 @@
         <v>30000</v>
       </c>
       <c r="S82" t="n">
-        <v>-6480.32</v>
+        <v>-2.680000000000291</v>
       </c>
       <c r="T82" t="n">
         <v>0</v>
@@ -10986,7 +10986,7 @@
         </is>
       </c>
       <c r="O83" t="n">
-        <v>60000</v>
+        <v>72918.68000000001</v>
       </c>
       <c r="P83" t="n">
         <v>77824.64</v>
@@ -10998,7 +10998,7 @@
         <v>60000</v>
       </c>
       <c r="S83" t="n">
-        <v>-12960.60000000001</v>
+        <v>-41.91999999999825</v>
       </c>
       <c r="T83" t="n">
         <v>0</v>
@@ -11118,7 +11118,7 @@
         </is>
       </c>
       <c r="O84" t="n">
-        <v>100343.75</v>
+        <v>122018.32</v>
       </c>
       <c r="P84" t="n">
         <v>150177.28</v>
@@ -11130,7 +11130,7 @@
         <v>100343.75</v>
       </c>
       <c r="S84" t="n">
-        <v>-21675.29000000001</v>
+        <v>-0.7200000000011642</v>
       </c>
       <c r="T84" t="n">
         <v>0</v>
@@ -11250,19 +11250,19 @@
         </is>
       </c>
       <c r="O85" t="n">
-        <v>78000</v>
+        <v>94848.83</v>
       </c>
       <c r="P85" t="n">
         <v>94848.8</v>
       </c>
       <c r="Q85" t="n">
-        <v>94848.8</v>
+        <v>94848.83</v>
       </c>
       <c r="R85" t="n">
         <v>78000</v>
       </c>
       <c r="S85" t="n">
-        <v>-16848.8</v>
+        <v>0</v>
       </c>
       <c r="T85" t="n">
         <v>0</v>
@@ -11382,7 +11382,7 @@
         </is>
       </c>
       <c r="O86" t="n">
-        <v>88562.5</v>
+        <v>107690.16</v>
       </c>
       <c r="P86" t="n">
         <v>132545.12</v>
@@ -11394,7 +11394,7 @@
         <v>88562.5</v>
       </c>
       <c r="S86" t="n">
-        <v>-19130.41</v>
+        <v>-2.75</v>
       </c>
       <c r="T86" t="n">
         <v>0</v>
@@ -11514,7 +11514,7 @@
         </is>
       </c>
       <c r="O87" t="n">
-        <v>69062.5</v>
+        <v>83965.91</v>
       </c>
       <c r="P87" t="n">
         <v>103360.96</v>
@@ -11526,7 +11526,7 @@
         <v>69062.5</v>
       </c>
       <c r="S87" t="n">
-        <v>-14918.28</v>
+        <v>-14.86999999999534</v>
       </c>
       <c r="T87" t="n">
         <v>0</v>
@@ -11646,7 +11646,7 @@
         </is>
       </c>
       <c r="O88" t="n">
-        <v>58000</v>
+        <v>70517.24000000001</v>
       </c>
       <c r="P88" t="n">
         <v>141057.28</v>
@@ -11658,7 +11658,7 @@
         <v>58000</v>
       </c>
       <c r="S88" t="n">
-        <v>-12528.64</v>
+        <v>-11.39999999999418</v>
       </c>
       <c r="T88" t="n">
         <v>0</v>
@@ -11778,7 +11778,7 @@
         </is>
       </c>
       <c r="O89" t="n">
-        <v>25000</v>
+        <v>30398.43</v>
       </c>
       <c r="P89" t="n">
         <v>48640.48</v>
@@ -11790,7 +11790,7 @@
         <v>25000</v>
       </c>
       <c r="S89" t="n">
-        <v>-8440.330000000002</v>
+        <v>-3041.900000000001</v>
       </c>
       <c r="T89" t="n">
         <v>0</v>
@@ -11910,19 +11910,19 @@
         </is>
       </c>
       <c r="O90" t="n">
-        <v>40313.45</v>
+        <v>49021.38</v>
       </c>
       <c r="P90" t="n">
         <v>156865.44</v>
       </c>
       <c r="Q90" t="n">
-        <v>49020.45</v>
+        <v>49021.38</v>
       </c>
       <c r="R90" t="n">
         <v>40313.45</v>
       </c>
       <c r="S90" t="n">
-        <v>-8706.999999999993</v>
+        <v>0</v>
       </c>
       <c r="T90" t="n">
         <v>0</v>
@@ -12042,7 +12042,7 @@
         </is>
       </c>
       <c r="O91" t="n">
-        <v>38437.5</v>
+        <v>46740.41</v>
       </c>
       <c r="P91" t="n">
         <v>49856.48</v>
@@ -12054,7 +12054,7 @@
         <v>38437.5</v>
       </c>
       <c r="S91" t="n">
-        <v>-8302.950000000004</v>
+        <v>-0.04000000000087311</v>
       </c>
       <c r="T91" t="n">
         <v>0</v>
@@ -12174,19 +12174,19 @@
         </is>
       </c>
       <c r="O92" t="n">
-        <v>121000</v>
+        <v>147137.29</v>
       </c>
       <c r="P92" t="n">
         <v>147137.28</v>
       </c>
       <c r="Q92" t="n">
-        <v>147137.28</v>
+        <v>147137.29</v>
       </c>
       <c r="R92" t="n">
         <v>121000</v>
       </c>
       <c r="S92" t="n">
-        <v>-26137.28</v>
+        <v>0</v>
       </c>
       <c r="T92" t="n">
         <v>0</v>
@@ -12306,19 +12306,19 @@
         </is>
       </c>
       <c r="O93" t="n">
-        <v>107000</v>
+        <v>130113.14</v>
       </c>
       <c r="P93" t="n">
         <v>130113.12</v>
       </c>
       <c r="Q93" t="n">
-        <v>130113.12</v>
+        <v>130113.14</v>
       </c>
       <c r="R93" t="n">
         <v>107000</v>
       </c>
       <c r="S93" t="n">
-        <v>-23113.12000000001</v>
+        <v>0</v>
       </c>
       <c r="T93" t="n">
         <v>0</v>
@@ -12438,7 +12438,7 @@
         </is>
       </c>
       <c r="O94" t="n">
-        <v>57062.5</v>
+        <v>69388.59</v>
       </c>
       <c r="P94" t="n">
         <v>100928.96</v>
@@ -12450,7 +12450,7 @@
         <v>57062.5</v>
       </c>
       <c r="S94" t="n">
-        <v>-12326.16</v>
+        <v>-0.07000000000698492</v>
       </c>
       <c r="T94" t="n">
         <v>0</v>
@@ -12570,7 +12570,7 @@
         </is>
       </c>
       <c r="O95" t="n">
-        <v>16875</v>
+        <v>19763.64</v>
       </c>
       <c r="P95" t="n">
         <v>85120.8</v>
@@ -12582,7 +12582,7 @@
         <v>16875</v>
       </c>
       <c r="S95" t="n">
-        <v>-9725.25</v>
+        <v>-6836.610000000001</v>
       </c>
       <c r="T95" t="n">
         <v>0</v>
@@ -12702,19 +12702,19 @@
         </is>
       </c>
       <c r="O96" t="n">
-        <v>29625.02</v>
+        <v>36024.34</v>
       </c>
       <c r="P96" t="n">
         <v>96064.8</v>
       </c>
       <c r="Q96" t="n">
-        <v>36024.3</v>
+        <v>36024.34</v>
       </c>
       <c r="R96" t="n">
         <v>29625.02</v>
       </c>
       <c r="S96" t="n">
-        <v>-6399.280000000002</v>
+        <v>0</v>
       </c>
       <c r="T96" t="n">
         <v>0</v>
@@ -12834,7 +12834,7 @@
         </is>
       </c>
       <c r="O97" t="n">
-        <v>43875</v>
+        <v>53334.58</v>
       </c>
       <c r="P97" t="n">
         <v>65664.64</v>
@@ -12846,7 +12846,7 @@
         <v>43875</v>
       </c>
       <c r="S97" t="n">
-        <v>-9477.520000000004</v>
+        <v>-17.94000000000233</v>
       </c>
       <c r="T97" t="n">
         <v>0</v>
@@ -12966,7 +12966,7 @@
         </is>
       </c>
       <c r="O98" t="n">
-        <v>121875</v>
+        <v>148201.3</v>
       </c>
       <c r="P98" t="n">
         <v>182401.6</v>
@@ -12978,7 +12978,7 @@
         <v>121875</v>
       </c>
       <c r="S98" t="n">
-        <v>-26326.29999999999</v>
+        <v>0</v>
       </c>
       <c r="T98" t="n">
         <v>0</v>
@@ -13098,7 +13098,7 @@
         </is>
       </c>
       <c r="O99" t="n">
-        <v>87500</v>
+        <v>106400.93</v>
       </c>
       <c r="P99" t="n">
         <v>121601.12</v>
@@ -13110,7 +13110,7 @@
         <v>87500</v>
       </c>
       <c r="S99" t="n">
-        <v>-18900.98</v>
+        <v>-0.04999999998835847</v>
       </c>
       <c r="T99" t="n">
         <v>0</v>
@@ -13230,7 +13230,7 @@
         </is>
       </c>
       <c r="O100" t="n">
-        <v>446250</v>
+        <v>542643.4400000001</v>
       </c>
       <c r="P100" t="n">
         <v>620165.4400000001</v>
@@ -13242,7 +13242,7 @@
         <v>446250</v>
       </c>
       <c r="S100" t="n">
-        <v>-96394.76000000001</v>
+        <v>-1.319999999948777</v>
       </c>
       <c r="T100" t="n">
         <v>0</v>
@@ -13362,19 +13362,19 @@
         </is>
       </c>
       <c r="O101" t="n">
-        <v>42500.14</v>
+        <v>51680.59</v>
       </c>
       <c r="P101" t="n">
         <v>206721.76</v>
       </c>
       <c r="Q101" t="n">
-        <v>51680.44</v>
+        <v>51680.59</v>
       </c>
       <c r="R101" t="n">
         <v>42500.14</v>
       </c>
       <c r="S101" t="n">
-        <v>-9180.300000000003</v>
+        <v>0</v>
       </c>
       <c r="T101" t="n">
         <v>0</v>
@@ -13494,7 +13494,7 @@
         </is>
       </c>
       <c r="O102" t="n">
-        <v>15500</v>
+        <v>18838.18</v>
       </c>
       <c r="P102" t="n">
         <v>75392.64</v>
@@ -13506,7 +13506,7 @@
         <v>15500</v>
       </c>
       <c r="S102" t="n">
-        <v>-3348.160000000003</v>
+        <v>-9.980000000003201</v>
       </c>
       <c r="T102" t="n">
         <v>0</v>
@@ -13626,7 +13626,7 @@
         </is>
       </c>
       <c r="O103" t="n">
-        <v>52500</v>
+        <v>63838.64</v>
       </c>
       <c r="P103" t="n">
         <v>72960.64</v>
@@ -13638,7 +13638,7 @@
         <v>52500</v>
       </c>
       <c r="S103" t="n">
-        <v>-11340.56</v>
+        <v>-1.919999999998254</v>
       </c>
       <c r="T103" t="n">
         <v>0</v>
@@ -13758,7 +13758,7 @@
         </is>
       </c>
       <c r="O104" t="n">
-        <v>60000</v>
+        <v>72959.68000000001</v>
       </c>
       <c r="P104" t="n">
         <v>77824.64</v>
@@ -13770,7 +13770,7 @@
         <v>60000</v>
       </c>
       <c r="S104" t="n">
-        <v>-12960.60000000001</v>
+        <v>-0.9199999999982538</v>
       </c>
       <c r="T104" t="n">
         <v>0</v>
@@ -13890,19 +13890,19 @@
         </is>
       </c>
       <c r="O105" t="n">
-        <v>62812.54</v>
+        <v>76380.71000000001</v>
       </c>
       <c r="P105" t="n">
         <v>81472.64</v>
       </c>
       <c r="Q105" t="n">
-        <v>76380.60000000001</v>
+        <v>76380.71000000001</v>
       </c>
       <c r="R105" t="n">
         <v>62812.54</v>
       </c>
       <c r="S105" t="n">
-        <v>-13568.06</v>
+        <v>0</v>
       </c>
       <c r="T105" t="n">
         <v>0</v>
@@ -14022,7 +14022,7 @@
         </is>
       </c>
       <c r="O106" t="n">
-        <v>31875</v>
+        <v>38758.42</v>
       </c>
       <c r="P106" t="n">
         <v>62016.48</v>
@@ -14034,7 +14034,7 @@
         <v>31875</v>
       </c>
       <c r="S106" t="n">
-        <v>-6885.300000000003</v>
+        <v>-1.880000000004657</v>
       </c>
       <c r="T106" t="n">
         <v>0</v>
@@ -14154,7 +14154,7 @@
         </is>
       </c>
       <c r="O107" t="n">
-        <v>34375</v>
+        <v>41800.35</v>
       </c>
       <c r="P107" t="n">
         <v>66880.64</v>
@@ -14166,7 +14166,7 @@
         <v>34375</v>
       </c>
       <c r="S107" t="n">
-        <v>-7425.400000000001</v>
+        <v>-0.05000000000291038</v>
       </c>
       <c r="T107" t="n">
         <v>0</v>
@@ -14286,7 +14286,7 @@
         </is>
       </c>
       <c r="O108" t="n">
-        <v>33750</v>
+        <v>41035.56</v>
       </c>
       <c r="P108" t="n">
         <v>72960.64</v>
@@ -14298,7 +14298,7 @@
         <v>33750</v>
       </c>
       <c r="S108" t="n">
-        <v>-7290.360000000001</v>
+        <v>-4.80000000000291</v>
       </c>
       <c r="T108" t="n">
         <v>0</v>
@@ -14418,7 +14418,7 @@
         </is>
       </c>
       <c r="O109" t="n">
-        <v>66562.5</v>
+        <v>80937.75999999999</v>
       </c>
       <c r="P109" t="n">
         <v>86336.8</v>
@@ -14430,7 +14430,7 @@
         <v>66562.5</v>
       </c>
       <c r="S109" t="n">
-        <v>-14378.25</v>
+        <v>-2.990000000005239</v>
       </c>
       <c r="T109" t="n">
         <v>0</v>
@@ -14550,7 +14550,7 @@
         </is>
       </c>
       <c r="O110" t="n">
-        <v>102375</v>
+        <v>124472.34</v>
       </c>
       <c r="P110" t="n">
         <v>153217.28</v>
@@ -14562,7 +14562,7 @@
         <v>102375</v>
       </c>
       <c r="S110" t="n">
-        <v>-22114.04000000001</v>
+        <v>-16.70000000001164</v>
       </c>
       <c r="T110" t="n">
         <v>0</v>
@@ -14682,19 +14682,19 @@
         </is>
       </c>
       <c r="O111" t="n">
-        <v>37188.01</v>
+        <v>45220.91</v>
       </c>
       <c r="P111" t="n">
         <v>103360.96</v>
       </c>
       <c r="Q111" t="n">
-        <v>45220.42000000001</v>
+        <v>45220.91</v>
       </c>
       <c r="R111" t="n">
         <v>37188.01</v>
       </c>
       <c r="S111" t="n">
-        <v>-8032.410000000003</v>
+        <v>0</v>
       </c>
       <c r="T111" t="n">
         <v>0</v>
@@ -14814,7 +14814,7 @@
         </is>
       </c>
       <c r="O112" t="n">
-        <v>38812.5</v>
+        <v>47189.74</v>
       </c>
       <c r="P112" t="n">
         <v>83904.8</v>
@@ -14826,7 +14826,7 @@
         <v>38812.5</v>
       </c>
       <c r="S112" t="n">
-        <v>-8383.950000000004</v>
+        <v>-6.710000000006403</v>
       </c>
       <c r="T112" t="n">
         <v>0</v>
@@ -14946,7 +14946,7 @@
         </is>
       </c>
       <c r="O113" t="n">
-        <v>56875</v>
+        <v>69158.75</v>
       </c>
       <c r="P113" t="n">
         <v>85120.8</v>
@@ -14958,7 +14958,7 @@
         <v>56875</v>
       </c>
       <c r="S113" t="n">
-        <v>-12285.64999999999</v>
+        <v>-1.899999999994179</v>
       </c>
       <c r="T113" t="n">
         <v>0</v>
@@ -15078,7 +15078,7 @@
         </is>
       </c>
       <c r="O114" t="n">
-        <v>75000</v>
+        <v>91145.60000000001</v>
       </c>
       <c r="P114" t="n">
         <v>182401.6</v>
@@ -15090,7 +15090,7 @@
         <v>75000</v>
       </c>
       <c r="S114" t="n">
-        <v>-16200.8</v>
+        <v>-55.19999999999709</v>
       </c>
       <c r="T114" t="n">
         <v>0</v>
@@ -15210,7 +15210,7 @@
         </is>
       </c>
       <c r="O115" t="n">
-        <v>71000</v>
+        <v>86254.50999999999</v>
       </c>
       <c r="P115" t="n">
         <v>172673.44</v>
@@ -15222,7 +15222,7 @@
         <v>71000</v>
       </c>
       <c r="S115" t="n">
-        <v>-15336.72</v>
+        <v>-82.2100000000064</v>
       </c>
       <c r="T115" t="n">
         <v>0</v>
@@ -15342,7 +15342,7 @@
         </is>
       </c>
       <c r="O116" t="n">
-        <v>64125</v>
+        <v>77728.54000000001</v>
       </c>
       <c r="P116" t="n">
         <v>138625.28</v>
@@ -15354,7 +15354,7 @@
         <v>64125</v>
       </c>
       <c r="S116" t="n">
-        <v>-13851.72</v>
+        <v>-248.179999999993</v>
       </c>
       <c r="T116" t="n">
         <v>0</v>
@@ -15474,7 +15474,7 @@
         </is>
       </c>
       <c r="O117" t="n">
-        <v>168000</v>
+        <v>204288.05</v>
       </c>
       <c r="P117" t="n">
         <v>233474.08</v>
@@ -15486,7 +15486,7 @@
         <v>168000</v>
       </c>
       <c r="S117" t="n">
-        <v>-50881.95000000001</v>
+        <v>-14593.89999999999</v>
       </c>
       <c r="T117" t="n">
         <v>0</v>
@@ -15606,7 +15606,7 @@
         </is>
       </c>
       <c r="O118" t="n">
-        <v>91875</v>
+        <v>111717.24</v>
       </c>
       <c r="P118" t="n">
         <v>255362.24</v>
@@ -15618,7 +15618,7 @@
         <v>91875</v>
       </c>
       <c r="S118" t="n">
-        <v>-19845.98000000001</v>
+        <v>-3.740000000005239</v>
       </c>
       <c r="T118" t="n">
         <v>0</v>
@@ -15738,19 +15738,19 @@
         </is>
       </c>
       <c r="O119" t="n">
-        <v>40625</v>
+        <v>56126.61</v>
       </c>
       <c r="P119" t="n">
         <v>79040.64</v>
       </c>
       <c r="Q119" t="n">
-        <v>49400.4</v>
+        <v>56126.61</v>
       </c>
       <c r="R119" t="n">
         <v>40625</v>
       </c>
       <c r="S119" t="n">
-        <v>-8775.400000000001</v>
+        <v>0</v>
       </c>
       <c r="T119" t="n">
         <v>5848.64</v>
@@ -15870,7 +15870,7 @@
         </is>
       </c>
       <c r="O120" t="n">
-        <v>35625</v>
+        <v>43316.57</v>
       </c>
       <c r="P120" t="n">
         <v>69312.64</v>
@@ -15882,7 +15882,7 @@
         <v>35625</v>
       </c>
       <c r="S120" t="n">
-        <v>-7695.400000000001</v>
+        <v>-3.830000000001746</v>
       </c>
       <c r="T120" t="n">
         <v>0</v>
@@ -16002,7 +16002,7 @@
         </is>
       </c>
       <c r="O121" t="n">
-        <v>28125.54</v>
+        <v>34200.8</v>
       </c>
       <c r="P121" t="n">
         <v>103360.96</v>
@@ -16014,7 +16014,7 @@
         <v>28125.54</v>
       </c>
       <c r="S121" t="n">
-        <v>-10634.82</v>
+        <v>-4559.559999999998</v>
       </c>
       <c r="T121" t="n">
         <v>0</v>
@@ -16134,19 +16134,19 @@
         </is>
       </c>
       <c r="O122" t="n">
-        <v>37500.67</v>
+        <v>45601.07</v>
       </c>
       <c r="P122" t="n">
         <v>121601.12</v>
       </c>
       <c r="Q122" t="n">
-        <v>45600.42</v>
+        <v>45601.07</v>
       </c>
       <c r="R122" t="n">
         <v>37500.67</v>
       </c>
       <c r="S122" t="n">
-        <v>-8099.75</v>
+        <v>0</v>
       </c>
       <c r="T122" t="n">
         <v>0</v>
@@ -16266,7 +16266,7 @@
         </is>
       </c>
       <c r="O123" t="n">
-        <v>43750</v>
+        <v>53190.53</v>
       </c>
       <c r="P123" t="n">
         <v>60800.48</v>
@@ -16278,7 +16278,7 @@
         <v>43750</v>
       </c>
       <c r="S123" t="n">
-        <v>-9450.420000000006</v>
+        <v>-9.890000000006694</v>
       </c>
       <c r="T123" t="n">
         <v>0</v>
@@ -16398,19 +16398,19 @@
         </is>
       </c>
       <c r="O124" t="n">
-        <v>28000.01</v>
+        <v>34048.3</v>
       </c>
       <c r="P124" t="n">
         <v>38912.32</v>
       </c>
       <c r="Q124" t="n">
-        <v>34048.28</v>
+        <v>34048.3</v>
       </c>
       <c r="R124" t="n">
         <v>28000.01</v>
       </c>
       <c r="S124" t="n">
-        <v>-6048.269999999997</v>
+        <v>0</v>
       </c>
       <c r="T124" t="n">
         <v>0</v>
@@ -16530,7 +16530,7 @@
         </is>
       </c>
       <c r="O125" t="n">
-        <v>61250</v>
+        <v>74468.75</v>
       </c>
       <c r="P125" t="n">
         <v>85120.8</v>
@@ -16542,7 +16542,7 @@
         <v>61250</v>
       </c>
       <c r="S125" t="n">
-        <v>-13230.7</v>
+        <v>-11.94999999999709</v>
       </c>
       <c r="T125" t="n">
         <v>0</v>
@@ -16662,19 +16662,19 @@
         </is>
       </c>
       <c r="O126" t="n">
-        <v>50000.02</v>
+        <v>60800.55</v>
       </c>
       <c r="P126" t="n">
         <v>97280.8</v>
       </c>
       <c r="Q126" t="n">
-        <v>60800.5</v>
+        <v>60800.55</v>
       </c>
       <c r="R126" t="n">
         <v>50000.02</v>
       </c>
       <c r="S126" t="n">
-        <v>-10800.48</v>
+        <v>0</v>
       </c>
       <c r="T126" t="n">
         <v>0</v>
@@ -16794,19 +16794,19 @@
         </is>
       </c>
       <c r="O127" t="n">
-        <v>24500.54</v>
+        <v>29792.81</v>
       </c>
       <c r="P127" t="n">
         <v>119169.12</v>
       </c>
       <c r="Q127" t="n">
-        <v>29792.28</v>
+        <v>29792.81</v>
       </c>
       <c r="R127" t="n">
         <v>24500.54</v>
       </c>
       <c r="S127" t="n">
-        <v>-5291.739999999998</v>
+        <v>0</v>
       </c>
       <c r="T127" t="n">
         <v>0</v>
@@ -16926,19 +16926,19 @@
         </is>
       </c>
       <c r="O128" t="n">
-        <v>22000.24</v>
+        <v>26752.47</v>
       </c>
       <c r="P128" t="n">
         <v>53504.48</v>
       </c>
       <c r="Q128" t="n">
-        <v>26752.24</v>
+        <v>26752.47</v>
       </c>
       <c r="R128" t="n">
         <v>22000.24</v>
       </c>
       <c r="S128" t="n">
-        <v>-4752</v>
+        <v>0</v>
       </c>
       <c r="T128" t="n">
         <v>0</v>
@@ -17058,19 +17058,19 @@
         </is>
       </c>
       <c r="O129" t="n">
-        <v>42625.2</v>
+        <v>51832.66</v>
       </c>
       <c r="P129" t="n">
         <v>75392.64</v>
       </c>
       <c r="Q129" t="n">
-        <v>51832.44</v>
+        <v>51832.66</v>
       </c>
       <c r="R129" t="n">
         <v>42625.2</v>
       </c>
       <c r="S129" t="n">
-        <v>-9207.239999999998</v>
+        <v>0</v>
       </c>
       <c r="T129" t="n">
         <v>0</v>
@@ -17190,19 +17190,19 @@
         </is>
       </c>
       <c r="O130" t="n">
-        <v>67500.29000000001</v>
+        <v>82081.00999999999</v>
       </c>
       <c r="P130" t="n">
         <v>131329.12</v>
       </c>
       <c r="Q130" t="n">
-        <v>82080.7</v>
+        <v>82081.00999999999</v>
       </c>
       <c r="R130" t="n">
         <v>67500.29000000001</v>
       </c>
       <c r="S130" t="n">
-        <v>-14580.40999999999</v>
+        <v>0</v>
       </c>
       <c r="T130" t="n">
         <v>0</v>
@@ -17322,7 +17322,7 @@
         </is>
       </c>
       <c r="O131" t="n">
-        <v>95625</v>
+        <v>116278.37</v>
       </c>
       <c r="P131" t="n">
         <v>206721.76</v>
@@ -17334,7 +17334,7 @@
         <v>95625</v>
       </c>
       <c r="S131" t="n">
-        <v>-20655.99000000001</v>
+        <v>-2.620000000009895</v>
       </c>
       <c r="T131" t="n">
         <v>0</v>
@@ -17454,19 +17454,19 @@
         </is>
       </c>
       <c r="O132" t="n">
-        <v>30500</v>
+        <v>70670.22</v>
       </c>
       <c r="P132" t="n">
         <v>148353.28</v>
       </c>
       <c r="Q132" t="n">
-        <v>37088.32000000001</v>
+        <v>70670.22</v>
       </c>
       <c r="R132" t="n">
         <v>30500</v>
       </c>
       <c r="S132" t="n">
-        <v>-6588.320000000007</v>
+        <v>0</v>
       </c>
       <c r="T132" t="n">
         <v>14737.92</v>
@@ -17586,19 +17586,19 @@
         </is>
       </c>
       <c r="O133" t="n">
-        <v>28687.53</v>
+        <v>34884.33</v>
       </c>
       <c r="P133" t="n">
         <v>62016.48</v>
       </c>
       <c r="Q133" t="n">
-        <v>34884.27</v>
+        <v>34884.33</v>
       </c>
       <c r="R133" t="n">
         <v>28687.53</v>
       </c>
       <c r="S133" t="n">
-        <v>-6196.740000000005</v>
+        <v>0</v>
       </c>
       <c r="T133" t="n">
         <v>0</v>
@@ -17718,7 +17718,7 @@
         </is>
       </c>
       <c r="O134" t="n">
-        <v>30625</v>
+        <v>37191.75</v>
       </c>
       <c r="P134" t="n">
         <v>85120.8</v>
@@ -17730,7 +17730,7 @@
         <v>30625</v>
       </c>
       <c r="S134" t="n">
-        <v>-6615.349999999999</v>
+        <v>-48.59999999999854</v>
       </c>
       <c r="T134" t="n">
         <v>0</v>
@@ -17850,7 +17850,7 @@
         </is>
       </c>
       <c r="O135" t="n">
-        <v>34875</v>
+        <v>42348.99</v>
       </c>
       <c r="P135" t="n">
         <v>113088.96</v>
@@ -17862,7 +17862,7 @@
         <v>34875</v>
       </c>
       <c r="S135" t="n">
-        <v>-7533.360000000001</v>
+        <v>-59.37000000000262</v>
       </c>
       <c r="T135" t="n">
         <v>0</v>
@@ -17982,7 +17982,7 @@
         </is>
       </c>
       <c r="O136" t="n">
-        <v>43480.18</v>
+        <v>52093.62</v>
       </c>
       <c r="P136" t="n">
         <v>70528.64</v>
@@ -17994,7 +17994,7 @@
         <v>43480.18</v>
       </c>
       <c r="S136" t="n">
-        <v>-9416.299999999996</v>
+        <v>-802.8599999999933</v>
       </c>
       <c r="T136" t="n">
         <v>0</v>
@@ -18114,7 +18114,7 @@
         </is>
       </c>
       <c r="O137" t="n">
-        <v>34478.73</v>
+        <v>41229.07</v>
       </c>
       <c r="P137" t="n">
         <v>121601.12</v>
@@ -18126,7 +18126,7 @@
         <v>34478.73</v>
       </c>
       <c r="S137" t="n">
-        <v>-11121.69</v>
+        <v>-4371.349999999999</v>
       </c>
       <c r="T137" t="n">
         <v>0</v>
@@ -18246,19 +18246,19 @@
         </is>
       </c>
       <c r="O138" t="n">
-        <v>46875.04</v>
+        <v>57000.53</v>
       </c>
       <c r="P138" t="n">
         <v>60800.48</v>
       </c>
       <c r="Q138" t="n">
-        <v>57000.45</v>
+        <v>57000.53</v>
       </c>
       <c r="R138" t="n">
         <v>46875.04</v>
       </c>
       <c r="S138" t="n">
-        <v>-10125.41</v>
+        <v>0</v>
       </c>
       <c r="T138" t="n">
         <v>0</v>
@@ -18378,7 +18378,7 @@
         </is>
       </c>
       <c r="O139" t="n">
-        <v>103687.5</v>
+        <v>126083.26</v>
       </c>
       <c r="P139" t="n">
         <v>144097.28</v>
@@ -18390,7 +18390,7 @@
         <v>103687.5</v>
       </c>
       <c r="S139" t="n">
-        <v>-22397.62</v>
+        <v>-1.85999999998603</v>
       </c>
       <c r="T139" t="n">
         <v>0</v>
@@ -18510,7 +18510,7 @@
         </is>
       </c>
       <c r="O140" t="n">
-        <v>118500</v>
+        <v>144095.69</v>
       </c>
       <c r="P140" t="n">
         <v>192129.76</v>
@@ -18522,7 +18522,7 @@
         <v>118500</v>
       </c>
       <c r="S140" t="n">
-        <v>-25597.32000000001</v>
+        <v>-1.630000000004657</v>
       </c>
       <c r="T140" t="n">
         <v>0</v>
@@ -18642,7 +18642,7 @@
         </is>
       </c>
       <c r="O141" t="n">
-        <v>42437.5</v>
+        <v>51572.03</v>
       </c>
       <c r="P141" t="n">
         <v>117952.96</v>
@@ -18654,7 +18654,7 @@
         <v>42437.5</v>
       </c>
       <c r="S141" t="n">
-        <v>-9166.919999999998</v>
+        <v>-32.38999999999942</v>
       </c>
       <c r="T141" t="n">
         <v>0</v>
@@ -18774,7 +18774,7 @@
         </is>
       </c>
       <c r="O142" t="n">
-        <v>34375</v>
+        <v>41795.53</v>
       </c>
       <c r="P142" t="n">
         <v>60800.48</v>
@@ -18786,7 +18786,7 @@
         <v>34375</v>
       </c>
       <c r="S142" t="n">
-        <v>-11225.36</v>
+        <v>-3804.830000000002</v>
       </c>
       <c r="T142" t="n">
         <v>0</v>
@@ -18906,7 +18906,7 @@
         </is>
       </c>
       <c r="O143" t="n">
-        <v>37375</v>
+        <v>45445.49</v>
       </c>
       <c r="P143" t="n">
         <v>55936.48</v>
@@ -18918,7 +18918,7 @@
         <v>37375</v>
       </c>
       <c r="S143" t="n">
-        <v>-8073.389999999999</v>
+        <v>-2.900000000001455</v>
       </c>
       <c r="T143" t="n">
         <v>0</v>
@@ -19038,19 +19038,19 @@
         </is>
       </c>
       <c r="O144" t="n">
-        <v>44625</v>
+        <v>84720.27</v>
       </c>
       <c r="P144" t="n">
         <v>144705.28</v>
       </c>
       <c r="Q144" t="n">
-        <v>54264.48</v>
+        <v>84720.27</v>
       </c>
       <c r="R144" t="n">
         <v>44625</v>
       </c>
       <c r="S144" t="n">
-        <v>-9639.479999999996</v>
+        <v>0</v>
       </c>
       <c r="T144" t="n">
         <v>7437.5</v>
@@ -19170,19 +19170,19 @@
         </is>
       </c>
       <c r="O145" t="n">
-        <v>27187.5</v>
+        <v>33060.31</v>
       </c>
       <c r="P145" t="n">
         <v>35264.32</v>
       </c>
       <c r="Q145" t="n">
-        <v>33060.3</v>
+        <v>33060.31</v>
       </c>
       <c r="R145" t="n">
         <v>27187.5</v>
       </c>
       <c r="S145" t="n">
-        <v>-5872.800000000003</v>
+        <v>0</v>
       </c>
       <c r="T145" t="n">
         <v>0</v>
@@ -19302,19 +19302,19 @@
         </is>
       </c>
       <c r="O146" t="n">
-        <v>71250.46000000001</v>
+        <v>86641.22</v>
       </c>
       <c r="P146" t="n">
         <v>138625.28</v>
       </c>
       <c r="Q146" t="n">
-        <v>86640.8</v>
+        <v>86641.22</v>
       </c>
       <c r="R146" t="n">
         <v>71250.46000000001</v>
       </c>
       <c r="S146" t="n">
-        <v>-15390.34</v>
+        <v>0</v>
       </c>
       <c r="T146" t="n">
         <v>0</v>
@@ -19434,7 +19434,7 @@
         </is>
       </c>
       <c r="O147" t="n">
-        <v>51562.73</v>
+        <v>62700.8</v>
       </c>
       <c r="P147" t="n">
         <v>91200.8</v>
@@ -19446,7 +19446,7 @@
         <v>51562.73</v>
       </c>
       <c r="S147" t="n">
-        <v>-16837.87</v>
+        <v>-5699.800000000003</v>
       </c>
       <c r="T147" t="n">
         <v>0</v>
@@ -19566,7 +19566,7 @@
         </is>
       </c>
       <c r="O148" t="n">
-        <v>56000</v>
+        <v>68096.60000000001</v>
       </c>
       <c r="P148" t="n">
         <v>68096.64</v>
@@ -19578,7 +19578,7 @@
         <v>56000</v>
       </c>
       <c r="S148" t="n">
-        <v>-12096.64</v>
+        <v>-0.03999999999359716</v>
       </c>
       <c r="T148" t="n">
         <v>0</v>
@@ -19698,7 +19698,7 @@
         </is>
       </c>
       <c r="O149" t="n">
-        <v>103125</v>
+        <v>124983.09</v>
       </c>
       <c r="P149" t="n">
         <v>133761.12</v>
@@ -19710,7 +19710,7 @@
         <v>103125</v>
       </c>
       <c r="S149" t="n">
-        <v>-22276.04999999999</v>
+        <v>-417.9599999999919</v>
       </c>
       <c r="T149" t="n">
         <v>0</v>
@@ -19830,7 +19830,7 @@
         </is>
       </c>
       <c r="O150" t="n">
-        <v>70312.5</v>
+        <v>85494.8</v>
       </c>
       <c r="P150" t="n">
         <v>91200.8</v>
@@ -19842,7 +19842,7 @@
         <v>70312.5</v>
       </c>
       <c r="S150" t="n">
-        <v>-15188.25</v>
+        <v>-5.94999999999709</v>
       </c>
       <c r="T150" t="n">
         <v>0</v>
@@ -19962,19 +19962,19 @@
         </is>
       </c>
       <c r="O151" t="n">
-        <v>66562.57000000001</v>
+        <v>80940.75999999999</v>
       </c>
       <c r="P151" t="n">
         <v>86336.8</v>
       </c>
       <c r="Q151" t="n">
-        <v>80940.75</v>
+        <v>80940.75999999999</v>
       </c>
       <c r="R151" t="n">
         <v>66562.57000000001</v>
       </c>
       <c r="S151" t="n">
-        <v>-14378.17999999999</v>
+        <v>0</v>
       </c>
       <c r="T151" t="n">
         <v>0</v>
@@ -20094,19 +20094,19 @@
         </is>
       </c>
       <c r="O152" t="n">
-        <v>15937.55</v>
+        <v>19380.21</v>
       </c>
       <c r="P152" t="n">
         <v>62016.48</v>
       </c>
       <c r="Q152" t="n">
-        <v>19380.15</v>
+        <v>19380.21</v>
       </c>
       <c r="R152" t="n">
         <v>15937.55</v>
       </c>
       <c r="S152" t="n">
-        <v>-3442.6</v>
+        <v>0</v>
       </c>
       <c r="T152" t="n">
         <v>0</v>
@@ -20226,19 +20226,19 @@
         </is>
       </c>
       <c r="O153" t="n">
-        <v>15939.33</v>
+        <v>19412.72</v>
       </c>
       <c r="P153" t="n">
         <v>62114.88</v>
       </c>
       <c r="Q153" t="n">
-        <v>19410.9</v>
+        <v>19412.72</v>
       </c>
       <c r="R153" t="n">
         <v>15939.33</v>
       </c>
       <c r="S153" t="n">
-        <v>-3471.570000000002</v>
+        <v>0</v>
       </c>
       <c r="T153" t="n">
         <v>0</v>
@@ -20358,7 +20358,7 @@
         </is>
       </c>
       <c r="O154" t="n">
-        <v>63750</v>
+        <v>77511.09</v>
       </c>
       <c r="P154" t="n">
         <v>124033.12</v>
@@ -20370,7 +20370,7 @@
         <v>63750</v>
       </c>
       <c r="S154" t="n">
-        <v>-13770.7</v>
+        <v>-9.610000000000582</v>
       </c>
       <c r="T154" t="n">
         <v>0</v>
@@ -20490,7 +20490,7 @@
         </is>
       </c>
       <c r="O155" t="n">
-        <v>28695.74</v>
+        <v>34892.54</v>
       </c>
       <c r="P155" t="n">
         <v>62016.48</v>
@@ -20502,7 +20502,7 @@
         <v>28695.74</v>
       </c>
       <c r="S155" t="n">
-        <v>-10064.56</v>
+        <v>-3867.760000000002</v>
       </c>
       <c r="T155" t="n">
         <v>0</v>
@@ -20622,7 +20622,7 @@
         </is>
       </c>
       <c r="O156" t="n">
-        <v>112500.02</v>
+        <v>136801.2</v>
       </c>
       <c r="P156" t="n">
         <v>182401.6</v>
@@ -20634,7 +20634,7 @@
         <v>112500.02</v>
       </c>
       <c r="S156" t="n">
-        <v>-24301.18000000001</v>
+        <v>0</v>
       </c>
       <c r="T156" t="n">
         <v>0</v>
@@ -20754,19 +20754,19 @@
         </is>
       </c>
       <c r="O157" t="n">
-        <v>39000.12</v>
+        <v>47424.52</v>
       </c>
       <c r="P157" t="n">
         <v>63232.48</v>
       </c>
       <c r="Q157" t="n">
-        <v>47424.36</v>
+        <v>47424.52</v>
       </c>
       <c r="R157" t="n">
         <v>39000.12</v>
       </c>
       <c r="S157" t="n">
-        <v>-8424.239999999998</v>
+        <v>0</v>
       </c>
       <c r="T157" t="n">
         <v>0</v>
@@ -20886,7 +20886,7 @@
         </is>
       </c>
       <c r="O158" t="n">
-        <v>150000</v>
+        <v>182401.6</v>
       </c>
       <c r="P158" t="n">
         <v>182401.6</v>
@@ -20898,7 +20898,7 @@
         <v>150000</v>
       </c>
       <c r="S158" t="n">
-        <v>-32401.60000000001</v>
+        <v>0</v>
       </c>
       <c r="T158" t="n">
         <v>0</v>
@@ -21018,7 +21018,7 @@
         </is>
       </c>
       <c r="O159" t="n">
-        <v>60000</v>
+        <v>72956.04000000001</v>
       </c>
       <c r="P159" t="n">
         <v>145921.28</v>
@@ -21030,7 +21030,7 @@
         <v>60000</v>
       </c>
       <c r="S159" t="n">
-        <v>-12960.64</v>
+        <v>-4.599999999991269</v>
       </c>
       <c r="T159" t="n">
         <v>0</v>
@@ -21150,19 +21150,19 @@
         </is>
       </c>
       <c r="O160" t="n">
-        <v>77500.00999999999</v>
+        <v>94240.85000000001</v>
       </c>
       <c r="P160" t="n">
         <v>188481.6</v>
       </c>
       <c r="Q160" t="n">
-        <v>94240.8</v>
+        <v>94240.85000000001</v>
       </c>
       <c r="R160" t="n">
         <v>77500.00999999999</v>
       </c>
       <c r="S160" t="n">
-        <v>-16740.79000000001</v>
+        <v>0</v>
       </c>
       <c r="T160" t="n">
         <v>0</v>
@@ -21282,7 +21282,7 @@
         </is>
       </c>
       <c r="O161" t="n">
-        <v>53437.5</v>
+        <v>64979.61</v>
       </c>
       <c r="P161" t="n">
         <v>69312.64</v>
@@ -21294,7 +21294,7 @@
         <v>53437.5</v>
       </c>
       <c r="S161" t="n">
-        <v>-11543.1</v>
+        <v>-0.9899999999979627</v>
       </c>
       <c r="T161" t="n">
         <v>0</v>
@@ -21414,7 +21414,7 @@
         </is>
       </c>
       <c r="O162" t="n">
-        <v>86937.5</v>
+        <v>105705.14</v>
       </c>
       <c r="P162" t="n">
         <v>130113.12</v>
@@ -21426,7 +21426,7 @@
         <v>86937.5</v>
       </c>
       <c r="S162" t="n">
-        <v>-18779.41</v>
+        <v>-11.77000000000407</v>
       </c>
       <c r="T162" t="n">
         <v>0</v>
@@ -21546,7 +21546,7 @@
         </is>
       </c>
       <c r="O163" t="n">
-        <v>49875</v>
+        <v>60648.5</v>
       </c>
       <c r="P163" t="n">
         <v>138625.28</v>
@@ -21558,7 +21558,7 @@
         <v>49875</v>
       </c>
       <c r="S163" t="n">
-        <v>-10773.56</v>
+        <v>-0.05999999999767169</v>
       </c>
       <c r="T163" t="n">
         <v>0</v>
@@ -21678,7 +21678,7 @@
         </is>
       </c>
       <c r="O164" t="n">
-        <v>37187.5</v>
+        <v>45175.91</v>
       </c>
       <c r="P164" t="n">
         <v>103360.96</v>
@@ -21690,7 +21690,7 @@
         <v>37187.5</v>
       </c>
       <c r="S164" t="n">
-        <v>-8032.920000000006</v>
+        <v>-44.51000000000204</v>
       </c>
       <c r="T164" t="n">
         <v>0</v>
@@ -21810,7 +21810,7 @@
         </is>
       </c>
       <c r="O165" t="n">
-        <v>50750</v>
+        <v>61710.62</v>
       </c>
       <c r="P165" t="n">
         <v>70528.64</v>
@@ -21822,7 +21822,7 @@
         <v>50750</v>
       </c>
       <c r="S165" t="n">
-        <v>-10962.56</v>
+        <v>-1.939999999995052</v>
       </c>
       <c r="T165" t="n">
         <v>0</v>
@@ -21942,19 +21942,19 @@
         </is>
       </c>
       <c r="O166" t="n">
-        <v>34125.1</v>
+        <v>41496.45</v>
       </c>
       <c r="P166" t="n">
         <v>51072.48</v>
       </c>
       <c r="Q166" t="n">
-        <v>41496.39</v>
+        <v>41496.45</v>
       </c>
       <c r="R166" t="n">
         <v>34125.1</v>
       </c>
       <c r="S166" t="n">
-        <v>-7371.290000000001</v>
+        <v>0</v>
       </c>
       <c r="T166" t="n">
         <v>0</v>
@@ -22074,7 +22074,7 @@
         </is>
       </c>
       <c r="O167" t="n">
-        <v>49875</v>
+        <v>60646.61</v>
       </c>
       <c r="P167" t="n">
         <v>69312.64</v>
@@ -22086,7 +22086,7 @@
         <v>49875</v>
       </c>
       <c r="S167" t="n">
-        <v>-10773.56</v>
+        <v>-1.94999999999709</v>
       </c>
       <c r="T167" t="n">
         <v>0</v>
@@ -22206,7 +22206,7 @@
         </is>
       </c>
       <c r="O168" t="n">
-        <v>46062.5</v>
+        <v>55987.71</v>
       </c>
       <c r="P168" t="n">
         <v>81472.64</v>
@@ -22218,7 +22218,7 @@
         <v>46062.5</v>
       </c>
       <c r="S168" t="n">
-        <v>-9949.940000000002</v>
+        <v>-24.7300000000032</v>
       </c>
       <c r="T168" t="n">
         <v>0</v>
@@ -22338,7 +22338,7 @@
         </is>
       </c>
       <c r="O169" t="n">
-        <v>48125</v>
+        <v>58493.75</v>
       </c>
       <c r="P169" t="n">
         <v>85120.8</v>
@@ -22350,7 +22350,7 @@
         <v>48125</v>
       </c>
       <c r="S169" t="n">
-        <v>-10395.55</v>
+        <v>-26.80000000000291</v>
       </c>
       <c r="T169" t="n">
         <v>0</v>
@@ -22470,19 +22470,19 @@
         </is>
       </c>
       <c r="O170" t="n">
-        <v>34501.36</v>
+        <v>41953.72</v>
       </c>
       <c r="P170" t="n">
         <v>223745.92</v>
       </c>
       <c r="Q170" t="n">
-        <v>41952.36000000002</v>
+        <v>41953.72</v>
       </c>
       <c r="R170" t="n">
         <v>34501.36</v>
       </c>
       <c r="S170" t="n">
-        <v>-7451.000000000015</v>
+        <v>0</v>
       </c>
       <c r="T170" t="n">
         <v>0</v>
@@ -22602,7 +22602,7 @@
         </is>
       </c>
       <c r="O171" t="n">
-        <v>22000</v>
+        <v>26752.23</v>
       </c>
       <c r="P171" t="n">
         <v>53504.48</v>
@@ -22614,7 +22614,7 @@
         <v>22000</v>
       </c>
       <c r="S171" t="n">
-        <v>-4752.240000000002</v>
+        <v>-0.01000000000203727</v>
       </c>
       <c r="T171" t="n">
         <v>0</v>
@@ -22734,19 +22734,19 @@
         </is>
       </c>
       <c r="O172" t="n">
-        <v>52500.93</v>
+        <v>63841.49</v>
       </c>
       <c r="P172" t="n">
         <v>170241.44</v>
       </c>
       <c r="Q172" t="n">
-        <v>63840.54000000001</v>
+        <v>63841.49</v>
       </c>
       <c r="R172" t="n">
         <v>52500.93</v>
       </c>
       <c r="S172" t="n">
-        <v>-11339.61000000001</v>
+        <v>0</v>
       </c>
       <c r="T172" t="n">
         <v>0</v>
@@ -22866,7 +22866,7 @@
         </is>
       </c>
       <c r="O173" t="n">
-        <v>21375</v>
+        <v>25992.21</v>
       </c>
       <c r="P173" t="n">
         <v>69312.64</v>
@@ -22878,7 +22878,7 @@
         <v>21375</v>
       </c>
       <c r="S173" t="n">
-        <v>-4617.239999999998</v>
+        <v>-0.02999999999883585</v>
       </c>
       <c r="T173" t="n">
         <v>0</v>
@@ -22998,19 +22998,19 @@
         </is>
       </c>
       <c r="O174" t="n">
-        <v>60125.15</v>
+        <v>73112.79000000001</v>
       </c>
       <c r="P174" t="n">
         <v>89984.8</v>
       </c>
       <c r="Q174" t="n">
-        <v>73112.64999999999</v>
+        <v>73112.79000000001</v>
       </c>
       <c r="R174" t="n">
         <v>60125.15</v>
       </c>
       <c r="S174" t="n">
-        <v>-12987.49999999999</v>
+        <v>0</v>
       </c>
       <c r="T174" t="n">
         <v>0</v>
@@ -23130,7 +23130,7 @@
         </is>
       </c>
       <c r="O175" t="n">
-        <v>42250</v>
+        <v>51365.55</v>
       </c>
       <c r="P175" t="n">
         <v>63232.48</v>
@@ -23142,7 +23142,7 @@
         <v>42250</v>
       </c>
       <c r="S175" t="n">
-        <v>-13078.42000000001</v>
+        <v>-3962.870000000003</v>
       </c>
       <c r="T175" t="n">
         <v>0</v>
@@ -23262,7 +23262,7 @@
         </is>
       </c>
       <c r="O176" t="n">
-        <v>73562.5</v>
+        <v>89428.14</v>
       </c>
       <c r="P176" t="n">
         <v>130113.12</v>
@@ -23274,7 +23274,7 @@
         <v>73562.5</v>
       </c>
       <c r="S176" t="n">
-        <v>-15890.27</v>
+        <v>-24.63000000000466</v>
       </c>
       <c r="T176" t="n">
         <v>0</v>
@@ -23394,19 +23394,19 @@
         </is>
       </c>
       <c r="O177" t="n">
-        <v>50500.55</v>
+        <v>61409.08</v>
       </c>
       <c r="P177" t="n">
         <v>122817.12</v>
       </c>
       <c r="Q177" t="n">
-        <v>61408.56</v>
+        <v>61409.08</v>
       </c>
       <c r="R177" t="n">
         <v>50500.55</v>
       </c>
       <c r="S177" t="n">
-        <v>-10908.00999999999</v>
+        <v>0</v>
       </c>
       <c r="T177" t="n">
         <v>0</v>
@@ -23526,19 +23526,19 @@
         </is>
       </c>
       <c r="O178" t="n">
-        <v>82500.06</v>
+        <v>100320.94</v>
       </c>
       <c r="P178" t="n">
         <v>107008.96</v>
       </c>
       <c r="Q178" t="n">
-        <v>100320.9</v>
+        <v>100320.94</v>
       </c>
       <c r="R178" t="n">
         <v>82500.06</v>
       </c>
       <c r="S178" t="n">
-        <v>-17820.84000000001</v>
+        <v>0</v>
       </c>
       <c r="T178" t="n">
         <v>0</v>
@@ -23658,7 +23658,7 @@
         </is>
       </c>
       <c r="O179" t="n">
-        <v>47812.5</v>
+        <v>58136.54</v>
       </c>
       <c r="P179" t="n">
         <v>62016.48</v>
@@ -23670,7 +23670,7 @@
         <v>47812.5</v>
       </c>
       <c r="S179" t="n">
-        <v>-10327.95</v>
+        <v>-3.910000000003492</v>
       </c>
       <c r="T179" t="n">
         <v>0</v>
@@ -23790,7 +23790,7 @@
         </is>
       </c>
       <c r="O180" t="n">
-        <v>55312.5</v>
+        <v>67259.63</v>
       </c>
       <c r="P180" t="n">
         <v>71744.64</v>
@@ -23802,7 +23802,7 @@
         <v>55312.5</v>
       </c>
       <c r="S180" t="n">
-        <v>-11948.10000000001</v>
+        <v>-0.9700000000011642</v>
       </c>
       <c r="T180" t="n">
         <v>0</v>
@@ -23922,7 +23922,7 @@
         </is>
       </c>
       <c r="O181" t="n">
-        <v>26875</v>
+        <v>32679.46</v>
       </c>
       <c r="P181" t="n">
         <v>52288.48</v>
@@ -23934,7 +23934,7 @@
         <v>26875</v>
       </c>
       <c r="S181" t="n">
-        <v>-5805.300000000003</v>
+        <v>-0.8400000000037835</v>
       </c>
       <c r="T181" t="n">
         <v>0</v>
@@ -24054,7 +24054,7 @@
         </is>
       </c>
       <c r="O182" t="n">
-        <v>56250</v>
+        <v>68400.60000000001</v>
       </c>
       <c r="P182" t="n">
         <v>218881.92</v>
@@ -24066,7 +24066,7 @@
         <v>56250</v>
       </c>
       <c r="S182" t="n">
-        <v>-12150.60000000001</v>
+        <v>0</v>
       </c>
       <c r="T182" t="n">
         <v>0</v>
@@ -24186,19 +24186,19 @@
         </is>
       </c>
       <c r="O183" t="n">
-        <v>93000</v>
+        <v>113088.99</v>
       </c>
       <c r="P183" t="n">
         <v>113088.96</v>
       </c>
       <c r="Q183" t="n">
-        <v>113088.96</v>
+        <v>113088.99</v>
       </c>
       <c r="R183" t="n">
         <v>93000</v>
       </c>
       <c r="S183" t="n">
-        <v>-20088.96000000001</v>
+        <v>0</v>
       </c>
       <c r="T183" t="n">
         <v>0</v>
@@ -24318,7 +24318,7 @@
         </is>
       </c>
       <c r="O184" t="n">
-        <v>15000</v>
+        <v>18237.6</v>
       </c>
       <c r="P184" t="n">
         <v>72960.64</v>
@@ -24330,7 +24330,7 @@
         <v>15000</v>
       </c>
       <c r="S184" t="n">
-        <v>-3240.160000000003</v>
+        <v>-2.56000000000131</v>
       </c>
       <c r="T184" t="n">
         <v>0</v>
@@ -24450,19 +24450,19 @@
         </is>
       </c>
       <c r="O185" t="n">
-        <v>75000</v>
+        <v>101980</v>
       </c>
       <c r="P185" t="n">
         <v>102400</v>
       </c>
       <c r="Q185" t="n">
-        <v>96000</v>
+        <v>101980</v>
       </c>
       <c r="R185" t="n">
         <v>75000</v>
       </c>
       <c r="S185" t="n">
-        <v>-21000</v>
+        <v>0</v>
       </c>
       <c r="T185" t="n">
         <v>5000</v>
@@ -24582,7 +24582,7 @@
         </is>
       </c>
       <c r="O186" t="n">
-        <v>220500</v>
+        <v>268128.69</v>
       </c>
       <c r="P186" t="n">
         <v>306434.72</v>
@@ -24594,7 +24594,7 @@
         <v>220500</v>
       </c>
       <c r="S186" t="n">
-        <v>-47630.38</v>
+        <v>-1.690000000002328</v>
       </c>
       <c r="T186" t="n">
         <v>0</v>
@@ -24714,19 +24714,19 @@
         </is>
       </c>
       <c r="O187" t="n">
-        <v>54562.96</v>
+        <v>66349.03</v>
       </c>
       <c r="P187" t="n">
         <v>117952.96</v>
       </c>
       <c r="Q187" t="n">
-        <v>66348.54000000001</v>
+        <v>66349.03</v>
       </c>
       <c r="R187" t="n">
         <v>54562.96</v>
       </c>
       <c r="S187" t="n">
-        <v>-11785.58000000001</v>
+        <v>0</v>
       </c>
       <c r="T187" t="n">
         <v>0</v>
@@ -24846,7 +24846,7 @@
         </is>
       </c>
       <c r="O188" t="n">
-        <v>47125</v>
+        <v>57304.47</v>
       </c>
       <c r="P188" t="n">
         <v>70528.64</v>
@@ -24858,7 +24858,7 @@
         <v>47125</v>
       </c>
       <c r="S188" t="n">
-        <v>-10179.52</v>
+        <v>-0.05000000000291038</v>
       </c>
       <c r="T188" t="n">
         <v>0</v>
@@ -24978,19 +24978,19 @@
         </is>
       </c>
       <c r="O189" t="n">
-        <v>108875.18</v>
+        <v>132393.34</v>
       </c>
       <c r="P189" t="n">
         <v>162945.44</v>
       </c>
       <c r="Q189" t="n">
-        <v>132393.17</v>
+        <v>132393.34</v>
       </c>
       <c r="R189" t="n">
         <v>108875.18</v>
       </c>
       <c r="S189" t="n">
-        <v>-23517.99000000001</v>
+        <v>0</v>
       </c>
       <c r="T189" t="n">
         <v>0</v>
@@ -25110,7 +25110,7 @@
         </is>
       </c>
       <c r="O190" t="n">
-        <v>93437.5</v>
+        <v>113618.23</v>
       </c>
       <c r="P190" t="n">
         <v>139841.28</v>
@@ -25122,7 +25122,7 @@
         <v>93437.5</v>
       </c>
       <c r="S190" t="n">
-        <v>-20183.54000000001</v>
+        <v>-2.810000000012224</v>
       </c>
       <c r="T190" t="n">
         <v>0</v>
@@ -25242,7 +25242,7 @@
         </is>
       </c>
       <c r="O191" t="n">
-        <v>45500</v>
+        <v>55320.56</v>
       </c>
       <c r="P191" t="n">
         <v>68096.64</v>
@@ -25254,7 +25254,7 @@
         <v>45500</v>
       </c>
       <c r="S191" t="n">
-        <v>-9828.520000000004</v>
+        <v>-7.960000000006403</v>
       </c>
       <c r="T191" t="n">
         <v>0</v>
@@ -25374,7 +25374,7 @@
         </is>
       </c>
       <c r="O192" t="n">
-        <v>124250</v>
+        <v>151083.42</v>
       </c>
       <c r="P192" t="n">
         <v>172673.44</v>
@@ -25386,7 +25386,7 @@
         <v>124250</v>
       </c>
       <c r="S192" t="n">
-        <v>-26839.26000000001</v>
+        <v>-5.839999999996508</v>
       </c>
       <c r="T192" t="n">
         <v>0</v>
@@ -25506,7 +25506,7 @@
         </is>
       </c>
       <c r="O193" t="n">
-        <v>120750</v>
+        <v>146831.47</v>
       </c>
       <c r="P193" t="n">
         <v>167809.44</v>
@@ -25518,7 +25518,7 @@
         <v>120750</v>
       </c>
       <c r="S193" t="n">
-        <v>-36571.35000000001</v>
+        <v>-10489.88</v>
       </c>
       <c r="T193" t="n">
         <v>0</v>
@@ -25638,19 +25638,19 @@
         </is>
       </c>
       <c r="O194" t="n">
-        <v>34375</v>
+        <v>45978.59</v>
       </c>
       <c r="P194" t="n">
         <v>66880.64</v>
       </c>
       <c r="Q194" t="n">
-        <v>41800.4</v>
+        <v>45978.59</v>
       </c>
       <c r="R194" t="n">
         <v>34375</v>
       </c>
       <c r="S194" t="n">
-        <v>-7425.400000000001</v>
+        <v>0</v>
       </c>
       <c r="T194" t="n">
         <v>3437.5</v>
@@ -25770,7 +25770,7 @@
         </is>
       </c>
       <c r="O195" t="n">
-        <v>15000</v>
+        <v>18239.93</v>
       </c>
       <c r="P195" t="n">
         <v>48640.48</v>
@@ -25782,7 +25782,7 @@
         <v>15000</v>
       </c>
       <c r="S195" t="n">
-        <v>-3240.18</v>
+        <v>-0.25</v>
       </c>
       <c r="T195" t="n">
         <v>0</v>
@@ -25902,7 +25902,7 @@
         </is>
       </c>
       <c r="O196" t="n">
-        <v>74937.5</v>
+        <v>91079.16</v>
       </c>
       <c r="P196" t="n">
         <v>132545.12</v>
@@ -25914,7 +25914,7 @@
         <v>74937.5</v>
       </c>
       <c r="S196" t="n">
-        <v>-16187.26999999999</v>
+        <v>-45.60999999998603</v>
       </c>
       <c r="T196" t="n">
         <v>0</v>
@@ -26034,7 +26034,7 @@
         </is>
       </c>
       <c r="O197" t="n">
-        <v>59500</v>
+        <v>72350.73</v>
       </c>
       <c r="P197" t="n">
         <v>82688.8</v>
@@ -26046,7 +26046,7 @@
         <v>59500</v>
       </c>
       <c r="S197" t="n">
-        <v>-12852.7</v>
+        <v>-1.970000000001164</v>
       </c>
       <c r="T197" t="n">
         <v>0</v>
@@ -26166,7 +26166,7 @@
         </is>
       </c>
       <c r="O198" t="n">
-        <v>103125</v>
+        <v>125351.6</v>
       </c>
       <c r="P198" t="n">
         <v>182401.6</v>
@@ -26178,7 +26178,7 @@
         <v>103125</v>
       </c>
       <c r="S198" t="n">
-        <v>-33676.20000000001</v>
+        <v>-11449.60000000001</v>
       </c>
       <c r="T198" t="n">
         <v>0</v>
@@ -26293,7 +26293,7 @@
         </is>
       </c>
       <c r="O199" t="n">
-        <v>81250</v>
+        <v>98800.85000000001</v>
       </c>
       <c r="P199" t="n">
         <v>158081.44</v>
@@ -26305,7 +26305,7 @@
         <v>81250</v>
       </c>
       <c r="S199" t="n">
-        <v>-17550.89999999999</v>
+        <v>-0.04999999998835847</v>
       </c>
       <c r="T199" t="n">
         <v>0</v>
@@ -26425,19 +26425,19 @@
         </is>
       </c>
       <c r="O200" t="n">
-        <v>49000</v>
+        <v>59584.52</v>
       </c>
       <c r="P200" t="n">
         <v>59584.48</v>
       </c>
       <c r="Q200" t="n">
-        <v>59584.48</v>
+        <v>59584.52</v>
       </c>
       <c r="R200" t="n">
         <v>49000</v>
       </c>
       <c r="S200" t="n">
-        <v>-10584.48</v>
+        <v>0</v>
       </c>
       <c r="T200" t="n">
         <v>0</v>
@@ -26557,7 +26557,7 @@
         </is>
       </c>
       <c r="O201" t="n">
-        <v>32187.5</v>
+        <v>39053.96</v>
       </c>
       <c r="P201" t="n">
         <v>125249.12</v>
@@ -26569,7 +26569,7 @@
         <v>32187.5</v>
       </c>
       <c r="S201" t="n">
-        <v>-6952.850000000006</v>
+        <v>-86.39000000000669</v>
       </c>
       <c r="T201" t="n">
         <v>0</v>
@@ -26689,7 +26689,7 @@
         </is>
       </c>
       <c r="O202" t="n">
-        <v>126562.5</v>
+        <v>153900.44</v>
       </c>
       <c r="P202" t="n">
         <v>164161.44</v>
@@ -26701,7 +26701,7 @@
         <v>126562.5</v>
       </c>
       <c r="S202" t="n">
-        <v>-27338.85000000001</v>
+        <v>-0.9100000000034925</v>
       </c>
       <c r="T202" t="n">
         <v>0</v>
@@ -26821,19 +26821,19 @@
         </is>
       </c>
       <c r="O203" t="n">
-        <v>70000.44</v>
+        <v>85121.19</v>
       </c>
       <c r="P203" t="n">
         <v>136193.12</v>
       </c>
       <c r="Q203" t="n">
-        <v>85120.7</v>
+        <v>85121.19</v>
       </c>
       <c r="R203" t="n">
         <v>70000.44</v>
       </c>
       <c r="S203" t="n">
-        <v>-15120.25999999999</v>
+        <v>0</v>
       </c>
       <c r="T203" t="n">
         <v>0</v>
@@ -26953,19 +26953,19 @@
         </is>
       </c>
       <c r="O204" t="n">
-        <v>56250.48</v>
+        <v>68401.07000000001</v>
       </c>
       <c r="P204" t="n">
         <v>121601.12</v>
       </c>
       <c r="Q204" t="n">
-        <v>68400.63</v>
+        <v>68401.07000000001</v>
       </c>
       <c r="R204" t="n">
         <v>56250.48</v>
       </c>
       <c r="S204" t="n">
-        <v>-12150.15</v>
+        <v>0</v>
       </c>
       <c r="T204" t="n">
         <v>0</v>
@@ -27085,7 +27085,7 @@
         </is>
       </c>
       <c r="O205" t="n">
-        <v>55250</v>
+        <v>67169.73</v>
       </c>
       <c r="P205" t="n">
         <v>82688.8</v>
@@ -27097,7 +27097,7 @@
         <v>55250</v>
       </c>
       <c r="S205" t="n">
-        <v>-11934.64999999999</v>
+        <v>-14.91999999999825</v>
       </c>
       <c r="T205" t="n">
         <v>0</v>
@@ -27212,7 +27212,7 @@
         </is>
       </c>
       <c r="O206" t="n">
-        <v>31875</v>
+        <v>38690.91</v>
       </c>
       <c r="P206" t="n">
         <v>103360.96</v>
@@ -27224,7 +27224,7 @@
         <v>31875</v>
       </c>
       <c r="S206" t="n">
-        <v>-6885.360000000001</v>
+        <v>-69.44999999999709</v>
       </c>
       <c r="T206" t="n">
         <v>0</v>
@@ -27344,7 +27344,7 @@
         </is>
       </c>
       <c r="O207" t="n">
-        <v>63250</v>
+        <v>76887.98</v>
       </c>
       <c r="P207" t="n">
         <v>111872.96</v>
@@ -27356,7 +27356,7 @@
         <v>63250</v>
       </c>
       <c r="S207" t="n">
-        <v>-13662.66</v>
+        <v>-24.68000000000757</v>
       </c>
       <c r="T207" t="n">
         <v>0</v>
@@ -27476,7 +27476,7 @@
         </is>
       </c>
       <c r="O208" t="n">
-        <v>56250</v>
+        <v>68391.60000000001</v>
       </c>
       <c r="P208" t="n">
         <v>182401.6</v>
@@ -27488,7 +27488,7 @@
         <v>56250</v>
       </c>
       <c r="S208" t="n">
-        <v>-12150.60000000001</v>
+        <v>-9</v>
       </c>
       <c r="T208" t="n">
         <v>0</v>
@@ -27603,7 +27603,7 @@
         </is>
       </c>
       <c r="O209" t="n">
-        <v>234375</v>
+        <v>285002.47</v>
       </c>
       <c r="P209" t="n">
         <v>760006.72</v>
@@ -27615,7 +27615,7 @@
         <v>234375</v>
       </c>
       <c r="S209" t="n">
-        <v>-50627.52000000002</v>
+        <v>-0.04999999998835847</v>
       </c>
       <c r="T209" t="n">
         <v>0</v>
@@ -27735,7 +27735,7 @@
         </is>
       </c>
       <c r="O210" t="n">
-        <v>19500</v>
+        <v>23701.42</v>
       </c>
       <c r="P210" t="n">
         <v>47424.48</v>
@@ -27747,7 +27747,7 @@
         <v>19500</v>
       </c>
       <c r="S210" t="n">
-        <v>-4212.240000000002</v>
+        <v>-10.81999999999971</v>
       </c>
       <c r="T210" t="n">
         <v>0</v>
@@ -27867,7 +27867,7 @@
         </is>
       </c>
       <c r="O211" t="n">
-        <v>125937.5</v>
+        <v>153120.65</v>
       </c>
       <c r="P211" t="n">
         <v>188481.6</v>
@@ -27879,7 +27879,7 @@
         <v>125937.5</v>
       </c>
       <c r="S211" t="n">
-        <v>-27203.79999999999</v>
+        <v>-20.64999999999418</v>
       </c>
       <c r="T211" t="n">
         <v>0</v>
@@ -27999,19 +27999,19 @@
         </is>
       </c>
       <c r="O212" t="n">
-        <v>40500.16</v>
+        <v>49248.58</v>
       </c>
       <c r="P212" t="n">
         <v>65664.64</v>
       </c>
       <c r="Q212" t="n">
-        <v>49248.48</v>
+        <v>49248.58</v>
       </c>
       <c r="R212" t="n">
         <v>40500.16</v>
       </c>
       <c r="S212" t="n">
-        <v>-8748.319999999992</v>
+        <v>0</v>
       </c>
       <c r="T212" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Add: changing format to output
</commit_message>
<xml_diff>
--- a/output_automatizado.xlsx
+++ b/output_automatizado.xlsx
@@ -628,7 +628,8 @@
   <dimension ref="A2:AJ215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -28181,6 +28182,11 @@
       <c r="AH213" t="n">
         <v>0</v>
       </c>
+      <c r="AI213" t="inlineStr">
+        <is>
+          <t>Vigente</t>
+        </is>
+      </c>
       <c r="AJ213" t="inlineStr">
         <is>
           <t>000000102</t>
@@ -28293,6 +28299,11 @@
       </c>
       <c r="AH214" t="n">
         <v>0</v>
+      </c>
+      <c r="AI214" t="inlineStr">
+        <is>
+          <t>Vigente</t>
+        </is>
       </c>
       <c r="AJ214" t="inlineStr">
         <is>
@@ -28380,7 +28391,8 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add: Adding filter func to the output
</commit_message>
<xml_diff>
--- a/output_automatizado.xlsx
+++ b/output_automatizado.xlsx
@@ -10,7 +10,10 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cartera" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mora" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cartera'!$A$6:$AJ$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Mora'!$A$6:$N$6</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -28375,6 +28378,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A6:AJ6"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -28898,6 +28902,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A6:N6"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Add: fellback to exception in cantidad_prestada = NULL, using inplace cantidad_entregada
</commit_message>
<xml_diff>
--- a/output_automatizado.xlsx
+++ b/output_automatizado.xlsx
@@ -28097,6 +28097,9 @@
       <c r="E213" t="n">
         <v>2</v>
       </c>
+      <c r="F213" t="n">
+        <v>365172</v>
+      </c>
       <c r="G213" t="inlineStr">
         <is>
           <t>MIGRADO</t>
@@ -28219,6 +28222,9 @@
       </c>
       <c r="E214" t="n">
         <v>1</v>
+      </c>
+      <c r="F214" t="n">
+        <v>191790</v>
       </c>
       <c r="G214" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add: updating all calculus
</commit_message>
<xml_diff>
--- a/output_automatizado.xlsx
+++ b/output_automatizado.xlsx
@@ -28357,59 +28357,59 @@
         </is>
       </c>
       <c r="F215">
-        <f>SUBTOTAL(109,F7:F214)</f>
+        <f>SUBTOTAL(9,F$7:F$214)</f>
         <v/>
       </c>
       <c r="M215">
-        <f>SUBTOTAL(109,M7:M214)</f>
+        <f>SUBTOTAL(9,M$7:M$214)</f>
         <v/>
       </c>
       <c r="O215">
-        <f>SUBTOTAL(109,O7:O214)</f>
+        <f>SUBTOTAL(9,O$7:O$214)</f>
         <v/>
       </c>
       <c r="P215">
-        <f>SUBTOTAL(109,P7:P214)</f>
+        <f>SUBTOTAL(9,P$7:P$214)</f>
         <v/>
       </c>
       <c r="Q215">
-        <f>SUBTOTAL(109,Q7:Q214)</f>
+        <f>SUBTOTAL(9,Q$7:Q$214)</f>
         <v/>
       </c>
       <c r="R215" s="23">
-        <f>SUBTOTAL(109,R7:R214)</f>
+        <f>SUBTOTAL(9,R$7:R$214)</f>
         <v/>
       </c>
       <c r="S215">
-        <f>SUBTOTAL(109,S7:S214)</f>
+        <f>SUBTOTAL(9,S$7:S$214)</f>
         <v/>
       </c>
       <c r="T215">
-        <f>SUBTOTAL(109,T7:T214)</f>
+        <f>SUBTOTAL(9,T$7:T$214)</f>
         <v/>
       </c>
       <c r="U215">
-        <f>SUBTOTAL(109,U7:U214)</f>
+        <f>SUBTOTAL(9,U$7:U$214)</f>
         <v/>
       </c>
       <c r="V215">
-        <f>SUBTOTAL(109,V7:V214)</f>
+        <f>SUBTOTAL(9,V$7:V$214)</f>
         <v/>
       </c>
       <c r="X215">
-        <f>SUBTOTAL(109,X7:X214)</f>
+        <f>SUBTOTAL(9,X$7:X$214)</f>
         <v/>
       </c>
       <c r="Y215">
-        <f>SUBTOTAL(109,Y7:Y214)</f>
+        <f>SUBTOTAL(9,Y$7:Y$214)</f>
         <v/>
       </c>
       <c r="Z215">
-        <f>SUBTOTAL(109,Z7:Z214)</f>
+        <f>SUBTOTAL(9,Z$7:Z$214)</f>
         <v/>
       </c>
       <c r="AG215">
-        <f>SUBTOTAL(109,AG7:AG214)</f>
+        <f>SUBTOTAL(9,AG$7:AG$214)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Unresponsible commit : CHECKING OUTPUT DATA in the next iteration
</commit_message>
<xml_diff>
--- a/output_automatizado.xlsx
+++ b/output_automatizado.xlsx
@@ -28753,6 +28753,11 @@
       </c>
     </row>
     <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>JUDITH PATRICIA SERRANO HERRER</t>
+        </is>
+      </c>
       <c r="B218" t="inlineStr">
         <is>
           <t>Betancourt Rojas Jacqueline</t>
@@ -29007,6 +29012,11 @@
       </c>
     </row>
     <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>JUDITH PATRICIA SERRANO HERRER</t>
+        </is>
+      </c>
       <c r="B220" t="inlineStr">
         <is>
           <t>Betancourt Rojas Jacqueline</t>
@@ -29393,6 +29403,11 @@
       </c>
     </row>
     <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>JUDITH PATRICIA SERRANO HERRER</t>
+        </is>
+      </c>
       <c r="B223" t="inlineStr">
         <is>
           <t>ORTEGA FORTANEL GABRIELA</t>

</xml_diff>

<commit_message>
Corrigiendo nombres de promotor y gernete
</commit_message>
<xml_diff>
--- a/output_automatizado.xlsx
+++ b/output_automatizado.xlsx
@@ -280,7 +280,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaCartera" displayName="TablaCartera" ref="A6:AJ231" headerRowCount="1" totalsRowShown="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaCartera" displayName="TablaCartera" ref="A6:AJ232" headerRowCount="1" totalsRowShown="1">
   <tableColumns count="36">
     <tableColumn id="1" name="Nombre del gerente" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Nombre promotor"/>
@@ -324,7 +324,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TablaMora" displayName="TablaMora" ref="A6:N16" headerRowCount="1" totalsRowShown="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TablaMora" displayName="TablaMora" ref="A6:N13" headerRowCount="1" totalsRowShown="1">
   <tableColumns count="14">
     <tableColumn id="1" name="Nombre del gerente" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Nombre del promotor"/>
@@ -634,7 +634,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:AJ231"/>
+  <dimension ref="A2:AJ232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -965,19 +965,19 @@
         <v>29640.26</v>
       </c>
       <c r="N7" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O7" s="21" t="n">
-        <v>474244.16</v>
+        <v>444603.9</v>
       </c>
       <c r="P7" s="21" t="n">
         <v>474244.16</v>
       </c>
       <c r="Q7" s="21" t="n">
-        <v>474244.16</v>
+        <v>444603.9</v>
       </c>
       <c r="R7" s="23" t="n">
-        <v>390000</v>
+        <v>365625</v>
       </c>
       <c r="S7" s="21" t="n">
         <v>0</v>
@@ -1007,13 +1007,13 @@
         <v>7</v>
       </c>
       <c r="AB7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AE7" t="n">
         <v>16</v>
@@ -1025,7 +1025,7 @@
         <v>9516.829999999998</v>
       </c>
       <c r="AH7" s="20" t="n">
-        <v>0</v>
+        <v>0.3210778178059166</v>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ponce Galindo Alicia Berenice</t>
+          <t>Contreras Martinez Jose Luis</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -2284,7 +2284,7 @@
         <v>45982</v>
       </c>
       <c r="O17" s="21" t="n">
-        <v>13951.73</v>
+        <v>13519.73</v>
       </c>
       <c r="P17" s="21" t="n">
         <v>94848.8</v>
@@ -2293,10 +2293,10 @@
         <v>17784.14999999999</v>
       </c>
       <c r="R17" s="23" t="n">
-        <v>11845.61</v>
+        <v>11413.61</v>
       </c>
       <c r="S17" s="21" t="n">
-        <v>-3832.419999999995</v>
+        <v>-4264.419999999995</v>
       </c>
       <c r="T17" s="21" t="n">
         <v>0</v>
@@ -2412,23 +2412,21 @@
       <c r="M18" s="21" t="n">
         <v>7448.07</v>
       </c>
-      <c r="N18" s="22" t="n">
-        <v>45980</v>
-      </c>
+      <c r="N18" s="22" t="n"/>
       <c r="O18" s="21" t="n">
-        <v>22344.8</v>
+        <v>0</v>
       </c>
       <c r="P18" s="21" t="n">
         <v>119169.12</v>
       </c>
       <c r="Q18" s="21" t="n">
-        <v>22344.8</v>
+        <v>14896.14</v>
       </c>
       <c r="R18" s="23" t="n">
-        <v>18375.6</v>
+        <v>0</v>
       </c>
       <c r="S18" s="21" t="n">
-        <v>0</v>
+        <v>-14896.14</v>
       </c>
       <c r="T18" s="21" t="n">
         <v>0</v>
@@ -2455,13 +2453,13 @@
         <v>7</v>
       </c>
       <c r="AB18" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AC18" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AD18" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE18" t="n">
         <v>16</v>
@@ -2473,11 +2471,11 @@
         <v>6071.749999999998</v>
       </c>
       <c r="AH18" s="20" t="n">
-        <v>0.0627085529952984</v>
+        <v>0.05822937063849137</v>
       </c>
       <c r="AI18" t="inlineStr">
         <is>
-          <t>Vigente</t>
+          <t>Desertor sin mora</t>
         </is>
       </c>
       <c r="AJ18" t="inlineStr">
@@ -2676,23 +2674,21 @@
       <c r="M20" s="21" t="n">
         <v>3882.18</v>
       </c>
-      <c r="N20" s="22" t="n">
-        <v>45980</v>
-      </c>
+      <c r="N20" s="22" t="n"/>
       <c r="O20" s="21" t="n">
-        <v>15530.72</v>
+        <v>0</v>
       </c>
       <c r="P20" s="21" t="n">
         <v>62114.88</v>
       </c>
       <c r="Q20" s="21" t="n">
-        <v>15530.72</v>
+        <v>11646.54</v>
       </c>
       <c r="R20" s="23" t="n">
-        <v>12752.01</v>
+        <v>0</v>
       </c>
       <c r="S20" s="21" t="n">
-        <v>0</v>
+        <v>-11646.54</v>
       </c>
       <c r="T20" s="21" t="n">
         <v>0</v>
@@ -2719,13 +2715,13 @@
         <v>5</v>
       </c>
       <c r="AB20" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AC20" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="AD20" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE20" t="n">
         <v>16</v>
@@ -2737,11 +2733,11 @@
         <v>8929.82</v>
       </c>
       <c r="AH20" s="20" t="n">
-        <v>0.1916839679424104</v>
+        <v>0.1769390473314557</v>
       </c>
       <c r="AI20" t="inlineStr">
         <is>
-          <t>Vigente</t>
+          <t>Desertor sin mora</t>
         </is>
       </c>
       <c r="AJ20" t="inlineStr">
@@ -2938,11 +2934,9 @@
       <c r="M22" s="21" t="n">
         <v>5396.05</v>
       </c>
-      <c r="N22" s="22" t="n">
-        <v>45985</v>
-      </c>
+      <c r="N22" s="22" t="n"/>
       <c r="O22" s="21" t="n">
-        <v>5368.71</v>
+        <v>0</v>
       </c>
       <c r="P22" s="21" t="n">
         <v>86336.8</v>
@@ -2951,10 +2945,10 @@
         <v>16188.14999999999</v>
       </c>
       <c r="R22" s="23" t="n">
-        <v>4437.5</v>
+        <v>0</v>
       </c>
       <c r="S22" s="21" t="n">
-        <v>-10819.44</v>
+        <v>-16188.14999999999</v>
       </c>
       <c r="T22" s="21" t="n">
         <v>0</v>
@@ -2984,10 +2978,10 @@
         <v>13</v>
       </c>
       <c r="AC22" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AD22" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE22" t="n">
         <v>16</v>
@@ -3003,7 +2997,7 @@
       </c>
       <c r="AI22" t="inlineStr">
         <is>
-          <t>Vigente</t>
+          <t>Desertor sin mora</t>
         </is>
       </c>
       <c r="AJ22" t="inlineStr">
@@ -3202,23 +3196,21 @@
       <c r="M24" s="21" t="n">
         <v>13680.12</v>
       </c>
-      <c r="N24" s="22" t="n">
-        <v>45980</v>
-      </c>
+      <c r="N24" s="22" t="n"/>
       <c r="O24" s="21" t="n">
-        <v>54720.48</v>
+        <v>0</v>
       </c>
       <c r="P24" s="21" t="n">
         <v>218881.92</v>
       </c>
       <c r="Q24" s="21" t="n">
-        <v>54720.48000000001</v>
+        <v>41040.36000000002</v>
       </c>
       <c r="R24" s="23" t="n">
-        <v>45000</v>
+        <v>0</v>
       </c>
       <c r="S24" s="21" t="n">
-        <v>-7.275957614183426e-12</v>
+        <v>-41040.36000000002</v>
       </c>
       <c r="T24" s="21" t="n">
         <v>0</v>
@@ -3245,13 +3237,13 @@
         <v>6</v>
       </c>
       <c r="AB24" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AC24" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="AD24" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AE24" t="n">
         <v>16</v>
@@ -3263,11 +3255,11 @@
         <v>8326.55999999999</v>
       </c>
       <c r="AH24" s="20" t="n">
-        <v>0.05072177729435116</v>
+        <v>0.04682010211786261</v>
       </c>
       <c r="AI24" t="inlineStr">
         <is>
-          <t>Vigente</t>
+          <t>Desertor sin mora</t>
         </is>
       </c>
       <c r="AJ24" t="inlineStr">
@@ -3284,7 +3276,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ponce Galindo Alicia Berenice</t>
+          <t>Contreras Martinez Jose Luis</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -3335,19 +3327,19 @@
         <v>9272.08</v>
       </c>
       <c r="N25" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O25" s="21" t="n">
-        <v>70670.22</v>
+        <v>66866.22</v>
       </c>
       <c r="P25" s="21" t="n">
         <v>148353.28</v>
       </c>
       <c r="Q25" s="21" t="n">
-        <v>70670.22</v>
+        <v>66866.22</v>
       </c>
       <c r="R25" s="23" t="n">
-        <v>30500</v>
+        <v>22875</v>
       </c>
       <c r="S25" s="21" t="n">
         <v>0</v>
@@ -3356,16 +3348,16 @@
         <v>14737.92</v>
       </c>
       <c r="U25" s="21" t="n">
-        <v>13902.74</v>
+        <v>17723.74</v>
       </c>
       <c r="V25" s="21" t="n">
-        <v>28640.66</v>
+        <v>32461.66</v>
       </c>
       <c r="W25" s="20" t="n">
-        <v>0.4842803580480839</v>
+        <v>0.5866212380725544</v>
       </c>
       <c r="X25" s="21" t="n">
-        <v>30500</v>
+        <v>22875</v>
       </c>
       <c r="Y25" s="21" t="n">
         <v>2537.92</v>
@@ -3377,25 +3369,25 @@
         <v>10</v>
       </c>
       <c r="AB25" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AC25" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AD25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AE25" t="n">
         <v>16</v>
       </c>
       <c r="AF25" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AG25" s="21" t="n">
         <v>2537.92</v>
       </c>
       <c r="AH25" s="20" t="n">
-        <v>0.02280969678144854</v>
+        <v>0.02105510472133711</v>
       </c>
       <c r="AI25" t="inlineStr">
         <is>
@@ -3863,22 +3855,22 @@
         <v>11400.1</v>
       </c>
       <c r="N29" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O29" s="21" t="n">
-        <v>56913.6</v>
+        <v>45505.6</v>
       </c>
       <c r="P29" s="21" t="n">
         <v>182401.6</v>
       </c>
       <c r="Q29" s="21" t="n">
-        <v>57000.5</v>
+        <v>45600.39999999999</v>
       </c>
       <c r="R29" s="23" t="n">
-        <v>46875</v>
+        <v>37500</v>
       </c>
       <c r="S29" s="21" t="n">
-        <v>-86.90000000000146</v>
+        <v>-94.79999999999563</v>
       </c>
       <c r="T29" s="21" t="n">
         <v>0</v>
@@ -3896,7 +3888,7 @@
         <v>0</v>
       </c>
       <c r="Y29" s="21" t="n">
-        <v>8290</v>
+        <v>9042</v>
       </c>
       <c r="Z29" s="21" t="n">
         <v>18750</v>
@@ -3905,13 +3897,13 @@
         <v>8</v>
       </c>
       <c r="AB29" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AC29" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AD29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE29" t="n">
         <v>16</v>
@@ -3920,10 +3912,10 @@
         <v>0</v>
       </c>
       <c r="AG29" s="21" t="n">
-        <v>8290</v>
+        <v>9042</v>
       </c>
       <c r="AH29" s="20" t="n">
-        <v>0.0661078730569349</v>
+        <v>0.06609591143937334</v>
       </c>
       <c r="AI29" t="inlineStr">
         <is>
@@ -3998,16 +3990,16 @@
         <v>45985</v>
       </c>
       <c r="O30" s="21" t="n">
-        <v>50920.48</v>
+        <v>40736.39</v>
       </c>
       <c r="P30" s="21" t="n">
         <v>162945.44</v>
       </c>
       <c r="Q30" s="21" t="n">
-        <v>50920.48</v>
+        <v>40736.39</v>
       </c>
       <c r="R30" s="23" t="n">
-        <v>41875.03</v>
+        <v>33500.02</v>
       </c>
       <c r="S30" s="21" t="n">
         <v>0</v>
@@ -4181,7 +4173,7 @@
         <v>16</v>
       </c>
       <c r="AF31" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG31" s="21" t="n">
         <v>3776</v>
@@ -4394,7 +4386,7 @@
         <v>45985</v>
       </c>
       <c r="O33" s="21" t="n">
-        <v>19763.64</v>
+        <v>15200.64</v>
       </c>
       <c r="P33" s="21" t="n">
         <v>85120.8</v>
@@ -4403,10 +4395,10 @@
         <v>21280.2</v>
       </c>
       <c r="R33" s="23" t="n">
-        <v>16875</v>
+        <v>13125</v>
       </c>
       <c r="S33" s="21" t="n">
-        <v>-1516.559999999998</v>
+        <v>-6079.559999999998</v>
       </c>
       <c r="T33" s="21" t="n">
         <v>0</v>
@@ -4424,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="Y33" s="21" t="n">
-        <v>3894</v>
+        <v>4212</v>
       </c>
       <c r="Z33" s="21" t="n">
         <v>14000</v>
@@ -4448,10 +4440,10 @@
         <v>0</v>
       </c>
       <c r="AG33" s="21" t="n">
-        <v>3894</v>
+        <v>4212</v>
       </c>
       <c r="AH33" s="20" t="n">
-        <v>0.06099566733395363</v>
+        <v>0.06597682352609467</v>
       </c>
       <c r="AI33" t="inlineStr">
         <is>
@@ -4655,7 +4647,7 @@
         <v>9804.09</v>
       </c>
       <c r="N35" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O35" s="21" t="n">
         <v>49021.38</v>
@@ -4667,25 +4659,25 @@
         <v>49021.38</v>
       </c>
       <c r="R35" s="23" t="n">
-        <v>40313.45</v>
+        <v>32250</v>
       </c>
       <c r="S35" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T35" s="21" t="n">
-        <v>0</v>
+        <v>8063.45</v>
       </c>
       <c r="U35" s="21" t="n">
         <v>0</v>
       </c>
       <c r="V35" s="21" t="n">
-        <v>0</v>
+        <v>8063.45</v>
       </c>
       <c r="W35" s="20" t="n">
-        <v>0</v>
+        <v>0.2000188522689078</v>
       </c>
       <c r="X35" s="21" t="n">
-        <v>0</v>
+        <v>32250</v>
       </c>
       <c r="Y35" s="21" t="n">
         <v>6519</v>
@@ -4697,13 +4689,13 @@
         <v>7</v>
       </c>
       <c r="AB35" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AC35" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AD35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE35" t="n">
         <v>16</v>
@@ -4715,7 +4707,7 @@
         <v>6519</v>
       </c>
       <c r="AH35" s="20" t="n">
-        <v>0.06044787059649224</v>
+        <v>0.05541054804678455</v>
       </c>
       <c r="AI35" t="inlineStr">
         <is>
@@ -4790,19 +4782,19 @@
         <v>45985</v>
       </c>
       <c r="O36" s="21" t="n">
-        <v>55479.46</v>
+        <v>44383.35</v>
       </c>
       <c r="P36" s="21" t="n">
         <v>177537.6</v>
       </c>
       <c r="Q36" s="21" t="n">
-        <v>55479.46</v>
+        <v>44384.39999999999</v>
       </c>
       <c r="R36" s="23" t="n">
-        <v>45625</v>
+        <v>36500</v>
       </c>
       <c r="S36" s="21" t="n">
-        <v>0</v>
+        <v>-1.049999999995634</v>
       </c>
       <c r="T36" s="21" t="n">
         <v>0</v>
@@ -5054,19 +5046,19 @@
         <v>45980</v>
       </c>
       <c r="O38" s="21" t="n">
-        <v>45601.28</v>
+        <v>36481.28</v>
       </c>
       <c r="P38" s="21" t="n">
         <v>145921.28</v>
       </c>
       <c r="Q38" s="21" t="n">
-        <v>45601.28</v>
+        <v>45600.39999999999</v>
       </c>
       <c r="R38" s="23" t="n">
-        <v>37500.86</v>
+        <v>30000.96</v>
       </c>
       <c r="S38" s="21" t="n">
-        <v>0</v>
+        <v>-9119.119999999995</v>
       </c>
       <c r="T38" s="21" t="n">
         <v>0</v>
@@ -5084,7 +5076,7 @@
         <v>0</v>
       </c>
       <c r="Y38" s="21" t="n">
-        <v>5159</v>
+        <v>5628</v>
       </c>
       <c r="Z38" s="21" t="n">
         <v>15000</v>
@@ -5108,10 +5100,10 @@
         <v>0</v>
       </c>
       <c r="AG38" s="21" t="n">
-        <v>5159</v>
+        <v>5628</v>
       </c>
       <c r="AH38" s="20" t="n">
-        <v>0.05142498750010965</v>
+        <v>0.05609998636375597</v>
       </c>
       <c r="AI38" t="inlineStr">
         <is>
@@ -5186,19 +5178,19 @@
         <v>45980</v>
       </c>
       <c r="O39" s="21" t="n">
-        <v>36101.01</v>
+        <v>28881.01</v>
       </c>
       <c r="P39" s="21" t="n">
         <v>115520.96</v>
       </c>
       <c r="Q39" s="21" t="n">
-        <v>36101.01</v>
+        <v>36100.3</v>
       </c>
       <c r="R39" s="23" t="n">
-        <v>29688.2</v>
+        <v>23750.76</v>
       </c>
       <c r="S39" s="21" t="n">
-        <v>0</v>
+        <v>-7219.290000000001</v>
       </c>
       <c r="T39" s="21" t="n">
         <v>0</v>
@@ -5216,7 +5208,7 @@
         <v>0</v>
       </c>
       <c r="Y39" s="21" t="n">
-        <v>5080</v>
+        <v>5540</v>
       </c>
       <c r="Z39" s="21" t="n">
         <v>19000</v>
@@ -5240,10 +5232,10 @@
         <v>0</v>
       </c>
       <c r="AG39" s="21" t="n">
-        <v>5080</v>
+        <v>5540</v>
       </c>
       <c r="AH39" s="20" t="n">
-        <v>0.06396320554374642</v>
+        <v>0.06975514935282583</v>
       </c>
       <c r="AI39" t="inlineStr">
         <is>
@@ -6188,7 +6180,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Ponce Galindo Alicia Berenice</t>
+          <t>Contreras Martinez Jose Luis</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -6293,7 +6285,7 @@
         <v>16</v>
       </c>
       <c r="AF47" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AG47" s="21" t="n">
         <v>1230</v>
@@ -7166,34 +7158,34 @@
         <v>45982</v>
       </c>
       <c r="O54" s="21" t="n">
-        <v>66632.27</v>
+        <v>45212.27</v>
       </c>
       <c r="P54" s="21" t="n">
         <v>144705.28</v>
       </c>
       <c r="Q54" s="21" t="n">
-        <v>66632.27</v>
+        <v>45220.39999999999</v>
       </c>
       <c r="R54" s="23" t="n">
         <v>37187.5</v>
       </c>
       <c r="S54" s="21" t="n">
-        <v>0</v>
+        <v>-8.129999999990105</v>
       </c>
       <c r="T54" s="21" t="n">
-        <v>12730.89</v>
+        <v>0</v>
       </c>
       <c r="U54" s="21" t="n">
         <v>0</v>
       </c>
       <c r="V54" s="21" t="n">
-        <v>12730.89</v>
+        <v>0</v>
       </c>
       <c r="W54" s="20" t="n">
-        <v>0.2550340666035102</v>
+        <v>0</v>
       </c>
       <c r="X54" s="21" t="n">
-        <v>37187.5</v>
+        <v>0</v>
       </c>
       <c r="Y54" s="21" t="n">
         <v>5496</v>
@@ -7217,7 +7209,7 @@
         <v>16</v>
       </c>
       <c r="AF54" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG54" s="21" t="n">
         <v>5496</v>
@@ -7295,22 +7287,22 @@
         <v>5168.05</v>
       </c>
       <c r="N55" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O55" s="21" t="n">
-        <v>31008.23</v>
+        <v>25840.18</v>
       </c>
       <c r="P55" s="21" t="n">
         <v>82688.8</v>
       </c>
       <c r="Q55" s="21" t="n">
-        <v>31008.3</v>
+        <v>25840.25</v>
       </c>
       <c r="R55" s="23" t="n">
-        <v>25500</v>
+        <v>21250</v>
       </c>
       <c r="S55" s="21" t="n">
-        <v>-0.07000000000334694</v>
+        <v>-0.06999999999970896</v>
       </c>
       <c r="T55" s="21" t="n">
         <v>0</v>
@@ -7328,7 +7320,7 @@
         <v>0</v>
       </c>
       <c r="Y55" s="21" t="n">
-        <v>3557.549999999998</v>
+        <v>4021.499999999998</v>
       </c>
       <c r="Z55" s="21" t="n">
         <v>11333.33333333333</v>
@@ -7337,13 +7329,13 @@
         <v>6</v>
       </c>
       <c r="AB55" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AC55" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AD55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AE55" t="n">
         <v>16</v>
@@ -7352,10 +7344,10 @@
         <v>0</v>
       </c>
       <c r="AG55" s="21" t="n">
-        <v>3557.549999999998</v>
+        <v>4021.499999999998</v>
       </c>
       <c r="AH55" s="20" t="n">
-        <v>0.06883737579938272</v>
+        <v>0.07074059056915256</v>
       </c>
       <c r="AI55" t="inlineStr">
         <is>
@@ -8090,16 +8082,16 @@
         <v>45985</v>
       </c>
       <c r="O61" s="21" t="n">
-        <v>45220.91</v>
+        <v>38760.91</v>
       </c>
       <c r="P61" s="21" t="n">
         <v>103360.96</v>
       </c>
       <c r="Q61" s="21" t="n">
-        <v>45220.91</v>
+        <v>38760.91</v>
       </c>
       <c r="R61" s="23" t="n">
-        <v>37188.01</v>
+        <v>31875.58</v>
       </c>
       <c r="S61" s="21" t="n">
         <v>0</v>
@@ -8351,22 +8343,22 @@
         <v>8436.07</v>
       </c>
       <c r="N63" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O63" s="21" t="n">
-        <v>59020.11</v>
+        <v>50578.11</v>
       </c>
       <c r="P63" s="21" t="n">
         <v>134977.12</v>
       </c>
       <c r="Q63" s="21" t="n">
-        <v>59052.48999999999</v>
+        <v>50616.42</v>
       </c>
       <c r="R63" s="23" t="n">
-        <v>48562.5</v>
+        <v>41625</v>
       </c>
       <c r="S63" s="21" t="n">
-        <v>-32.3799999999901</v>
+        <v>-38.30999999999767</v>
       </c>
       <c r="T63" s="21" t="n">
         <v>0</v>
@@ -8384,7 +8376,7 @@
         <v>0</v>
       </c>
       <c r="Y63" s="21" t="n">
-        <v>3807.93</v>
+        <v>4229.93</v>
       </c>
       <c r="Z63" s="21" t="n">
         <v>18500</v>
@@ -8393,13 +8385,13 @@
         <v>6</v>
       </c>
       <c r="AB63" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AC63" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD63" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE63" t="n">
         <v>16</v>
@@ -8408,10 +8400,10 @@
         <v>0</v>
       </c>
       <c r="AG63" s="21" t="n">
-        <v>3807.93</v>
+        <v>4229.93</v>
       </c>
       <c r="AH63" s="20" t="n">
-        <v>0.05015408043476801</v>
+        <v>0.05014100167495054</v>
       </c>
       <c r="AI63" t="inlineStr">
         <is>
@@ -8483,22 +8475,22 @@
         <v>7372.06</v>
       </c>
       <c r="N64" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O64" s="21" t="n">
-        <v>51572.03</v>
+        <v>44196.03</v>
       </c>
       <c r="P64" s="21" t="n">
         <v>117952.96</v>
       </c>
       <c r="Q64" s="21" t="n">
-        <v>51604.42</v>
+        <v>44232.36</v>
       </c>
       <c r="R64" s="23" t="n">
-        <v>42437.5</v>
+        <v>36375</v>
       </c>
       <c r="S64" s="21" t="n">
-        <v>-32.38999999999942</v>
+        <v>-36.33000000000175</v>
       </c>
       <c r="T64" s="21" t="n">
         <v>0</v>
@@ -8516,7 +8508,7 @@
         <v>0</v>
       </c>
       <c r="Y64" s="21" t="n">
-        <v>3621</v>
+        <v>4023</v>
       </c>
       <c r="Z64" s="21" t="n">
         <v>16166.66666666667</v>
@@ -8525,13 +8517,13 @@
         <v>6</v>
       </c>
       <c r="AB64" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AC64" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD64" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE64" t="n">
         <v>16</v>
@@ -8540,10 +8532,10 @@
         <v>0</v>
       </c>
       <c r="AG64" s="21" t="n">
-        <v>3621</v>
+        <v>4023</v>
       </c>
       <c r="AH64" s="20" t="n">
-        <v>0.05457542848719805</v>
+        <v>0.0545709069106871</v>
       </c>
       <c r="AI64" t="inlineStr">
         <is>
@@ -8615,22 +8607,22 @@
         <v>11172.1</v>
       </c>
       <c r="N65" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O65" s="21" t="n">
-        <v>78161.57000000001</v>
+        <v>66983.57000000001</v>
       </c>
       <c r="P65" s="21" t="n">
         <v>178753.6</v>
       </c>
       <c r="Q65" s="21" t="n">
-        <v>78204.7</v>
+        <v>67032.60000000001</v>
       </c>
       <c r="R65" s="23" t="n">
-        <v>64312.5</v>
+        <v>55125</v>
       </c>
       <c r="S65" s="21" t="n">
-        <v>-43.1299999999901</v>
+        <v>-49.02999999999884</v>
       </c>
       <c r="T65" s="21" t="n">
         <v>0</v>
@@ -8648,7 +8640,7 @@
         <v>0</v>
       </c>
       <c r="Y65" s="21" t="n">
-        <v>5805</v>
+        <v>6450</v>
       </c>
       <c r="Z65" s="21" t="n">
         <v>24500</v>
@@ -8657,13 +8649,13 @@
         <v>6</v>
       </c>
       <c r="AB65" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AC65" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AD65" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AE65" t="n">
         <v>16</v>
@@ -8672,7 +8664,7 @@
         <v>0</v>
       </c>
       <c r="AG65" s="21" t="n">
-        <v>5805</v>
+        <v>6450</v>
       </c>
       <c r="AH65" s="20" t="n">
         <v>0.05773310299764592</v>
@@ -8696,7 +8688,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Ponce Galindo Alicia Berenice</t>
+          <t>Contreras Martinez Jose Luis</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -9356,7 +9348,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Ponce Galindo Alicia Berenice</t>
+          <t>Contreras Martinez Jose Luis</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -9989,7 +9981,7 @@
         <v>16</v>
       </c>
       <c r="AF75" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG75" s="21" t="n">
         <v>7586</v>
@@ -11258,16 +11250,16 @@
         <v>45985</v>
       </c>
       <c r="O85" s="21" t="n">
-        <v>94240.85000000001</v>
+        <v>82460.75</v>
       </c>
       <c r="P85" s="21" t="n">
         <v>188481.6</v>
       </c>
       <c r="Q85" s="21" t="n">
-        <v>94240.85000000001</v>
+        <v>82460.75</v>
       </c>
       <c r="R85" s="23" t="n">
-        <v>77500.00999999999</v>
+        <v>67812.53</v>
       </c>
       <c r="S85" s="21" t="n">
         <v>0</v>
@@ -12314,16 +12306,16 @@
         <v>45985</v>
       </c>
       <c r="O93" s="21" t="n">
-        <v>66349.03</v>
+        <v>58977.03</v>
       </c>
       <c r="P93" s="21" t="n">
         <v>117952.96</v>
       </c>
       <c r="Q93" s="21" t="n">
-        <v>66349.03</v>
+        <v>58977.03</v>
       </c>
       <c r="R93" s="23" t="n">
-        <v>54562.96</v>
+        <v>48500.51</v>
       </c>
       <c r="S93" s="21" t="n">
         <v>0</v>
@@ -12446,19 +12438,19 @@
         <v>45985</v>
       </c>
       <c r="O94" s="21" t="n">
-        <v>34892.54</v>
+        <v>31018.54</v>
       </c>
       <c r="P94" s="21" t="n">
         <v>62016.48</v>
       </c>
       <c r="Q94" s="21" t="n">
-        <v>34892.54</v>
+        <v>34884.27</v>
       </c>
       <c r="R94" s="23" t="n">
-        <v>28695.74</v>
+        <v>25510.27</v>
       </c>
       <c r="S94" s="21" t="n">
-        <v>0</v>
+        <v>-3865.730000000003</v>
       </c>
       <c r="T94" s="21" t="n">
         <v>0</v>
@@ -12575,22 +12567,22 @@
         <v>4788.04</v>
       </c>
       <c r="N95" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O95" s="21" t="n">
-        <v>43086.67</v>
+        <v>38298.67</v>
       </c>
       <c r="P95" s="21" t="n">
         <v>76608.64</v>
       </c>
       <c r="Q95" s="21" t="n">
-        <v>43092.36</v>
+        <v>38304.32</v>
       </c>
       <c r="R95" s="23" t="n">
-        <v>35437.5</v>
+        <v>31500</v>
       </c>
       <c r="S95" s="21" t="n">
-        <v>-5.690000000002328</v>
+        <v>-5.650000000001455</v>
       </c>
       <c r="T95" s="21" t="n">
         <v>0</v>
@@ -12608,7 +12600,7 @@
         <v>0</v>
       </c>
       <c r="Y95" s="21" t="n">
-        <v>2448</v>
+        <v>2805</v>
       </c>
       <c r="Z95" s="21" t="n">
         <v>12600</v>
@@ -12617,13 +12609,13 @@
         <v>5</v>
       </c>
       <c r="AB95" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC95" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD95" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AE95" t="n">
         <v>16</v>
@@ -12632,10 +12624,10 @@
         <v>0</v>
       </c>
       <c r="AG95" s="21" t="n">
-        <v>2448</v>
+        <v>2805</v>
       </c>
       <c r="AH95" s="20" t="n">
-        <v>0.07303913202777874</v>
+        <v>0.07322933810076775</v>
       </c>
       <c r="AI95" t="inlineStr">
         <is>
@@ -12707,22 +12699,22 @@
         <v>6840.06</v>
       </c>
       <c r="N96" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O96" s="21" t="n">
-        <v>61559.96</v>
+        <v>54719.96</v>
       </c>
       <c r="P96" s="21" t="n">
         <v>109440.96</v>
       </c>
       <c r="Q96" s="21" t="n">
-        <v>61560.54</v>
+        <v>54720.48</v>
       </c>
       <c r="R96" s="23" t="n">
-        <v>50625</v>
+        <v>45000</v>
       </c>
       <c r="S96" s="21" t="n">
-        <v>-0.5800000000017462</v>
+        <v>-0.5200000000040745</v>
       </c>
       <c r="T96" s="21" t="n">
         <v>0</v>
@@ -12740,7 +12732,7 @@
         <v>0</v>
       </c>
       <c r="Y96" s="21" t="n">
-        <v>2536.42</v>
+        <v>2896.42</v>
       </c>
       <c r="Z96" s="21" t="n">
         <v>15000</v>
@@ -12749,13 +12741,13 @@
         <v>6</v>
       </c>
       <c r="AB96" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC96" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD96" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AE96" t="n">
         <v>16</v>
@@ -12764,10 +12756,10 @@
         <v>0</v>
       </c>
       <c r="AG96" s="21" t="n">
-        <v>2536.42</v>
+        <v>2896.42</v>
       </c>
       <c r="AH96" s="20" t="n">
-        <v>0.05297405494772184</v>
+        <v>0.05293118773811926</v>
       </c>
       <c r="AI96" t="inlineStr">
         <is>
@@ -12839,22 +12831,22 @@
         <v>8664.08</v>
       </c>
       <c r="N97" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O97" s="21" t="n">
-        <v>77728.54000000001</v>
+        <v>69056.44</v>
       </c>
       <c r="P97" s="21" t="n">
         <v>138625.28</v>
       </c>
       <c r="Q97" s="21" t="n">
-        <v>77976.72</v>
+        <v>69312.64</v>
       </c>
       <c r="R97" s="23" t="n">
-        <v>64125</v>
+        <v>57000</v>
       </c>
       <c r="S97" s="21" t="n">
-        <v>-248.179999999993</v>
+        <v>-256.1999999999971</v>
       </c>
       <c r="T97" s="21" t="n">
         <v>0</v>
@@ -12872,7 +12864,7 @@
         <v>0</v>
       </c>
       <c r="Y97" s="21" t="n">
-        <v>3745.839999999998</v>
+        <v>4313.749999999998</v>
       </c>
       <c r="Z97" s="21" t="n">
         <v>12666.66666666667</v>
@@ -12881,13 +12873,13 @@
         <v>9</v>
       </c>
       <c r="AB97" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AC97" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD97" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AE97" t="n">
         <v>16</v>
@@ -12896,10 +12888,10 @@
         <v>0</v>
       </c>
       <c r="AG97" s="21" t="n">
-        <v>3745.839999999998</v>
+        <v>4313.749999999998</v>
       </c>
       <c r="AH97" s="20" t="n">
-        <v>0.06176304927932334</v>
+        <v>0.06223612316599105</v>
       </c>
       <c r="AI97" t="inlineStr">
         <is>
@@ -13004,7 +12996,7 @@
         <v>0</v>
       </c>
       <c r="Y98" s="21" t="n">
-        <v>6064.749999999996</v>
+        <v>6632.659999999996</v>
       </c>
       <c r="Z98" s="21" t="n">
         <v>10200</v>
@@ -13028,10 +13020,10 @@
         <v>0</v>
       </c>
       <c r="AG98" s="21" t="n">
-        <v>6064.749999999996</v>
+        <v>6632.659999999996</v>
       </c>
       <c r="AH98" s="20" t="n">
-        <v>0.2235258388461535</v>
+        <v>0.2444570493888996</v>
       </c>
       <c r="AI98" t="inlineStr">
         <is>
@@ -13106,7 +13098,7 @@
         <v>45980</v>
       </c>
       <c r="O99" s="21" t="n">
-        <v>42366.66</v>
+        <v>37648.66</v>
       </c>
       <c r="P99" s="21" t="n">
         <v>75392.64</v>
@@ -13115,10 +13107,10 @@
         <v>42408.36</v>
       </c>
       <c r="R99" s="23" t="n">
-        <v>34875</v>
+        <v>31000</v>
       </c>
       <c r="S99" s="21" t="n">
-        <v>-41.69999999999709</v>
+        <v>-4759.699999999997</v>
       </c>
       <c r="T99" s="21" t="n">
         <v>0</v>
@@ -13136,7 +13128,7 @@
         <v>0</v>
       </c>
       <c r="Y99" s="21" t="n">
-        <v>1700</v>
+        <v>1945</v>
       </c>
       <c r="Z99" s="21" t="n">
         <v>10333.33333333333</v>
@@ -13160,10 +13152,10 @@
         <v>0</v>
       </c>
       <c r="AG99" s="21" t="n">
-        <v>1700</v>
+        <v>1945</v>
       </c>
       <c r="AH99" s="20" t="n">
-        <v>0.0515397031555638</v>
+        <v>0.05896748390445388</v>
       </c>
       <c r="AI99" t="inlineStr">
         <is>
@@ -14291,40 +14283,40 @@
         <v>4180.04</v>
       </c>
       <c r="N108" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O108" s="21" t="n">
-        <v>45978.59</v>
+        <v>37617.59</v>
       </c>
       <c r="P108" s="21" t="n">
         <v>66880.64</v>
       </c>
       <c r="Q108" s="21" t="n">
-        <v>45978.59</v>
+        <v>37620.36</v>
       </c>
       <c r="R108" s="23" t="n">
-        <v>34375</v>
+        <v>30937.5</v>
       </c>
       <c r="S108" s="21" t="n">
-        <v>0</v>
+        <v>-2.769999999996799</v>
       </c>
       <c r="T108" s="21" t="n">
-        <v>3437.5</v>
+        <v>0</v>
       </c>
       <c r="U108" s="21" t="n">
         <v>0</v>
       </c>
       <c r="V108" s="21" t="n">
-        <v>3437.5</v>
+        <v>0</v>
       </c>
       <c r="W108" s="20" t="n">
-        <v>0.09090909090909091</v>
+        <v>0</v>
       </c>
       <c r="X108" s="21" t="n">
-        <v>34375</v>
+        <v>0</v>
       </c>
       <c r="Y108" s="21" t="n">
-        <v>866</v>
+        <v>886</v>
       </c>
       <c r="Z108" s="21" t="n">
         <v>11000</v>
@@ -14333,25 +14325,25 @@
         <v>5</v>
       </c>
       <c r="AB108" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC108" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD108" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE108" t="n">
         <v>16</v>
       </c>
       <c r="AF108" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AG108" s="21" t="n">
-        <v>866</v>
+        <v>886</v>
       </c>
       <c r="AH108" s="20" t="n">
-        <v>0.03452917515940836</v>
+        <v>0.0302799563093723</v>
       </c>
       <c r="AI108" t="inlineStr">
         <is>
@@ -14819,19 +14811,19 @@
         <v>8664.08</v>
       </c>
       <c r="N112" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O112" s="21" t="n">
-        <v>86641.22</v>
+        <v>77977.22</v>
       </c>
       <c r="P112" s="21" t="n">
         <v>138625.28</v>
       </c>
       <c r="Q112" s="21" t="n">
-        <v>86641.22</v>
+        <v>77977.22</v>
       </c>
       <c r="R112" s="23" t="n">
-        <v>71250.46000000001</v>
+        <v>64125.54</v>
       </c>
       <c r="S112" s="21" t="n">
         <v>0</v>
@@ -14852,7 +14844,7 @@
         <v>0</v>
       </c>
       <c r="Y112" s="21" t="n">
-        <v>5216</v>
+        <v>6082</v>
       </c>
       <c r="Z112" s="21" t="n">
         <v>16285.71428571429</v>
@@ -14861,13 +14853,13 @@
         <v>7</v>
       </c>
       <c r="AB112" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC112" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD112" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE112" t="n">
         <v>16</v>
@@ -14876,10 +14868,10 @@
         <v>0</v>
       </c>
       <c r="AG112" s="21" t="n">
-        <v>5216</v>
+        <v>6082</v>
       </c>
       <c r="AH112" s="20" t="n">
-        <v>0.1003376392338637</v>
+        <v>0.100282677775037</v>
       </c>
       <c r="AI112" t="inlineStr">
         <is>
@@ -15083,22 +15075,22 @@
         <v>5776.05</v>
       </c>
       <c r="N114" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O114" s="21" t="n">
-        <v>57724.76</v>
+        <v>51942.76</v>
       </c>
       <c r="P114" s="21" t="n">
         <v>92416.8</v>
       </c>
       <c r="Q114" s="21" t="n">
-        <v>57760.5</v>
+        <v>51984.45</v>
       </c>
       <c r="R114" s="23" t="n">
-        <v>47500</v>
+        <v>42750</v>
       </c>
       <c r="S114" s="21" t="n">
-        <v>-35.73999999999796</v>
+        <v>-41.69000000000233</v>
       </c>
       <c r="T114" s="21" t="n">
         <v>0</v>
@@ -15116,7 +15108,7 @@
         <v>0</v>
       </c>
       <c r="Y114" s="21" t="n">
-        <v>1746</v>
+        <v>2035</v>
       </c>
       <c r="Z114" s="21" t="n">
         <v>12666.66666666667</v>
@@ -15125,13 +15117,13 @@
         <v>6</v>
       </c>
       <c r="AB114" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC114" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD114" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE114" t="n">
         <v>16</v>
@@ -15140,10 +15132,10 @@
         <v>0</v>
       </c>
       <c r="AG114" s="21" t="n">
-        <v>1746</v>
+        <v>2035</v>
       </c>
       <c r="AH114" s="20" t="n">
-        <v>0.05038045030773625</v>
+        <v>0.05033098496624609</v>
       </c>
       <c r="AI114" t="inlineStr">
         <is>
@@ -15218,19 +15210,19 @@
         <v>45985</v>
       </c>
       <c r="O115" s="21" t="n">
-        <v>121599.71</v>
+        <v>109438.71</v>
       </c>
       <c r="P115" s="21" t="n">
         <v>194561.76</v>
       </c>
       <c r="Q115" s="21" t="n">
-        <v>121599.71</v>
+        <v>109440.99</v>
       </c>
       <c r="R115" s="23" t="n">
-        <v>100000</v>
+        <v>90000</v>
       </c>
       <c r="S115" s="21" t="n">
-        <v>0</v>
+        <v>-2.279999999998836</v>
       </c>
       <c r="T115" s="21" t="n">
         <v>0</v>
@@ -15347,22 +15339,22 @@
         <v>4332.04</v>
       </c>
       <c r="N116" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O116" s="21" t="n">
-        <v>43316.57</v>
+        <v>38983.57</v>
       </c>
       <c r="P116" s="21" t="n">
         <v>69312.64</v>
       </c>
       <c r="Q116" s="21" t="n">
-        <v>43320.4</v>
+        <v>38988.36</v>
       </c>
       <c r="R116" s="23" t="n">
-        <v>35625</v>
+        <v>32062.5</v>
       </c>
       <c r="S116" s="21" t="n">
-        <v>-3.830000000001746</v>
+        <v>-4.790000000000873</v>
       </c>
       <c r="T116" s="21" t="n">
         <v>0</v>
@@ -15380,7 +15372,7 @@
         <v>0</v>
       </c>
       <c r="Y116" s="21" t="n">
-        <v>2045.96</v>
+        <v>2477.96</v>
       </c>
       <c r="Z116" s="21" t="n">
         <v>11400</v>
@@ -15389,13 +15381,13 @@
         <v>5</v>
       </c>
       <c r="AB116" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC116" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD116" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE116" t="n">
         <v>16</v>
@@ -15404,10 +15396,10 @@
         <v>0</v>
       </c>
       <c r="AG116" s="21" t="n">
-        <v>2045.96</v>
+        <v>2477.96</v>
       </c>
       <c r="AH116" s="20" t="n">
-        <v>0.07871426241062718</v>
+        <v>0.08171537790839552</v>
       </c>
       <c r="AI116" t="inlineStr">
         <is>
@@ -15479,37 +15471,37 @@
         <v>4940.04</v>
       </c>
       <c r="N117" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O117" s="21" t="n">
-        <v>53801.61</v>
+        <v>52496.61</v>
       </c>
       <c r="P117" s="21" t="n">
         <v>79040.64</v>
       </c>
       <c r="Q117" s="21" t="n">
-        <v>53801.61</v>
+        <v>52496.61</v>
       </c>
       <c r="R117" s="23" t="n">
-        <v>40625</v>
+        <v>36562.5</v>
       </c>
       <c r="S117" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T117" s="21" t="n">
-        <v>4062.5</v>
+        <v>7704.92</v>
       </c>
       <c r="U117" s="21" t="n">
-        <v>0</v>
+        <v>331.29</v>
       </c>
       <c r="V117" s="21" t="n">
-        <v>4062.5</v>
+        <v>8036.21</v>
       </c>
       <c r="W117" s="20" t="n">
-        <v>0.09090909090909091</v>
+        <v>0.180189292470567</v>
       </c>
       <c r="X117" s="21" t="n">
-        <v>40625</v>
+        <v>36562.5</v>
       </c>
       <c r="Y117" s="21" t="n">
         <v>1204.92</v>
@@ -15521,25 +15513,25 @@
         <v>5</v>
       </c>
       <c r="AB117" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC117" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD117" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE117" t="n">
         <v>16</v>
       </c>
       <c r="AF117" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AG117" s="21" t="n">
         <v>1204.92</v>
       </c>
       <c r="AH117" s="20" t="n">
-        <v>0.04065149270046397</v>
+        <v>0.03484413660039769</v>
       </c>
       <c r="AI117" t="inlineStr">
         <is>
@@ -15611,22 +15603,22 @@
         <v>4940.04</v>
       </c>
       <c r="N118" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O118" s="21" t="n">
-        <v>42198.69</v>
+        <v>37252.69</v>
       </c>
       <c r="P118" s="21" t="n">
         <v>79040.64</v>
       </c>
       <c r="Q118" s="21" t="n">
-        <v>49400.4</v>
+        <v>44460.36</v>
       </c>
       <c r="R118" s="23" t="n">
-        <v>35178.33</v>
+        <v>31109.89</v>
       </c>
       <c r="S118" s="21" t="n">
-        <v>-7201.709999999999</v>
+        <v>-7207.669999999998</v>
       </c>
       <c r="T118" s="21" t="n">
         <v>0</v>
@@ -15644,7 +15636,7 @@
         <v>0</v>
       </c>
       <c r="Y118" s="21" t="n">
-        <v>2128</v>
+        <v>2432</v>
       </c>
       <c r="Z118" s="21" t="n">
         <v>10833.33333333333</v>
@@ -15653,13 +15645,13 @@
         <v>6</v>
       </c>
       <c r="AB118" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC118" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD118" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE118" t="n">
         <v>16</v>
@@ -15668,10 +15660,10 @@
         <v>0</v>
       </c>
       <c r="AG118" s="21" t="n">
-        <v>2128</v>
+        <v>2432</v>
       </c>
       <c r="AH118" s="20" t="n">
-        <v>0.07179429046458463</v>
+        <v>0.07032910086326657</v>
       </c>
       <c r="AI118" t="inlineStr">
         <is>
@@ -15743,19 +15735,19 @@
         <v>3192.03</v>
       </c>
       <c r="N119" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O119" s="21" t="n">
-        <v>31920.45</v>
+        <v>28728.45</v>
       </c>
       <c r="P119" s="21" t="n">
         <v>51072.48</v>
       </c>
       <c r="Q119" s="21" t="n">
-        <v>31920.45</v>
+        <v>28728.45</v>
       </c>
       <c r="R119" s="23" t="n">
-        <v>26250.16</v>
+        <v>23625.2</v>
       </c>
       <c r="S119" s="21" t="n">
         <v>0</v>
@@ -15776,7 +15768,7 @@
         <v>0</v>
       </c>
       <c r="Y119" s="21" t="n">
-        <v>1224</v>
+        <v>1428</v>
       </c>
       <c r="Z119" s="21" t="n">
         <v>7000</v>
@@ -15785,13 +15777,13 @@
         <v>6</v>
       </c>
       <c r="AB119" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC119" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD119" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE119" t="n">
         <v>16</v>
@@ -15800,10 +15792,10 @@
         <v>0</v>
       </c>
       <c r="AG119" s="21" t="n">
-        <v>1224</v>
+        <v>1428</v>
       </c>
       <c r="AH119" s="20" t="n">
-        <v>0.06390917378596066</v>
+        <v>0.06390917378596064</v>
       </c>
       <c r="AI119" t="inlineStr">
         <is>
@@ -15875,22 +15867,22 @@
         <v>16340.14</v>
       </c>
       <c r="N120" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O120" s="21" t="n">
-        <v>163401.15</v>
+        <v>147061.15</v>
       </c>
       <c r="P120" s="21" t="n">
         <v>261442.24</v>
       </c>
       <c r="Q120" s="21" t="n">
-        <v>163401.4</v>
+        <v>147061.26</v>
       </c>
       <c r="R120" s="23" t="n">
-        <v>134375</v>
+        <v>120937.5</v>
       </c>
       <c r="S120" s="21" t="n">
-        <v>-0.2500000000291038</v>
+        <v>-0.110000000015134</v>
       </c>
       <c r="T120" s="21" t="n">
         <v>0</v>
@@ -15908,7 +15900,7 @@
         <v>0</v>
       </c>
       <c r="Y120" s="21" t="n">
-        <v>9803</v>
+        <v>11437</v>
       </c>
       <c r="Z120" s="21" t="n">
         <v>43000</v>
@@ -15917,13 +15909,13 @@
         <v>5</v>
       </c>
       <c r="AB120" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AC120" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD120" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE120" t="n">
         <v>16</v>
@@ -15932,10 +15924,10 @@
         <v>0</v>
       </c>
       <c r="AG120" s="21" t="n">
-        <v>9803</v>
+        <v>11437</v>
       </c>
       <c r="AH120" s="20" t="n">
-        <v>0.09998894338318602</v>
+        <v>0.09999040050190162</v>
       </c>
       <c r="AI120" t="inlineStr">
         <is>
@@ -16142,37 +16134,37 @@
         <v>45981</v>
       </c>
       <c r="O122" s="21" t="n">
-        <v>58493.75</v>
+        <v>53167.75</v>
       </c>
       <c r="P122" s="21" t="n">
         <v>85120.8</v>
       </c>
       <c r="Q122" s="21" t="n">
-        <v>58493.75</v>
+        <v>53200.5</v>
       </c>
       <c r="R122" s="23" t="n">
         <v>43750</v>
       </c>
       <c r="S122" s="21" t="n">
-        <v>0</v>
+        <v>-32.75</v>
       </c>
       <c r="T122" s="21" t="n">
-        <v>4375</v>
+        <v>0</v>
       </c>
       <c r="U122" s="21" t="n">
         <v>0</v>
       </c>
       <c r="V122" s="21" t="n">
-        <v>4375</v>
+        <v>0</v>
       </c>
       <c r="W122" s="20" t="n">
-        <v>0.09090909090909091</v>
+        <v>0</v>
       </c>
       <c r="X122" s="21" t="n">
-        <v>43750</v>
+        <v>0</v>
       </c>
       <c r="Y122" s="21" t="n">
-        <v>1303</v>
+        <v>1563</v>
       </c>
       <c r="Z122" s="21" t="n">
         <v>11666.66666666667</v>
@@ -16193,13 +16185,13 @@
         <v>16</v>
       </c>
       <c r="AF122" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AG122" s="21" t="n">
-        <v>1303</v>
+        <v>1563</v>
       </c>
       <c r="AH122" s="20" t="n">
-        <v>0.04082041835446408</v>
+        <v>0.0489657052095375</v>
       </c>
       <c r="AI122" t="inlineStr">
         <is>
@@ -17063,22 +17055,22 @@
         <v>8284.07</v>
       </c>
       <c r="N129" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O129" s="21" t="n">
-        <v>91079.16</v>
+        <v>82786.16</v>
       </c>
       <c r="P129" s="21" t="n">
         <v>132545.12</v>
       </c>
       <c r="Q129" s="21" t="n">
-        <v>91124.76999999999</v>
+        <v>82840.7</v>
       </c>
       <c r="R129" s="23" t="n">
-        <v>74937.5</v>
+        <v>68125</v>
       </c>
       <c r="S129" s="21" t="n">
-        <v>-45.60999999998603</v>
+        <v>-54.5399999999936</v>
       </c>
       <c r="T129" s="21" t="n">
         <v>0</v>
@@ -17096,7 +17088,7 @@
         <v>0</v>
       </c>
       <c r="Y129" s="21" t="n">
-        <v>2210</v>
+        <v>2625</v>
       </c>
       <c r="Z129" s="21" t="n">
         <v>12111.11111111111</v>
@@ -17105,13 +17097,13 @@
         <v>9</v>
       </c>
       <c r="AB129" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC129" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AD129" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AE129" t="n">
         <v>16</v>
@@ -17120,10 +17112,10 @@
         <v>0</v>
       </c>
       <c r="AG129" s="21" t="n">
-        <v>2210</v>
+        <v>2625</v>
       </c>
       <c r="AH129" s="20" t="n">
-        <v>0.05335541587649549</v>
+        <v>0.05281220462888411</v>
       </c>
       <c r="AI129" t="inlineStr">
         <is>
@@ -17327,22 +17319,22 @@
         <v>8588.08</v>
       </c>
       <c r="N131" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O131" s="21" t="n">
-        <v>94461.21000000001</v>
+        <v>85872.21000000001</v>
       </c>
       <c r="P131" s="21" t="n">
         <v>137409.28</v>
       </c>
       <c r="Q131" s="21" t="n">
-        <v>94468.88</v>
+        <v>85880.8</v>
       </c>
       <c r="R131" s="23" t="n">
-        <v>77687.5</v>
+        <v>70625</v>
       </c>
       <c r="S131" s="21" t="n">
-        <v>-7.669999999998254</v>
+        <v>-8.589999999996508</v>
       </c>
       <c r="T131" s="21" t="n">
         <v>0</v>
@@ -17369,13 +17361,13 @@
         <v>8</v>
       </c>
       <c r="AB131" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC131" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AD131" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AE131" t="n">
         <v>16</v>
@@ -17387,7 +17379,7 @@
         <v>3403</v>
       </c>
       <c r="AH131" s="20" t="n">
-        <v>0.07924937820793472</v>
+        <v>0.06604114850661227</v>
       </c>
       <c r="AI131" t="inlineStr">
         <is>
@@ -17459,22 +17451,22 @@
         <v>8132.070000000001</v>
       </c>
       <c r="N132" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O132" s="21" t="n">
-        <v>89428.14</v>
+        <v>81291.14</v>
       </c>
       <c r="P132" s="21" t="n">
         <v>130113.12</v>
       </c>
       <c r="Q132" s="21" t="n">
-        <v>89452.77</v>
+        <v>81320.70000000001</v>
       </c>
       <c r="R132" s="23" t="n">
-        <v>73562.5</v>
+        <v>66875</v>
       </c>
       <c r="S132" s="21" t="n">
-        <v>-24.63000000000466</v>
+        <v>-29.56000000001222</v>
       </c>
       <c r="T132" s="21" t="n">
         <v>0</v>
@@ -17492,7 +17484,7 @@
         <v>0</v>
       </c>
       <c r="Y132" s="21" t="n">
-        <v>2070</v>
+        <v>2477</v>
       </c>
       <c r="Z132" s="21" t="n">
         <v>21400</v>
@@ -17501,13 +17493,13 @@
         <v>5</v>
       </c>
       <c r="AB132" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC132" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AD132" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AE132" t="n">
         <v>16</v>
@@ -17516,10 +17508,10 @@
         <v>0</v>
       </c>
       <c r="AG132" s="21" t="n">
-        <v>2070</v>
+        <v>2477</v>
       </c>
       <c r="AH132" s="20" t="n">
-        <v>0.05090954701570448</v>
+        <v>0.05076608210865539</v>
       </c>
       <c r="AI132" t="inlineStr">
         <is>
@@ -17726,7 +17718,7 @@
         <v>45980</v>
       </c>
       <c r="O134" s="21" t="n">
-        <v>125351.6</v>
+        <v>113941.6</v>
       </c>
       <c r="P134" s="21" t="n">
         <v>182401.6</v>
@@ -17735,10 +17727,10 @@
         <v>125401.1</v>
       </c>
       <c r="R134" s="23" t="n">
-        <v>103125</v>
+        <v>93750</v>
       </c>
       <c r="S134" s="21" t="n">
-        <v>-49.5</v>
+        <v>-11459.5</v>
       </c>
       <c r="T134" s="21" t="n">
         <v>0</v>
@@ -17756,7 +17748,7 @@
         <v>0</v>
       </c>
       <c r="Y134" s="21" t="n">
-        <v>2850</v>
+        <v>3420</v>
       </c>
       <c r="Z134" s="21" t="n">
         <v>15000</v>
@@ -17780,10 +17772,10 @@
         <v>0</v>
       </c>
       <c r="AG134" s="21" t="n">
-        <v>2850</v>
+        <v>3420</v>
       </c>
       <c r="AH134" s="20" t="n">
-        <v>0.04999956140735608</v>
+        <v>0.05999947368882729</v>
       </c>
       <c r="AI134" t="inlineStr">
         <is>
@@ -18386,7 +18378,7 @@
         <v>45980</v>
       </c>
       <c r="O139" s="21" t="n">
-        <v>56539.62</v>
+        <v>51827.58</v>
       </c>
       <c r="P139" s="21" t="n">
         <v>75392.64</v>
@@ -18395,10 +18387,10 @@
         <v>56544.48</v>
       </c>
       <c r="R139" s="23" t="n">
-        <v>46500</v>
+        <v>42625</v>
       </c>
       <c r="S139" s="21" t="n">
-        <v>-4.859999999993306</v>
+        <v>-4716.899999999994</v>
       </c>
       <c r="T139" s="21" t="n">
         <v>0</v>
@@ -18416,7 +18408,7 @@
         <v>0</v>
       </c>
       <c r="Y139" s="21" t="n">
-        <v>1878.96</v>
+        <v>2349.92</v>
       </c>
       <c r="Z139" s="21" t="n">
         <v>12400</v>
@@ -18440,10 +18432,10 @@
         <v>0</v>
       </c>
       <c r="AG139" s="21" t="n">
-        <v>1878.96</v>
+        <v>2349.92</v>
       </c>
       <c r="AH139" s="20" t="n">
-        <v>0.09968930654238929</v>
+        <v>0.1246763609816555</v>
       </c>
       <c r="AI139" t="inlineStr">
         <is>
@@ -18518,19 +18510,19 @@
         <v>45985</v>
       </c>
       <c r="O140" s="21" t="n">
-        <v>47424.52</v>
+        <v>43472.22</v>
       </c>
       <c r="P140" s="21" t="n">
         <v>63232.48</v>
       </c>
       <c r="Q140" s="21" t="n">
-        <v>47424.52</v>
+        <v>43472.33</v>
       </c>
       <c r="R140" s="23" t="n">
-        <v>39000.12</v>
+        <v>35750</v>
       </c>
       <c r="S140" s="21" t="n">
-        <v>0</v>
+        <v>-0.1100000000005821</v>
       </c>
       <c r="T140" s="21" t="n">
         <v>0</v>
@@ -18782,19 +18774,19 @@
         <v>45985</v>
       </c>
       <c r="O142" s="21" t="n">
-        <v>144095.69</v>
+        <v>132086.69</v>
       </c>
       <c r="P142" s="21" t="n">
         <v>192129.76</v>
       </c>
       <c r="Q142" s="21" t="n">
-        <v>144095.69</v>
+        <v>132089.21</v>
       </c>
       <c r="R142" s="23" t="n">
-        <v>118500</v>
+        <v>108625</v>
       </c>
       <c r="S142" s="21" t="n">
-        <v>0</v>
+        <v>-2.520000000018626</v>
       </c>
       <c r="T142" s="21" t="n">
         <v>0</v>
@@ -18911,19 +18903,19 @@
         <v>11400.1</v>
       </c>
       <c r="N143" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O143" s="21" t="n">
-        <v>136801.2</v>
+        <v>125401.1</v>
       </c>
       <c r="P143" s="21" t="n">
         <v>182401.6</v>
       </c>
       <c r="Q143" s="21" t="n">
-        <v>136801.2</v>
+        <v>125401.1</v>
       </c>
       <c r="R143" s="23" t="n">
-        <v>112500.02</v>
+        <v>103125</v>
       </c>
       <c r="S143" s="21" t="n">
         <v>0</v>
@@ -18944,7 +18936,7 @@
         <v>0</v>
       </c>
       <c r="Y143" s="21" t="n">
-        <v>3287.599999999999</v>
+        <v>4109.499999999998</v>
       </c>
       <c r="Z143" s="21" t="n">
         <v>25000</v>
@@ -18953,13 +18945,13 @@
         <v>6</v>
       </c>
       <c r="AB143" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC143" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD143" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AE143" t="n">
         <v>16</v>
@@ -18968,7 +18960,7 @@
         <v>0</v>
       </c>
       <c r="AG143" s="21" t="n">
-        <v>3287.599999999999</v>
+        <v>4109.499999999998</v>
       </c>
       <c r="AH143" s="20" t="n">
         <v>0.07209585880825603</v>
@@ -19046,7 +19038,7 @@
         <v>45980</v>
       </c>
       <c r="O144" s="21" t="n">
-        <v>61996.73</v>
+        <v>56823.73</v>
       </c>
       <c r="P144" s="21" t="n">
         <v>82688.8</v>
@@ -19055,10 +19047,10 @@
         <v>62016.60000000001</v>
       </c>
       <c r="R144" s="23" t="n">
-        <v>51000</v>
+        <v>46750</v>
       </c>
       <c r="S144" s="21" t="n">
-        <v>-19.87000000000262</v>
+        <v>-5192.870000000003</v>
       </c>
       <c r="T144" s="21" t="n">
         <v>0</v>
@@ -19076,7 +19068,7 @@
         <v>0</v>
       </c>
       <c r="Y144" s="21" t="n">
-        <v>1175</v>
+        <v>1469</v>
       </c>
       <c r="Z144" s="21" t="n">
         <v>11333.33333333333</v>
@@ -19100,10 +19092,10 @@
         <v>0</v>
       </c>
       <c r="AG144" s="21" t="n">
-        <v>1175</v>
+        <v>1469</v>
       </c>
       <c r="AH144" s="20" t="n">
-        <v>0.05683962035971014</v>
+        <v>0.07106161898588442</v>
       </c>
       <c r="AI144" t="inlineStr">
         <is>
@@ -19178,34 +19170,34 @@
         <v>45982</v>
       </c>
       <c r="O145" s="21" t="n">
-        <v>57304.47</v>
+        <v>52896.42</v>
       </c>
       <c r="P145" s="21" t="n">
         <v>70528.64</v>
       </c>
       <c r="Q145" s="21" t="n">
-        <v>57304.47</v>
+        <v>52896.48</v>
       </c>
       <c r="R145" s="23" t="n">
         <v>43500</v>
       </c>
       <c r="S145" s="21" t="n">
-        <v>0</v>
+        <v>-0.05999999999767169</v>
       </c>
       <c r="T145" s="21" t="n">
-        <v>3625</v>
+        <v>0</v>
       </c>
       <c r="U145" s="21" t="n">
         <v>0</v>
       </c>
       <c r="V145" s="21" t="n">
-        <v>3625</v>
+        <v>0</v>
       </c>
       <c r="W145" s="20" t="n">
-        <v>0.07692307692307693</v>
+        <v>0</v>
       </c>
       <c r="X145" s="21" t="n">
-        <v>43500</v>
+        <v>0</v>
       </c>
       <c r="Y145" s="21" t="n">
         <v>1763.799999999999</v>
@@ -19229,7 +19221,7 @@
         <v>16</v>
       </c>
       <c r="AF145" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG145" s="21" t="n">
         <v>1763.799999999999</v>
@@ -19970,7 +19962,7 @@
         <v>45980</v>
       </c>
       <c r="O151" s="21" t="n">
-        <v>49224.58</v>
+        <v>45114.58</v>
       </c>
       <c r="P151" s="21" t="n">
         <v>65664.64</v>
@@ -19979,10 +19971,10 @@
         <v>49248.48</v>
       </c>
       <c r="R151" s="23" t="n">
-        <v>40500</v>
+        <v>37125</v>
       </c>
       <c r="S151" s="21" t="n">
-        <v>-23.89999999999418</v>
+        <v>-4133.899999999994</v>
       </c>
       <c r="T151" s="21" t="n">
         <v>0</v>
@@ -20000,7 +19992,7 @@
         <v>0</v>
       </c>
       <c r="Y151" s="21" t="n">
-        <v>912</v>
+        <v>1140</v>
       </c>
       <c r="Z151" s="21" t="n">
         <v>9000</v>
@@ -20024,10 +20016,10 @@
         <v>0</v>
       </c>
       <c r="AG151" s="21" t="n">
-        <v>912</v>
+        <v>1140</v>
       </c>
       <c r="AH151" s="20" t="n">
-        <v>0.05555501408368339</v>
+        <v>0.06944376760460425</v>
       </c>
       <c r="AI151" t="inlineStr">
         <is>
@@ -21026,19 +21018,19 @@
         <v>45985</v>
       </c>
       <c r="O159" s="21" t="n">
-        <v>83965.91</v>
+        <v>77500.91</v>
       </c>
       <c r="P159" s="21" t="n">
         <v>103360.96</v>
       </c>
       <c r="Q159" s="21" t="n">
-        <v>83965.91</v>
+        <v>77520.72</v>
       </c>
       <c r="R159" s="23" t="n">
-        <v>69062.5</v>
+        <v>63750</v>
       </c>
       <c r="S159" s="21" t="n">
-        <v>0</v>
+        <v>-19.80999999999767</v>
       </c>
       <c r="T159" s="21" t="n">
         <v>0</v>
@@ -21287,22 +21279,22 @@
         <v>9386.08</v>
       </c>
       <c r="N161" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O161" s="21" t="n">
-        <v>122018.32</v>
+        <v>112632.32</v>
       </c>
       <c r="P161" s="21" t="n">
         <v>150177.28</v>
       </c>
       <c r="Q161" s="21" t="n">
-        <v>122019.04</v>
+        <v>112632.96</v>
       </c>
       <c r="R161" s="23" t="n">
-        <v>100343.75</v>
+        <v>92625</v>
       </c>
       <c r="S161" s="21" t="n">
-        <v>-0.7200000000011642</v>
+        <v>-0.639999999984866</v>
       </c>
       <c r="T161" s="21" t="n">
         <v>0</v>
@@ -21320,7 +21312,7 @@
         <v>0</v>
       </c>
       <c r="Y161" s="21" t="n">
-        <v>1409</v>
+        <v>1879</v>
       </c>
       <c r="Z161" s="21" t="n">
         <v>20583.33333333333</v>
@@ -21329,13 +21321,13 @@
         <v>6</v>
       </c>
       <c r="AB161" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC161" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD161" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AE161" t="n">
         <v>16</v>
@@ -21344,10 +21336,10 @@
         <v>0</v>
       </c>
       <c r="AG161" s="21" t="n">
-        <v>1409</v>
+        <v>1879</v>
       </c>
       <c r="AH161" s="20" t="n">
-        <v>0.05003863877856003</v>
+        <v>0.05004751717436885</v>
       </c>
       <c r="AI161" t="inlineStr">
         <is>
@@ -21419,22 +21411,22 @@
         <v>11780.1</v>
       </c>
       <c r="N162" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O162" s="21" t="n">
-        <v>153120.65</v>
+        <v>141333.65</v>
       </c>
       <c r="P162" s="21" t="n">
         <v>188481.6</v>
       </c>
       <c r="Q162" s="21" t="n">
-        <v>153141.3</v>
+        <v>141361.2</v>
       </c>
       <c r="R162" s="23" t="n">
-        <v>125937.5</v>
+        <v>116250</v>
       </c>
       <c r="S162" s="21" t="n">
-        <v>-20.64999999999418</v>
+        <v>-27.55000000001746</v>
       </c>
       <c r="T162" s="21" t="n">
         <v>0</v>
@@ -21452,7 +21444,7 @@
         <v>0</v>
       </c>
       <c r="Y162" s="21" t="n">
-        <v>2526</v>
+        <v>3368</v>
       </c>
       <c r="Z162" s="21" t="n">
         <v>22142.85714285714</v>
@@ -21461,13 +21453,13 @@
         <v>7</v>
       </c>
       <c r="AB162" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC162" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD162" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AE162" t="n">
         <v>16</v>
@@ -21476,7 +21468,7 @@
         <v>0</v>
       </c>
       <c r="AG162" s="21" t="n">
-        <v>2526</v>
+        <v>3368</v>
       </c>
       <c r="AH162" s="20" t="n">
         <v>0.07147647303503366</v>
@@ -21551,22 +21543,22 @@
         <v>10184.09</v>
       </c>
       <c r="N163" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O163" s="21" t="n">
-        <v>132393.34</v>
+        <v>122208.34</v>
       </c>
       <c r="P163" s="21" t="n">
         <v>162945.44</v>
       </c>
       <c r="Q163" s="21" t="n">
-        <v>132393.34</v>
+        <v>122209.08</v>
       </c>
       <c r="R163" s="23" t="n">
-        <v>108875.18</v>
+        <v>100500</v>
       </c>
       <c r="S163" s="21" t="n">
-        <v>0</v>
+        <v>-0.7400000000052387</v>
       </c>
       <c r="T163" s="21" t="n">
         <v>0</v>
@@ -21584,7 +21576,7 @@
         <v>0</v>
       </c>
       <c r="Y163" s="21" t="n">
-        <v>2911.91</v>
+        <v>3785.91</v>
       </c>
       <c r="Z163" s="21" t="n">
         <v>26800</v>
@@ -21593,13 +21585,13 @@
         <v>5</v>
       </c>
       <c r="AB163" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC163" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD163" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AE163" t="n">
         <v>16</v>
@@ -21608,10 +21600,10 @@
         <v>0</v>
       </c>
       <c r="AG163" s="21" t="n">
-        <v>2911.91</v>
+        <v>3785.91</v>
       </c>
       <c r="AH163" s="20" t="n">
-        <v>0.09530912105712602</v>
+        <v>0.09293687506689355</v>
       </c>
       <c r="AI163" t="inlineStr">
         <is>
@@ -21683,19 +21675,19 @@
         <v>5624.05</v>
       </c>
       <c r="N164" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O164" s="21" t="n">
-        <v>73112.79000000001</v>
+        <v>67488.79000000001</v>
       </c>
       <c r="P164" s="21" t="n">
         <v>89984.8</v>
       </c>
       <c r="Q164" s="21" t="n">
-        <v>73112.79000000001</v>
+        <v>67488.79000000001</v>
       </c>
       <c r="R164" s="23" t="n">
-        <v>60125.15</v>
+        <v>55500.19</v>
       </c>
       <c r="S164" s="21" t="n">
         <v>0</v>
@@ -21716,7 +21708,7 @@
         <v>0</v>
       </c>
       <c r="Y164" s="21" t="n">
-        <v>846</v>
+        <v>1128</v>
       </c>
       <c r="Z164" s="21" t="n">
         <v>14800</v>
@@ -21725,13 +21717,13 @@
         <v>5</v>
       </c>
       <c r="AB164" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC164" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD164" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AE164" t="n">
         <v>16</v>
@@ -21740,7 +21732,7 @@
         <v>0</v>
       </c>
       <c r="AG164" s="21" t="n">
-        <v>846</v>
+        <v>1128</v>
       </c>
       <c r="AH164" s="20" t="n">
         <v>0.05014180172651381</v>
@@ -21818,7 +21810,7 @@
         <v>45980</v>
       </c>
       <c r="O165" s="21" t="n">
-        <v>51365.55</v>
+        <v>47409.55</v>
       </c>
       <c r="P165" s="21" t="n">
         <v>63232.48</v>
@@ -21827,10 +21819,10 @@
         <v>51376.39</v>
       </c>
       <c r="R165" s="23" t="n">
-        <v>42250</v>
+        <v>39000</v>
       </c>
       <c r="S165" s="21" t="n">
-        <v>-10.83999999999651</v>
+        <v>-3966.839999999997</v>
       </c>
       <c r="T165" s="21" t="n">
         <v>0</v>
@@ -21848,7 +21840,7 @@
         <v>0</v>
       </c>
       <c r="Y165" s="21" t="n">
-        <v>591</v>
+        <v>789</v>
       </c>
       <c r="Z165" s="21" t="n">
         <v>10400</v>
@@ -21872,10 +21864,10 @@
         <v>0</v>
       </c>
       <c r="AG165" s="21" t="n">
-        <v>591</v>
+        <v>789</v>
       </c>
       <c r="AH165" s="20" t="n">
-        <v>0.04984779973836231</v>
+        <v>0.06654807782329587</v>
       </c>
       <c r="AI165" t="inlineStr">
         <is>
@@ -22947,7 +22939,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>ADRIANA ALEJALDRE GUZMAN</t>
+          <t>Garcia Herrera Jonathan</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -23138,37 +23130,37 @@
         <v>45982</v>
       </c>
       <c r="O175" s="21" t="n">
-        <v>266171.69</v>
+        <v>248976.52</v>
       </c>
       <c r="P175" s="21" t="n">
         <v>306434.72</v>
       </c>
       <c r="Q175" s="21" t="n">
-        <v>266171.69</v>
+        <v>248978.21</v>
       </c>
       <c r="R175" s="23" t="n">
         <v>204750</v>
       </c>
       <c r="S175" s="21" t="n">
-        <v>0</v>
+        <v>-1.690000000002328</v>
       </c>
       <c r="T175" s="21" t="n">
-        <v>15750</v>
+        <v>0</v>
       </c>
       <c r="U175" s="21" t="n">
         <v>0</v>
       </c>
       <c r="V175" s="21" t="n">
-        <v>15750</v>
+        <v>0</v>
       </c>
       <c r="W175" s="20" t="n">
-        <v>0.07142857142857144</v>
+        <v>0</v>
       </c>
       <c r="X175" s="21" t="n">
-        <v>204750</v>
+        <v>0</v>
       </c>
       <c r="Y175" s="21" t="n">
-        <v>20211</v>
+        <v>3015.830000000002</v>
       </c>
       <c r="Z175" s="21" t="n">
         <v>50400</v>
@@ -23189,13 +23181,13 @@
         <v>16</v>
       </c>
       <c r="AF175" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AG175" s="21" t="n">
-        <v>20211</v>
+        <v>3015.830000000002</v>
       </c>
       <c r="AH175" s="20" t="n">
-        <v>0.351761706375831</v>
+        <v>0.05248891726977502</v>
       </c>
       <c r="AI175" t="inlineStr">
         <is>
@@ -23411,25 +23403,25 @@
         <v>61710.62</v>
       </c>
       <c r="R177" s="23" t="n">
-        <v>50750</v>
+        <v>47125</v>
       </c>
       <c r="S177" s="21" t="n">
         <v>0</v>
       </c>
       <c r="T177" s="21" t="n">
-        <v>0</v>
+        <v>3625</v>
       </c>
       <c r="U177" s="21" t="n">
         <v>0</v>
       </c>
       <c r="V177" s="21" t="n">
-        <v>0</v>
+        <v>3625</v>
       </c>
       <c r="W177" s="20" t="n">
-        <v>0</v>
+        <v>0.07142857142857144</v>
       </c>
       <c r="X177" s="21" t="n">
-        <v>0</v>
+        <v>47125</v>
       </c>
       <c r="Y177" s="21" t="n">
         <v>767</v>
@@ -23534,19 +23526,19 @@
         <v>45985</v>
       </c>
       <c r="O178" s="21" t="n">
-        <v>72350.73</v>
+        <v>67181.73</v>
       </c>
       <c r="P178" s="21" t="n">
         <v>82688.8</v>
       </c>
       <c r="Q178" s="21" t="n">
-        <v>72350.73</v>
+        <v>67184.64999999999</v>
       </c>
       <c r="R178" s="23" t="n">
-        <v>59500</v>
+        <v>55250</v>
       </c>
       <c r="S178" s="21" t="n">
-        <v>0</v>
+        <v>-2.919999999998254</v>
       </c>
       <c r="T178" s="21" t="n">
         <v>0</v>
@@ -23663,22 +23655,22 @@
         <v>38760.34</v>
       </c>
       <c r="N179" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O179" s="21" t="n">
-        <v>542643.4400000001</v>
+        <v>503882.44</v>
       </c>
       <c r="P179" s="21" t="n">
         <v>620165.4400000001</v>
       </c>
       <c r="Q179" s="21" t="n">
-        <v>542644.76</v>
+        <v>503884.42</v>
       </c>
       <c r="R179" s="23" t="n">
-        <v>446250</v>
+        <v>414375</v>
       </c>
       <c r="S179" s="21" t="n">
-        <v>-1.319999999948777</v>
+        <v>-1.980000000039581</v>
       </c>
       <c r="T179" s="21" t="n">
         <v>0</v>
@@ -23705,13 +23697,13 @@
         <v>6</v>
       </c>
       <c r="AB179" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC179" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD179" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AE179" t="n">
         <v>16</v>
@@ -23798,7 +23790,7 @@
         <v>45980</v>
       </c>
       <c r="O180" s="21" t="n">
-        <v>57454.58</v>
+        <v>53349.58</v>
       </c>
       <c r="P180" s="21" t="n">
         <v>65664.64</v>
@@ -23807,10 +23799,10 @@
         <v>57456.56</v>
       </c>
       <c r="R180" s="23" t="n">
-        <v>47250</v>
+        <v>43875</v>
       </c>
       <c r="S180" s="21" t="n">
-        <v>-1.979999999995925</v>
+        <v>-4106.979999999996</v>
       </c>
       <c r="T180" s="21" t="n">
         <v>0</v>
@@ -23828,7 +23820,7 @@
         <v>0</v>
       </c>
       <c r="Y180" s="21" t="n">
-        <v>803</v>
+        <v>1190</v>
       </c>
       <c r="Z180" s="21" t="n">
         <v>10800</v>
@@ -23852,10 +23844,10 @@
         <v>0</v>
       </c>
       <c r="AG180" s="21" t="n">
-        <v>803</v>
+        <v>1190</v>
       </c>
       <c r="AH180" s="20" t="n">
-        <v>0.09783043050262669</v>
+        <v>0.1449790937710159</v>
       </c>
       <c r="AI180" t="inlineStr">
         <is>
@@ -24194,7 +24186,7 @@
         <v>45980</v>
       </c>
       <c r="O183" s="21" t="n">
-        <v>146831.47</v>
+        <v>136342.47</v>
       </c>
       <c r="P183" s="21" t="n">
         <v>167809.44</v>
@@ -24203,10 +24195,10 @@
         <v>146833.26</v>
       </c>
       <c r="R183" s="23" t="n">
-        <v>120750</v>
+        <v>112125</v>
       </c>
       <c r="S183" s="21" t="n">
-        <v>-1.790000000008149</v>
+        <v>-10490.79000000001</v>
       </c>
       <c r="T183" s="21" t="n">
         <v>0</v>
@@ -24224,7 +24216,7 @@
         <v>0</v>
       </c>
       <c r="Y183" s="21" t="n">
-        <v>1122</v>
+        <v>1683</v>
       </c>
       <c r="Z183" s="21" t="n">
         <v>17250</v>
@@ -24248,10 +24240,10 @@
         <v>0</v>
       </c>
       <c r="AG183" s="21" t="n">
-        <v>1122</v>
+        <v>1683</v>
       </c>
       <c r="AH183" s="20" t="n">
-        <v>0.05348924351335658</v>
+        <v>0.08023386527003487</v>
       </c>
       <c r="AI183" t="inlineStr">
         <is>
@@ -24326,19 +24318,19 @@
         <v>45980</v>
       </c>
       <c r="O184" s="21" t="n">
-        <v>137257.38</v>
+        <v>127453.38</v>
       </c>
       <c r="P184" s="21" t="n">
         <v>156865.44</v>
       </c>
       <c r="Q184" s="21" t="n">
-        <v>137257.38</v>
+        <v>137257.26</v>
       </c>
       <c r="R184" s="23" t="n">
-        <v>112875.16</v>
+        <v>104812.76</v>
       </c>
       <c r="S184" s="21" t="n">
-        <v>0</v>
+        <v>-9803.880000000005</v>
       </c>
       <c r="T184" s="21" t="n">
         <v>0</v>
@@ -24356,7 +24348,7 @@
         <v>0</v>
       </c>
       <c r="Y184" s="21" t="n">
-        <v>982</v>
+        <v>1473</v>
       </c>
       <c r="Z184" s="21" t="n">
         <v>21500</v>
@@ -24380,10 +24372,10 @@
         <v>0</v>
       </c>
       <c r="AG184" s="21" t="n">
-        <v>982</v>
+        <v>1473</v>
       </c>
       <c r="AH184" s="20" t="n">
-        <v>0.05008113960602157</v>
+        <v>0.07512170940903236</v>
       </c>
       <c r="AI184" t="inlineStr">
         <is>
@@ -24854,7 +24846,7 @@
         <v>45980</v>
       </c>
       <c r="O188" s="21" t="n">
-        <v>204288.05</v>
+        <v>189695.05</v>
       </c>
       <c r="P188" s="21" t="n">
         <v>233474.08</v>
@@ -24863,10 +24855,10 @@
         <v>204289.82</v>
       </c>
       <c r="R188" s="23" t="n">
-        <v>168000</v>
+        <v>156000</v>
       </c>
       <c r="S188" s="21" t="n">
-        <v>-1.769999999989523</v>
+        <v>-14594.76999999999</v>
       </c>
       <c r="T188" s="21" t="n">
         <v>0</v>
@@ -24884,7 +24876,7 @@
         <v>0</v>
       </c>
       <c r="Y188" s="21" t="n">
-        <v>1458</v>
+        <v>2187</v>
       </c>
       <c r="Z188" s="21" t="n">
         <v>32000</v>
@@ -24908,10 +24900,10 @@
         <v>0</v>
       </c>
       <c r="AG188" s="21" t="n">
-        <v>1458</v>
+        <v>2187</v>
       </c>
       <c r="AH188" s="20" t="n">
-        <v>0.04995843649967482</v>
+        <v>0.07493765474951224</v>
       </c>
       <c r="AI188" t="inlineStr">
         <is>
@@ -25514,7 +25506,7 @@
         <v>45982</v>
       </c>
       <c r="O193" s="21" t="n">
-        <v>93632.34</v>
+        <v>86943.74000000001</v>
       </c>
       <c r="P193" s="21" t="n">
         <v>107008.96</v>
@@ -25523,10 +25515,10 @@
         <v>93632.84000000001</v>
       </c>
       <c r="R193" s="23" t="n">
-        <v>77000</v>
+        <v>71500</v>
       </c>
       <c r="S193" s="21" t="n">
-        <v>-0.5000000000145519</v>
+        <v>-6689.100000000006</v>
       </c>
       <c r="T193" s="21" t="n">
         <v>0</v>
@@ -27039,7 +27031,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>IRVIN URIEL MORA VELAZCO</t>
+          <t>Olivares Morales Josue Edgar</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -27230,19 +27222,19 @@
         <v>45980</v>
       </c>
       <c r="O206" s="21" t="n">
-        <v>88920.78</v>
+        <v>82992.73</v>
       </c>
       <c r="P206" s="21" t="n">
         <v>94848.8</v>
       </c>
       <c r="Q206" s="21" t="n">
-        <v>88920.78</v>
+        <v>88920.75</v>
       </c>
       <c r="R206" s="23" t="n">
-        <v>73125.00999999999</v>
+        <v>68250</v>
       </c>
       <c r="S206" s="21" t="n">
-        <v>0</v>
+        <v>-5928.020000000004</v>
       </c>
       <c r="T206" s="21" t="n">
         <v>0</v>
@@ -27260,7 +27252,7 @@
         <v>0</v>
       </c>
       <c r="Y206" s="21" t="n">
-        <v>154.9499999999998</v>
+        <v>309.8999999999996</v>
       </c>
       <c r="Z206" s="21" t="n">
         <v>15600</v>
@@ -27284,10 +27276,10 @@
         <v>0</v>
       </c>
       <c r="AG206" s="21" t="n">
-        <v>154.9499999999998</v>
+        <v>309.8999999999996</v>
       </c>
       <c r="AH206" s="20" t="n">
-        <v>0.02613844350165734</v>
+        <v>0.05227688700331469</v>
       </c>
       <c r="AI206" t="inlineStr">
         <is>
@@ -28547,22 +28539,22 @@
         <v>16492.14</v>
       </c>
       <c r="N216" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O216" s="21" t="n">
-        <v>263874.31</v>
+        <v>246557.31</v>
       </c>
       <c r="P216" s="21" t="n">
         <v>263874.24</v>
       </c>
       <c r="Q216" s="21" t="n">
-        <v>263874.31</v>
+        <v>247382.1</v>
       </c>
       <c r="R216" s="23" t="n">
-        <v>217000</v>
+        <v>203437.5</v>
       </c>
       <c r="S216" s="21" t="n">
-        <v>0</v>
+        <v>-824.789999999979</v>
       </c>
       <c r="T216" s="21" t="n">
         <v>0</v>
@@ -28589,13 +28581,13 @@
         <v>12</v>
       </c>
       <c r="AB216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC216" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD216" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AE216" t="n">
         <v>16</v>
@@ -28679,19 +28671,19 @@
         <v>7068.06</v>
       </c>
       <c r="N217" s="22" t="n">
-        <v>45979</v>
+        <v>45986</v>
       </c>
       <c r="O217" s="21" t="n">
-        <v>113088.99</v>
+        <v>106020.93</v>
       </c>
       <c r="P217" s="21" t="n">
         <v>113088.96</v>
       </c>
       <c r="Q217" s="21" t="n">
-        <v>113088.99</v>
+        <v>106020.93</v>
       </c>
       <c r="R217" s="23" t="n">
-        <v>93000</v>
+        <v>87187.5</v>
       </c>
       <c r="S217" s="21" t="n">
         <v>0</v>
@@ -28712,7 +28704,7 @@
         <v>0</v>
       </c>
       <c r="Y217" s="21" t="n">
-        <v>0</v>
+        <v>780.9399999999996</v>
       </c>
       <c r="Z217" s="21" t="n">
         <v>18600</v>
@@ -28721,13 +28713,13 @@
         <v>5</v>
       </c>
       <c r="AB217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC217" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD217" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AE217" t="n">
         <v>16</v>
@@ -28736,10 +28728,10 @@
         <v>0</v>
       </c>
       <c r="AG217" s="21" t="n">
-        <v>0</v>
+        <v>780.9399999999996</v>
       </c>
       <c r="AH217" s="20" t="n">
-        <v>0</v>
+        <v>0.110488592343585</v>
       </c>
       <c r="AI217" t="inlineStr">
         <is>
@@ -28781,6 +28773,11 @@
       <c r="F218" s="21" t="n">
         <v>192000</v>
       </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>MIGRADO</t>
+        </is>
+      </c>
       <c r="H218" s="22" t="n">
         <v>45974</v>
       </c>
@@ -29040,6 +29037,11 @@
       <c r="F220" s="21" t="n">
         <v>207000</v>
       </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>MIGRADO</t>
+        </is>
+      </c>
       <c r="H220" s="22" t="n">
         <v>45975</v>
       </c>
@@ -29200,19 +29202,19 @@
         <v>45980</v>
       </c>
       <c r="O221" s="21" t="n">
-        <v>97280.85000000001</v>
+        <v>91200.85000000001</v>
       </c>
       <c r="P221" s="21" t="n">
         <v>97280.8</v>
       </c>
       <c r="Q221" s="21" t="n">
-        <v>97280.85000000001</v>
+        <v>97280.8</v>
       </c>
       <c r="R221" s="23" t="n">
-        <v>80000</v>
+        <v>75000.06</v>
       </c>
       <c r="S221" s="21" t="n">
-        <v>0</v>
+        <v>-6079.949999999997</v>
       </c>
       <c r="T221" s="21" t="n">
         <v>0</v>
@@ -29230,7 +29232,7 @@
         <v>0</v>
       </c>
       <c r="Y221" s="21" t="n">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="Z221" s="21" t="n">
         <v>13333.33333333333</v>
@@ -29254,7 +29256,7 @@
         <v>0</v>
       </c>
       <c r="AG221" s="21" t="n">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="AH221" s="20" t="n">
         <v>0</v>
@@ -29431,6 +29433,11 @@
       <c r="F223" s="21" t="n">
         <v>181000</v>
       </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>MIGRADO</t>
+        </is>
+      </c>
       <c r="H223" s="22" t="n">
         <v>45975</v>
       </c>
@@ -29664,7 +29671,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>JUAN EDMIUNDO LUNA AGUILLON</t>
+          <t>JUAN EDMUNDO LUNA AGUILLON</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -30456,63 +30463,195 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
+          <t>IRVIN URIEL MORA VELAZCO</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Cuautle Pacheco Jheimy</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>000246</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>LA CIMA DEL EXITO</t>
+        </is>
+      </c>
+      <c r="E231" s="16" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+      <c r="F231" s="21" t="n">
+        <v>61000</v>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>MIGRADO</t>
+        </is>
+      </c>
+      <c r="H231" s="22" t="n">
+        <v>45979</v>
+      </c>
+      <c r="I231" t="n">
+        <v>16</v>
+      </c>
+      <c r="J231" t="inlineStr">
+        <is>
+          <t>Martes</t>
+        </is>
+      </c>
+      <c r="K231" t="inlineStr">
+        <is>
+          <t>10:00</t>
+        </is>
+      </c>
+      <c r="L231" t="inlineStr">
+        <is>
+          <t>Semanal</t>
+        </is>
+      </c>
+      <c r="M231" s="21" t="n">
+        <v>4636.04</v>
+      </c>
+      <c r="N231" s="22" t="n">
+        <v>45986</v>
+      </c>
+      <c r="O231" s="21" t="n">
+        <v>74176.65000000001</v>
+      </c>
+      <c r="P231" s="21" t="n">
+        <v>74176.64</v>
+      </c>
+      <c r="Q231" s="21" t="n">
+        <v>74176.65000000001</v>
+      </c>
+      <c r="R231" s="23" t="n">
+        <v>61000</v>
+      </c>
+      <c r="S231" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T231" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U231" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V231" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W231" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="X231" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y231" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z231" s="21" t="n">
+        <v>12200</v>
+      </c>
+      <c r="AA231" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB231" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC231" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD231" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE231" t="n">
+        <v>16</v>
+      </c>
+      <c r="AF231" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG231" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH231" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI231" t="inlineStr">
+        <is>
+          <t>Vigente</t>
+        </is>
+      </c>
+      <c r="AJ231" t="inlineStr">
+        <is>
+          <t>000024601</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="F231">
-        <f>SUBTOTAL(9,F$7:F$230)</f>
+      <c r="F232">
+        <f>SUBTOTAL(9,F$7:F$231)</f>
         <v/>
       </c>
-      <c r="M231">
-        <f>SUBTOTAL(9,M$7:M$230)</f>
+      <c r="M232">
+        <f>SUBTOTAL(9,M$7:M$231)</f>
         <v/>
       </c>
-      <c r="O231">
-        <f>SUBTOTAL(9,O$7:O$230)</f>
+      <c r="O232">
+        <f>SUBTOTAL(9,O$7:O$231)</f>
         <v/>
       </c>
-      <c r="P231">
-        <f>SUBTOTAL(9,P$7:P$230)</f>
+      <c r="P232">
+        <f>SUBTOTAL(9,P$7:P$231)</f>
         <v/>
       </c>
-      <c r="Q231">
-        <f>SUBTOTAL(9,Q$7:Q$230)</f>
+      <c r="Q232">
+        <f>SUBTOTAL(9,Q$7:Q$231)</f>
         <v/>
       </c>
-      <c r="R231" s="23">
-        <f>SUBTOTAL(9,R$7:R$230)</f>
+      <c r="R232" s="23">
+        <f>SUBTOTAL(9,R$7:R$231)</f>
         <v/>
       </c>
-      <c r="S231">
-        <f>SUBTOTAL(9,S$7:S$230)</f>
+      <c r="S232">
+        <f>SUBTOTAL(9,S$7:S$231)</f>
         <v/>
       </c>
-      <c r="T231">
-        <f>SUBTOTAL(9,T$7:T$230)</f>
+      <c r="T232">
+        <f>SUBTOTAL(9,T$7:T$231)</f>
         <v/>
       </c>
-      <c r="U231">
-        <f>SUBTOTAL(9,U$7:U$230)</f>
+      <c r="U232">
+        <f>SUBTOTAL(9,U$7:U$231)</f>
         <v/>
       </c>
-      <c r="V231">
-        <f>SUBTOTAL(9,V$7:V$230)</f>
+      <c r="V232">
+        <f>SUBTOTAL(9,V$7:V$231)</f>
         <v/>
       </c>
-      <c r="X231">
-        <f>SUBTOTAL(9,X$7:X$230)</f>
+      <c r="X232">
+        <f>SUBTOTAL(9,X$7:X$231)</f>
         <v/>
       </c>
-      <c r="Y231">
-        <f>SUBTOTAL(9,Y$7:Y$230)</f>
+      <c r="Y232">
+        <f>SUBTOTAL(9,Y$7:Y$231)</f>
         <v/>
       </c>
-      <c r="Z231">
-        <f>SUBTOTAL(9,Z$7:Z$230)</f>
+      <c r="Z232">
+        <f>SUBTOTAL(9,Z$7:Z$231)</f>
         <v/>
       </c>
-      <c r="AG231">
-        <f>SUBTOTAL(9,AG$7:AG$230)</f>
+      <c r="AG232">
+        <f>SUBTOTAL(9,AG$7:AG$231)</f>
         <v/>
       </c>
     </row>
@@ -30531,7 +30670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
@@ -30653,7 +30792,7 @@
       </c>
       <c r="B7" s="16" t="inlineStr">
         <is>
-          <t>Ponce Galindo Alicia Berenice</t>
+          <t>Contreras Martinez Jose Luis</t>
         </is>
       </c>
       <c r="C7" s="16" t="inlineStr">
@@ -30675,49 +30814,49 @@
         <v>122000</v>
       </c>
       <c r="G7" s="26" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" s="21" t="n">
         <v>9272.08</v>
       </c>
       <c r="I7" s="21" t="n">
-        <v>28640.66</v>
+        <v>32461.66</v>
       </c>
       <c r="J7" s="27" t="n">
-        <v>0.4842803580480839</v>
+        <v>0.5866212380725544</v>
       </c>
       <c r="K7" s="21" t="n">
-        <v>30500</v>
+        <v>22875</v>
       </c>
       <c r="L7" s="28" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M7" s="21" t="n">
         <v>37088.32</v>
       </c>
       <c r="N7" s="21" t="n">
-        <v>111264.96</v>
+        <v>120537.04</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="16" t="inlineStr">
         <is>
-          <t>ADRIANA ALEJALDRE GUZMAN</t>
+          <t>JUDITH PATRICIA SERRANO HERRER</t>
         </is>
       </c>
       <c r="B8" s="16" t="inlineStr">
         <is>
-          <t>Ponce Galindo Alicia Berenice</t>
+          <t>Cabrera Flores Viridiana</t>
         </is>
       </c>
       <c r="C8" s="16" t="inlineStr">
         <is>
-          <t>000048</t>
+          <t>000035</t>
         </is>
       </c>
       <c r="D8" s="16" t="inlineStr">
         <is>
-          <t>UNA LUZ EN MI CAMINO</t>
+          <t>2 DE ABRIL</t>
         </is>
       </c>
       <c r="E8" s="26" t="inlineStr">
@@ -30726,52 +30865,52 @@
         </is>
       </c>
       <c r="F8" s="21" t="n">
-        <v>140000</v>
+        <v>129000</v>
       </c>
       <c r="G8" s="26" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8" s="21" t="n">
-        <v>10640.09</v>
+        <v>9804.09</v>
       </c>
       <c r="I8" s="21" t="n">
-        <v>22872.84</v>
+        <v>8063.45</v>
       </c>
       <c r="J8" s="27" t="n">
-        <v>0.3433182974487428</v>
+        <v>0.2000188522689078</v>
       </c>
       <c r="K8" s="21" t="n">
-        <v>43750</v>
+        <v>32250</v>
       </c>
       <c r="L8" s="28" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="M8" s="21" t="n">
-        <v>42560.36</v>
+        <v>39216.36</v>
       </c>
       <c r="N8" s="21" t="n">
-        <v>117040.99</v>
+        <v>117649.08</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="16" t="inlineStr">
         <is>
-          <t>IRVIN URIEL MORA VELAZCO</t>
+          <t>ADRIANA ALEJALDRE GUZMAN</t>
         </is>
       </c>
       <c r="B9" s="16" t="inlineStr">
         <is>
-          <t>Olivares Morales Josue Edgar</t>
+          <t>Contreras Martinez Jose Luis</t>
         </is>
       </c>
       <c r="C9" s="16" t="inlineStr">
         <is>
-          <t>000055</t>
+          <t>000048</t>
         </is>
       </c>
       <c r="D9" s="16" t="inlineStr">
         <is>
-          <t>MAGIA</t>
+          <t>UNA LUZ EN MI CAMINO</t>
         </is>
       </c>
       <c r="E9" s="26" t="inlineStr">
@@ -30780,31 +30919,31 @@
         </is>
       </c>
       <c r="F9" s="21" t="n">
-        <v>119000</v>
+        <v>140000</v>
       </c>
       <c r="G9" s="26" t="n">
         <v>11</v>
       </c>
       <c r="H9" s="21" t="n">
-        <v>9044.08</v>
+        <v>10640.09</v>
       </c>
       <c r="I9" s="21" t="n">
-        <v>12730.89</v>
+        <v>22872.84</v>
       </c>
       <c r="J9" s="27" t="n">
-        <v>0.2550340666035102</v>
+        <v>0.3433182974487428</v>
       </c>
       <c r="K9" s="21" t="n">
-        <v>37187.5</v>
+        <v>43750</v>
       </c>
       <c r="L9" s="28" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="M9" s="21" t="n">
-        <v>36176.32</v>
+        <v>42560.36</v>
       </c>
       <c r="N9" s="21" t="n">
-        <v>99484.88</v>
+        <v>117040.99</v>
       </c>
     </row>
     <row r="10">
@@ -30852,7 +30991,7 @@
         <v>86625</v>
       </c>
       <c r="L10" s="28" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M10" s="21" t="n">
         <v>60192.52</v>
@@ -30864,22 +31003,22 @@
     <row r="11">
       <c r="A11" s="16" t="inlineStr">
         <is>
-          <t>JUDITH PATRICIA SERRANO HERRER</t>
+          <t>JUAN EDMUNDO LUNA AGUILLON</t>
         </is>
       </c>
       <c r="B11" s="16" t="inlineStr">
         <is>
-          <t>ORTEGA FORTANEL GABRIELA</t>
+          <t>Sanchez Posada Jose Olimpo</t>
         </is>
       </c>
       <c r="C11" s="16" t="inlineStr">
         <is>
-          <t>000113</t>
+          <t>000122</t>
         </is>
       </c>
       <c r="D11" s="16" t="inlineStr">
         <is>
-          <t>DIAMANTINA</t>
+          <t>HOROSCOPOS</t>
         </is>
       </c>
       <c r="E11" s="26" t="inlineStr">
@@ -30888,52 +31027,52 @@
         </is>
       </c>
       <c r="F11" s="21" t="n">
-        <v>55000</v>
+        <v>65000</v>
       </c>
       <c r="G11" s="26" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H11" s="21" t="n">
-        <v>4180.04</v>
+        <v>4940.04</v>
       </c>
       <c r="I11" s="21" t="n">
-        <v>3437.5</v>
+        <v>8036.21</v>
       </c>
       <c r="J11" s="27" t="n">
-        <v>0.09090909090909091</v>
+        <v>0.180189292470567</v>
       </c>
       <c r="K11" s="21" t="n">
-        <v>34375</v>
+        <v>36562.5</v>
       </c>
       <c r="L11" s="28" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M11" s="21" t="n">
-        <v>16720.16</v>
+        <v>19760.16</v>
       </c>
       <c r="N11" s="21" t="n">
-        <v>25080.24</v>
+        <v>34580.28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="16" t="inlineStr">
         <is>
-          <t>JUAN EDMUNDO LUNA AGUILLON</t>
+          <t>IRVIN URIEL MORA VELAZCO</t>
         </is>
       </c>
       <c r="B12" s="16" t="inlineStr">
         <is>
-          <t>Sanchez Posada Jose Olimpo</t>
+          <t>Olivares Morales Josue Edgar</t>
         </is>
       </c>
       <c r="C12" s="16" t="inlineStr">
         <is>
-          <t>000122</t>
+          <t>000187</t>
         </is>
       </c>
       <c r="D12" s="16" t="inlineStr">
         <is>
-          <t>HOROSCOPOS</t>
+          <t>LA ANTORCHA</t>
         </is>
       </c>
       <c r="E12" s="26" t="inlineStr">
@@ -30942,223 +31081,61 @@
         </is>
       </c>
       <c r="F12" s="21" t="n">
-        <v>65000</v>
+        <v>58000</v>
       </c>
       <c r="G12" s="26" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H12" s="21" t="n">
-        <v>4940.04</v>
+        <v>4408.04</v>
       </c>
       <c r="I12" s="21" t="n">
-        <v>4062.5</v>
+        <v>3625</v>
       </c>
       <c r="J12" s="27" t="n">
-        <v>0.09090909090909091</v>
+        <v>0.07142857142857144</v>
       </c>
       <c r="K12" s="21" t="n">
-        <v>40625</v>
+        <v>47125</v>
       </c>
       <c r="L12" s="28" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="M12" s="21" t="n">
-        <v>19760.16</v>
+        <v>17632.16</v>
       </c>
       <c r="N12" s="21" t="n">
-        <v>29640.24</v>
+        <v>13224.12</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="16" t="inlineStr">
-        <is>
-          <t>ADRIANA ALEJALDRE GUZMAN</t>
-        </is>
-      </c>
-      <c r="B13" s="16" t="inlineStr">
-        <is>
-          <t>Contreras Martinez Jose Luis</t>
-        </is>
-      </c>
-      <c r="C13" s="16" t="inlineStr">
-        <is>
-          <t>000127</t>
-        </is>
-      </c>
-      <c r="D13" s="16" t="inlineStr">
-        <is>
-          <t>LUNA</t>
-        </is>
-      </c>
-      <c r="E13" s="26" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="F13" s="21" t="n">
-        <v>70000</v>
-      </c>
-      <c r="G13" s="26" t="n">
-        <v>6</v>
-      </c>
-      <c r="H13" s="21" t="n">
-        <v>5320.05</v>
-      </c>
-      <c r="I13" s="21" t="n">
-        <v>4375</v>
-      </c>
-      <c r="J13" s="27" t="n">
-        <v>0.09090909090909091</v>
-      </c>
-      <c r="K13" s="21" t="n">
-        <v>43750</v>
-      </c>
-      <c r="L13" s="28" t="n">
-        <v>4</v>
-      </c>
-      <c r="M13" s="21" t="n">
-        <v>21280.2</v>
-      </c>
-      <c r="N13" s="21" t="n">
-        <v>31920.3</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="16" t="inlineStr">
-        <is>
-          <t>JUDITH PATRICIA SERRANO HERRER</t>
-        </is>
-      </c>
-      <c r="B14" s="16" t="inlineStr">
-        <is>
-          <t>Becerril Aguirre Jonathan</t>
-        </is>
-      </c>
-      <c r="C14" s="16" t="inlineStr">
-        <is>
-          <t>000152</t>
-        </is>
-      </c>
-      <c r="D14" s="16" t="inlineStr">
-        <is>
-          <t>ANGELES</t>
-        </is>
-      </c>
-      <c r="E14" s="26" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="F14" s="21" t="n">
-        <v>58000</v>
-      </c>
-      <c r="G14" s="26" t="n">
-        <v>4</v>
-      </c>
-      <c r="H14" s="21" t="n">
-        <v>4408.04</v>
-      </c>
-      <c r="I14" s="21" t="n">
-        <v>3625</v>
-      </c>
-      <c r="J14" s="27" t="n">
-        <v>0.07692307692307693</v>
-      </c>
-      <c r="K14" s="21" t="n">
-        <v>43500</v>
-      </c>
-      <c r="L14" s="28" t="n">
-        <v>3</v>
-      </c>
-      <c r="M14" s="21" t="n">
-        <v>17632.16</v>
-      </c>
-      <c r="N14" s="21" t="n">
-        <v>17632.16</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="16" t="inlineStr">
-        <is>
-          <t>IRVIN URIEL MORA VELAZCO</t>
-        </is>
-      </c>
-      <c r="B15" s="16" t="inlineStr">
-        <is>
-          <t>Cuautle Pacheco Jheimy</t>
-        </is>
-      </c>
-      <c r="C15" s="16" t="inlineStr">
-        <is>
-          <t>000185</t>
-        </is>
-      </c>
-      <c r="D15" s="16" t="inlineStr">
-        <is>
-          <t>JOB</t>
-        </is>
-      </c>
-      <c r="E15" s="26" t="inlineStr">
-        <is>
-          <t>01</t>
-        </is>
-      </c>
-      <c r="F15" s="21" t="n">
-        <v>252000</v>
-      </c>
-      <c r="G15" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="H15" s="21" t="n">
-        <v>19152.17</v>
-      </c>
-      <c r="I15" s="21" t="n">
-        <v>15750</v>
-      </c>
-      <c r="J15" s="27" t="n">
-        <v>0.07142857142857144</v>
-      </c>
-      <c r="K15" s="21" t="n">
-        <v>204750</v>
-      </c>
-      <c r="L15" s="28" t="n">
-        <v>3</v>
-      </c>
-      <c r="M15" s="21" t="n">
-        <v>76608.68000000001</v>
-      </c>
-      <c r="N15" s="21" t="n">
-        <v>57456.51000000001</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="F16">
-        <f>SUBTOTAL(109,F7:F15)</f>
+      <c r="F13">
+        <f>SUBTOTAL(109,F7:F12)</f>
         <v/>
       </c>
-      <c r="H16">
-        <f>SUBTOTAL(109,H7:H15)</f>
+      <c r="H13">
+        <f>SUBTOTAL(109,H7:H12)</f>
         <v/>
       </c>
-      <c r="I16">
-        <f>SUBTOTAL(109,I7:I15)</f>
+      <c r="I13">
+        <f>SUBTOTAL(109,I7:I12)</f>
         <v/>
       </c>
-      <c r="K16">
-        <f>SUBTOTAL(109,K7:K15)</f>
+      <c r="K13">
+        <f>SUBTOTAL(109,K7:K12)</f>
         <v/>
       </c>
-      <c r="M16">
-        <f>SUBTOTAL(109,M7:M15)</f>
+      <c r="M13">
+        <f>SUBTOTAL(109,M7:M12)</f>
         <v/>
       </c>
-      <c r="N16">
-        <f>SUBTOTAL(109,N7:N15)</f>
+      <c r="N13">
+        <f>SUBTOTAL(109,N7:N12)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: repairing cartera insoluta cal
</commit_message>
<xml_diff>
--- a/output_automatizado.xlsx
+++ b/output_automatizado.xlsx
@@ -3339,7 +3339,7 @@
         <v>66866.22</v>
       </c>
       <c r="R25" s="23" t="n">
-        <v>22875</v>
+        <v>55336.66</v>
       </c>
       <c r="S25" s="21" t="n">
         <v>0</v>
@@ -4131,7 +4131,7 @@
         <v>23428.82</v>
       </c>
       <c r="R31" s="23" t="n">
-        <v>19250</v>
+        <v>19270.62</v>
       </c>
       <c r="S31" s="21" t="n">
         <v>0</v>
@@ -4659,7 +4659,7 @@
         <v>49021.38</v>
       </c>
       <c r="R35" s="23" t="n">
-        <v>32250</v>
+        <v>40313.45</v>
       </c>
       <c r="S35" s="21" t="n">
         <v>0</v>
@@ -6243,7 +6243,7 @@
         <v>79853.49000000001</v>
       </c>
       <c r="R47" s="23" t="n">
-        <v>43750</v>
+        <v>66622.84</v>
       </c>
       <c r="S47" s="21" t="n">
         <v>0</v>
@@ -9939,7 +9939,7 @@
         <v>119293.11</v>
       </c>
       <c r="R75" s="23" t="n">
-        <v>86625</v>
+        <v>99000</v>
       </c>
       <c r="S75" s="21" t="n">
         <v>0</v>
@@ -15483,7 +15483,7 @@
         <v>52496.61</v>
       </c>
       <c r="R117" s="23" t="n">
-        <v>36562.5</v>
+        <v>44598.71</v>
       </c>
       <c r="S117" s="21" t="n">
         <v>0</v>
@@ -23403,7 +23403,7 @@
         <v>61710.62</v>
       </c>
       <c r="R177" s="23" t="n">
-        <v>47125</v>
+        <v>50750</v>
       </c>
       <c r="S177" s="21" t="n">
         <v>0</v>

</xml_diff>